<commit_message>
Update forests data - 2025-09-27 05:36
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="553">
   <si>
     <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/briezuciema-pag/aogio.html</t>
   </si>
@@ -2076,7 +2076,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F132"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4719,6 +4719,146 @@
       </c>
       <c r="F132" s="3" t="s">
         <v>528</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E139" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>552</v>
       </c>
     </row>
   </sheetData>
@@ -4853,6 +4993,12 @@
     <hyperlink ref="A129" r:id="rId128"/>
     <hyperlink ref="A130" r:id="rId129"/>
     <hyperlink ref="A131" r:id="rId130"/>
+    <hyperlink ref="A134" r:id="rId131"/>
+    <hyperlink ref="A135" r:id="rId132"/>
+    <hyperlink ref="A136" r:id="rId133"/>
+    <hyperlink ref="A137" r:id="rId134"/>
+    <hyperlink ref="A138" r:id="rId135"/>
+    <hyperlink ref="A139" r:id="rId136"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -4864,7 +5010,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4901,135 +5047,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>530</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>532</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>536</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>537</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>540</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>545</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>550</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>551</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>552</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forests data - 2025-09-27 05:47
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="553">
   <si>
     <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/briezuciema-pag/aogio.html</t>
   </si>
@@ -2076,7 +2076,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F139"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4859,6 +4859,26 @@
       </c>
       <c r="F139" s="3" t="s">
         <v>552</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update forests data - 2025-09-29 12:17
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="434">
   <si>
     <t>link</t>
   </si>
@@ -1308,6 +1308,18 @@
   </si>
   <si>
     <t>36480010086</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/indras-pag/kgfdd.html</t>
+  </si>
+  <si>
+    <t>60620030054</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/madona/dbnfi.html</t>
+  </si>
+  <si>
+    <t>70900080055</t>
   </si>
 </sst>
 </file>
@@ -1372,13 +1384,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1720,7 +1732,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F128"/>
+  <dimension ref="A1:F136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4295,6 +4307,166 @@
       </c>
       <c r="F128" s="2">
         <v>45912.35902777778</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="F129" s="2">
+        <v>45926.27777777778</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E130" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="F130" s="2">
+        <v>45926.20486111111</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D131" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E131" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="F131" s="2">
+        <v>45926.25208333333</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="F132" s="2">
+        <v>45925.648611111115</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D133" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E133" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F133" s="2">
+        <v>45925.62638888889</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E134" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F134" s="2">
+        <v>45925.625</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E135" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="F135" s="2">
+        <v>45926.205555555556</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E136" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="F136" s="2">
+        <v>45926.20347222222</v>
       </c>
     </row>
   </sheetData>
@@ -4426,6 +4598,14 @@
     <hyperlink ref="A126" r:id="rId125"/>
     <hyperlink ref="A127" r:id="rId126"/>
     <hyperlink ref="A128" r:id="rId127"/>
+    <hyperlink ref="A129" r:id="rId128"/>
+    <hyperlink ref="A130" r:id="rId129"/>
+    <hyperlink ref="A131" r:id="rId130"/>
+    <hyperlink ref="A132" r:id="rId131"/>
+    <hyperlink ref="A133" r:id="rId132"/>
+    <hyperlink ref="A134" r:id="rId133"/>
+    <hyperlink ref="A135" r:id="rId134"/>
+    <hyperlink ref="A136" r:id="rId135"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -4437,7 +4617,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4455,195 +4635,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>411</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>412</v>
+        <v>430</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>431</v>
       </c>
       <c r="F2" s="2">
-        <v>45926.27777777778</v>
+        <v>45929.39791666667</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>414</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>415</v>
+        <v>432</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>433</v>
       </c>
       <c r="F3" s="2">
-        <v>45926.20486111111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>417</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="F4" s="2">
-        <v>45926.25208333333</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>420</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>421</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45925.648611111115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45925.62638888889</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>424</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="2">
-        <v>45925.625</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>426</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>427</v>
-      </c>
-      <c r="F8" s="2">
-        <v>45926.205555555556</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>426</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>429</v>
-      </c>
-      <c r="F9" s="2">
-        <v>45926.20347222222</v>
+        <v>45928.53611111111</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-09-30 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="448">
   <si>
     <t>link</t>
   </si>
@@ -1320,6 +1320,48 @@
   </si>
   <si>
     <t>70900080055</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/alsviku-pag/bdxkxj.html</t>
+  </si>
+  <si>
+    <t>Alūksne un raj.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/sausnejas-pag/gkipe.html</t>
+  </si>
+  <si>
+    <t>120 000 €</t>
+  </si>
+  <si>
+    <t>70920010011</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/cesvaines-l-t/adfpi.html</t>
+  </si>
+  <si>
+    <t>59 000 €</t>
+  </si>
+  <si>
+    <t>70270030008</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ogre-and-reg/mazozolu-pag/cenmm.html</t>
+  </si>
+  <si>
+    <t>74720080031</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/lendzu-pag/ddghm.html</t>
+  </si>
+  <si>
+    <t>8 100 €</t>
+  </si>
+  <si>
+    <t>2.70 ha.</t>
+  </si>
+  <si>
+    <t>78660050212</t>
   </si>
 </sst>
 </file>
@@ -1732,7 +1774,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4467,6 +4509,46 @@
       </c>
       <c r="F136" s="2">
         <v>45926.20347222222</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D137" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="F137" s="2">
+        <v>45929.39791666667</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D138" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E138" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="F138" s="2">
+        <v>45928.53611111111</v>
       </c>
     </row>
   </sheetData>
@@ -4606,6 +4688,8 @@
     <hyperlink ref="A134" r:id="rId133"/>
     <hyperlink ref="A135" r:id="rId134"/>
     <hyperlink ref="A136" r:id="rId135"/>
+    <hyperlink ref="A137" r:id="rId136"/>
+    <hyperlink ref="A138" r:id="rId137"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -4617,7 +4701,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4656,48 +4740,111 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>116</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>146</v>
+        <v>435</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>431</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>45929.39791666667</v>
+        <v>45929.90277777778</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>268</v>
+        <v>437</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>256</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>85</v>
+        <v>260</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="F3" s="2">
-        <v>45928.53611111111</v>
+        <v>45930.51458333334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45930.50486111111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45930.429861111115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45930.433333333334</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-10-01 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="455">
   <si>
     <t>link</t>
   </si>
@@ -1362,6 +1362,27 @@
   </si>
   <si>
     <t>78660050212</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/bauska-and-reg/iecavas-nov/ljoxm.html</t>
+  </si>
+  <si>
+    <t>9 500 €</t>
+  </si>
+  <si>
+    <t>40940090311</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kastulinas-pag/nhcfn.html</t>
+  </si>
+  <si>
+    <t>60720060103</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/erglu-pag/aclog.html</t>
+  </si>
+  <si>
+    <t>70600080065</t>
   </si>
 </sst>
 </file>
@@ -1774,7 +1795,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4549,6 +4570,106 @@
       </c>
       <c r="F138" s="2">
         <v>45928.53611111111</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D139" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E139" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F139" s="2">
+        <v>45929.90277777778</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="E140" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="F140" s="2">
+        <v>45930.51458333334</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D141" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E141" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="F141" s="2">
+        <v>45930.50486111111</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D142" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E142" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="F142" s="2">
+        <v>45930.429861111115</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="E143" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="F143" s="2">
+        <v>45930.433333333334</v>
       </c>
     </row>
   </sheetData>
@@ -4690,6 +4811,11 @@
     <hyperlink ref="A136" r:id="rId135"/>
     <hyperlink ref="A137" r:id="rId136"/>
     <hyperlink ref="A138" r:id="rId137"/>
+    <hyperlink ref="A139" r:id="rId138"/>
+    <hyperlink ref="A140" r:id="rId139"/>
+    <hyperlink ref="A141" r:id="rId140"/>
+    <hyperlink ref="A142" r:id="rId141"/>
+    <hyperlink ref="A143" r:id="rId142"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -4701,7 +4827,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4740,102 +4866,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>434</v>
+        <v>448</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>449</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>435</v>
+        <v>48</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>25</v>
+        <v>272</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>450</v>
       </c>
       <c r="F2" s="2">
-        <v>45929.90277777778</v>
+        <v>45931.53472222222</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>436</v>
+        <v>451</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>437</v>
+        <v>355</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>256</v>
+        <v>146</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>260</v>
+        <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="F3" s="2">
-        <v>45930.51458333334</v>
+        <v>45931.49166666667</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>439</v>
+        <v>453</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>440</v>
+        <v>116</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>256</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>441</v>
+        <v>454</v>
       </c>
       <c r="F4" s="2">
-        <v>45930.50486111111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>443</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45930.429861111115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45930.433333333334</v>
+        <v>45930.68472222222</v>
       </c>
     </row>
   </sheetData>
@@ -4843,8 +4929,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-10-02 12:16
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="464">
   <si>
     <t>link</t>
   </si>
@@ -1383,6 +1383,33 @@
   </si>
   <si>
     <t>70600080065</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/udrisu-pag/bkbix.html</t>
+  </si>
+  <si>
+    <t>35 880 €</t>
+  </si>
+  <si>
+    <t>60960020067/68</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/salacgrivas-l-t/cdkbp.html</t>
+  </si>
+  <si>
+    <t>66720040252</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/liepupes-pag/eepmh.html</t>
+  </si>
+  <si>
+    <t>39 000 €</t>
+  </si>
+  <si>
+    <t>6.50 ha.</t>
+  </si>
+  <si>
+    <t>66600090044</t>
   </si>
 </sst>
 </file>
@@ -1795,7 +1822,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F143"/>
+  <dimension ref="A1:F146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4670,6 +4697,66 @@
       </c>
       <c r="F143" s="2">
         <v>45930.433333333334</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D144" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E144" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="F144" s="2">
+        <v>45931.53472222222</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D145" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E145" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="F145" s="2">
+        <v>45931.49166666667</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D146" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E146" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="F146" s="2">
+        <v>45930.68472222222</v>
       </c>
     </row>
   </sheetData>
@@ -4816,6 +4903,9 @@
     <hyperlink ref="A141" r:id="rId140"/>
     <hyperlink ref="A142" r:id="rId141"/>
     <hyperlink ref="A143" r:id="rId142"/>
+    <hyperlink ref="A144" r:id="rId143"/>
+    <hyperlink ref="A145" r:id="rId144"/>
+    <hyperlink ref="A146" r:id="rId145"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -4866,62 +4956,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>48</v>
+        <v>146</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>272</v>
+        <v>75</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>450</v>
+        <v>457</v>
       </c>
       <c r="F2" s="2">
-        <v>45931.53472222222</v>
+        <v>45932.393055555556</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>355</v>
+        <v>274</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>146</v>
+        <v>208</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="F3" s="2">
-        <v>45931.49166666667</v>
+        <v>45931.83125</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>116</v>
+        <v>461</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>256</v>
+        <v>208</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>36</v>
+        <v>462</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
       <c r="F4" s="2">
-        <v>45930.68472222222</v>
+        <v>45931.757638888885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update forests data - 2025-10-03 12:16
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="480">
   <si>
     <t>link</t>
   </si>
@@ -1410,6 +1410,54 @@
   </si>
   <si>
     <t>66600090044</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/dobele-and-reg/auru-pag/ionih.html</t>
+  </si>
+  <si>
+    <t>46460080148</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kuldiga-and-reg/padures-pag/cggbgp.html</t>
+  </si>
+  <si>
+    <t>5 000 €</t>
+  </si>
+  <si>
+    <t>62720050064</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kuldiga-and-reg/padures-pag/cggbdp.html</t>
+  </si>
+  <si>
+    <t>26 500 €</t>
+  </si>
+  <si>
+    <t>5.12 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kuldiga-and-reg/padures-pag/cggbdm.html</t>
+  </si>
+  <si>
+    <t>4.36 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/liepaja-and-reg/dunikas-pag/ngxix.html</t>
+  </si>
+  <si>
+    <t>64520070098</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/aronas-pag/ahkjo.html</t>
+  </si>
+  <si>
+    <t>155 000 €</t>
+  </si>
+  <si>
+    <t>27 ha.</t>
+  </si>
+  <si>
+    <t>70420020025</t>
   </si>
 </sst>
 </file>
@@ -1822,7 +1870,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F146"/>
+  <dimension ref="A1:F149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4757,6 +4805,66 @@
       </c>
       <c r="F146" s="2">
         <v>45930.68472222222</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="C147" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D147" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E147" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="F147" s="2">
+        <v>45932.393055555556</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D148" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E148" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="F148" s="2">
+        <v>45931.83125</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D149" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="E149" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="F149" s="2">
+        <v>45931.757638888885</v>
       </c>
     </row>
   </sheetData>
@@ -4906,6 +5014,9 @@
     <hyperlink ref="A144" r:id="rId143"/>
     <hyperlink ref="A145" r:id="rId144"/>
     <hyperlink ref="A146" r:id="rId145"/>
+    <hyperlink ref="A147" r:id="rId146"/>
+    <hyperlink ref="A148" r:id="rId147"/>
+    <hyperlink ref="A149" r:id="rId148"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -4917,7 +5028,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4956,62 +5067,122 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>455</v>
+        <v>464</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>456</v>
+        <v>274</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>457</v>
+        <v>465</v>
       </c>
       <c r="F2" s="2">
-        <v>45932.393055555556</v>
+        <v>45933.61111111111</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>274</v>
+        <v>467</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>208</v>
+        <v>424</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>36</v>
+        <v>186</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>459</v>
+        <v>468</v>
       </c>
       <c r="F3" s="2">
-        <v>45931.83125</v>
+        <v>45933.45347222222</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>208</v>
+        <v>424</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>463</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2">
-        <v>45931.757638888885</v>
+        <v>45932.93611111111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45932.929861111115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45933.45416666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="F7" s="2">
+        <v>45933.45972222222</v>
       </c>
     </row>
   </sheetData>
@@ -5019,6 +5190,9 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-10-06 12:17
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="489">
   <si>
     <t>link</t>
   </si>
@@ -1458,6 +1458,33 @@
   </si>
   <si>
     <t>70420020025</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/naujenes-pag/phdno.html</t>
+  </si>
+  <si>
+    <t>91 500 €</t>
+  </si>
+  <si>
+    <t>12.35 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/dobele-and-reg/ukru-pag/bbxnld.html</t>
+  </si>
+  <si>
+    <t>46900040149</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/dobele-and-reg/dobele/mkolm.html</t>
+  </si>
+  <si>
+    <t>46520030029</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/preilu-pag/lelig.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/talsi-and-reg/vandzenes-pag/cenxi.html</t>
   </si>
 </sst>
 </file>
@@ -1870,7 +1897,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F149"/>
+  <dimension ref="A1:F155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4865,6 +4892,126 @@
       </c>
       <c r="F149" s="2">
         <v>45931.757638888885</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="B150" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D150" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E150" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="F150" s="2">
+        <v>45933.61111111111</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D151" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E151" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="F151" s="2">
+        <v>45933.45347222222</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="C152" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D152" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="E152" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F152" s="2">
+        <v>45932.93611111111</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D153" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="E153" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F153" s="2">
+        <v>45932.929861111115</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C154" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D154" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E154" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="F154" s="2">
+        <v>45933.45416666666</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="C155" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D155" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="E155" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="F155" s="2">
+        <v>45933.45972222222</v>
       </c>
     </row>
   </sheetData>
@@ -5017,6 +5164,12 @@
     <hyperlink ref="A147" r:id="rId146"/>
     <hyperlink ref="A148" r:id="rId147"/>
     <hyperlink ref="A149" r:id="rId148"/>
+    <hyperlink ref="A150" r:id="rId149"/>
+    <hyperlink ref="A151" r:id="rId150"/>
+    <hyperlink ref="A152" r:id="rId151"/>
+    <hyperlink ref="A153" r:id="rId152"/>
+    <hyperlink ref="A154" r:id="rId153"/>
+    <hyperlink ref="A155" r:id="rId154"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -5028,7 +5181,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5067,122 +5220,102 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>464</v>
+        <v>480</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>274</v>
+        <v>481</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>117</v>
+        <v>74</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>135</v>
+        <v>482</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>465</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>45933.61111111111</v>
+        <v>45936.052777777775</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>466</v>
+        <v>483</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>467</v>
+        <v>88</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>424</v>
+        <v>117</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>186</v>
+        <v>36</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>468</v>
+        <v>484</v>
       </c>
       <c r="F3" s="2">
-        <v>45933.45347222222</v>
+        <v>45934.77986111111</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>469</v>
+        <v>485</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>470</v>
+        <v>268</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>424</v>
+        <v>117</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>471</v>
+        <v>75</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>25</v>
+        <v>486</v>
       </c>
       <c r="F4" s="2">
-        <v>45932.93611111111</v>
+        <v>45933.72083333333</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>472</v>
+        <v>487</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>307</v>
+        <v>31</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>424</v>
+        <v>284</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>473</v>
+        <v>82</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="2">
-        <v>45932.929861111115</v>
+        <v>45934.59027777778</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>474</v>
+        <v>488</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>150</v>
+        <v>88</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>190</v>
+        <v>356</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>475</v>
+        <v>25</v>
       </c>
       <c r="F6" s="2">
-        <v>45933.45416666666</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>477</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>479</v>
-      </c>
-      <c r="F7" s="2">
-        <v>45933.45972222222</v>
+        <v>45934.82847222222</v>
       </c>
     </row>
   </sheetData>
@@ -5192,7 +5325,6 @@
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
     <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-10-07 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="498">
   <si>
     <t>link</t>
   </si>
@@ -1485,6 +1485,33 @@
   </si>
   <si>
     <t>https://www.ss.com/msg/lv/real-estate/wood/talsi-and-reg/vandzenes-pag/cenxi.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jekabpils-and-reg/kuku-pag/mfhkk.html</t>
+  </si>
+  <si>
+    <t>56700050044</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kaplavas-pag/dmief.html</t>
+  </si>
+  <si>
+    <t>126 000 €</t>
+  </si>
+  <si>
+    <t>60700090144</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/purenu-pag/ihhdc.html</t>
+  </si>
+  <si>
+    <t>68880010168</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/talsi-and-reg/gibulu-pag/demgx.html</t>
+  </si>
+  <si>
+    <t>19 000 €</t>
   </si>
 </sst>
 </file>
@@ -1897,7 +1924,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F155"/>
+  <dimension ref="A1:F160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5012,6 +5039,106 @@
       </c>
       <c r="F155" s="2">
         <v>45933.45972222222</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="C156" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D156" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="E156" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F156" s="2">
+        <v>45936.052777777775</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D157" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E157" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="F157" s="2">
+        <v>45934.77986111111</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D158" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E158" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="F158" s="2">
+        <v>45933.72083333333</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C159" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E159" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F159" s="2">
+        <v>45934.59027777778</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C160" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D160" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E160" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F160" s="2">
+        <v>45934.82847222222</v>
       </c>
     </row>
   </sheetData>
@@ -5170,6 +5297,11 @@
     <hyperlink ref="A153" r:id="rId152"/>
     <hyperlink ref="A154" r:id="rId153"/>
     <hyperlink ref="A155" r:id="rId154"/>
+    <hyperlink ref="A156" r:id="rId155"/>
+    <hyperlink ref="A157" r:id="rId156"/>
+    <hyperlink ref="A158" r:id="rId157"/>
+    <hyperlink ref="A159" r:id="rId158"/>
+    <hyperlink ref="A160" r:id="rId159"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -5181,7 +5313,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5220,102 +5352,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>480</v>
+        <v>489</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>481</v>
+        <v>268</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>74</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>482</v>
+        <v>59</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>490</v>
       </c>
       <c r="F2" s="2">
-        <v>45936.052777777775</v>
+        <v>45936.663888888885</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>483</v>
+        <v>491</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>88</v>
+        <v>492</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>36</v>
+        <v>302</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>484</v>
+        <v>493</v>
       </c>
       <c r="F3" s="2">
-        <v>45934.77986111111</v>
+        <v>45937.475694444445</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>485</v>
+        <v>494</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>268</v>
+        <v>102</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>117</v>
+        <v>234</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>75</v>
+        <v>13</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>486</v>
+        <v>495</v>
       </c>
       <c r="F4" s="2">
-        <v>45933.72083333333</v>
+        <v>45937.37430555555</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>487</v>
+        <v>496</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>497</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>284</v>
+        <v>356</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="2">
-        <v>45934.59027777778</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>488</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45934.82847222222</v>
+        <v>45937.46666666667</v>
       </c>
     </row>
   </sheetData>
@@ -5324,7 +5436,6 @@
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-10-08 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="504">
   <si>
     <t>link</t>
   </si>
@@ -1512,6 +1512,24 @@
   </si>
   <si>
     <t>19 000 €</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/kubulu-pag/cddkb.html</t>
+  </si>
+  <si>
+    <t>38580030185</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/malinovas-pag/mknjo.html</t>
+  </si>
+  <si>
+    <t>20 500 €</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/rusonas-pag/hfiff.html</t>
+  </si>
+  <si>
+    <t>7670 002 0088</t>
   </si>
 </sst>
 </file>
@@ -1924,7 +1942,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F160"/>
+  <dimension ref="A1:F164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5139,6 +5157,86 @@
       </c>
       <c r="F160" s="2">
         <v>45934.82847222222</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C161" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D161" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E161" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="F161" s="2">
+        <v>45936.663888888885</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="C162" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D162" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E162" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="F162" s="2">
+        <v>45937.475694444445</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C163" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D163" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E163" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="F163" s="2">
+        <v>45937.37430555555</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="C164" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D164" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E164" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F164" s="2">
+        <v>45937.46666666667</v>
       </c>
     </row>
   </sheetData>
@@ -5302,6 +5400,10 @@
     <hyperlink ref="A158" r:id="rId157"/>
     <hyperlink ref="A159" r:id="rId158"/>
     <hyperlink ref="A160" r:id="rId159"/>
+    <hyperlink ref="A161" r:id="rId160"/>
+    <hyperlink ref="A162" r:id="rId161"/>
+    <hyperlink ref="A163" r:id="rId162"/>
+    <hyperlink ref="A164" r:id="rId163"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -5313,7 +5415,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5352,82 +5454,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>489</v>
+        <v>498</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>127</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>490</v>
+        <v>499</v>
       </c>
       <c r="F2" s="2">
-        <v>45936.663888888885</v>
+        <v>45938.54236111111</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>491</v>
+        <v>500</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>492</v>
+        <v>501</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>146</v>
+        <v>74</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>302</v>
+        <v>36</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>493</v>
+        <v>79</v>
       </c>
       <c r="F3" s="2">
-        <v>45937.475694444445</v>
+        <v>45937.643055555556</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>494</v>
+        <v>502</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>234</v>
+        <v>284</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>13</v>
+        <v>272</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
       <c r="F4" s="2">
-        <v>45937.37430555555</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>497</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45937.46666666667</v>
+        <v>45938.44861111111</v>
       </c>
     </row>
   </sheetData>
@@ -5435,7 +5517,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-10-09 12:17
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="512">
   <si>
     <t>link</t>
   </si>
@@ -1530,6 +1530,30 @@
   </si>
   <si>
     <t>7670 002 0088</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/demenes-pag/penmn.html</t>
+  </si>
+  <si>
+    <t>6 500 €</t>
+  </si>
+  <si>
+    <t>44500070575</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kraslavas-pag/exinl.html</t>
+  </si>
+  <si>
+    <t>3.55 ha.</t>
+  </si>
+  <si>
+    <t>60680040692</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/dagdas-pag/bklfdl.html</t>
+  </si>
+  <si>
+    <t>605400103313</t>
   </si>
 </sst>
 </file>
@@ -1942,7 +1966,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F164"/>
+  <dimension ref="A1:F167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5237,6 +5261,66 @@
       </c>
       <c r="F164" s="2">
         <v>45937.46666666667</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C165" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D165" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E165" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="F165" s="2">
+        <v>45938.54236111111</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="C166" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E166" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F166" s="2">
+        <v>45937.643055555556</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C167" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D167" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E167" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="F167" s="2">
+        <v>45938.44861111111</v>
       </c>
     </row>
   </sheetData>
@@ -5404,6 +5488,9 @@
     <hyperlink ref="A162" r:id="rId161"/>
     <hyperlink ref="A163" r:id="rId162"/>
     <hyperlink ref="A164" r:id="rId163"/>
+    <hyperlink ref="A165" r:id="rId164"/>
+    <hyperlink ref="A166" r:id="rId165"/>
+    <hyperlink ref="A167" r:id="rId166"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -5454,62 +5541,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>274</v>
+        <v>505</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>59</v>
+        <v>186</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="F2" s="2">
-        <v>45938.54236111111</v>
+        <v>45939.38125</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>501</v>
+        <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>74</v>
+        <v>146</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>36</v>
+        <v>508</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>79</v>
+        <v>509</v>
       </c>
       <c r="F3" s="2">
-        <v>45937.643055555556</v>
+        <v>45939.524305555555</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>502</v>
+        <v>510</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>131</v>
+        <v>39</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>284</v>
+        <v>146</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>272</v>
+        <v>82</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>503</v>
+        <v>511</v>
       </c>
       <c r="F4" s="2">
-        <v>45938.44861111111</v>
+        <v>45938.941666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update forests data - 2025-10-10 12:17
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="527">
   <si>
     <t>link</t>
   </si>
@@ -1554,6 +1554,51 @@
   </si>
   <si>
     <t>605400103313</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/drabesu-pag/kcbcn.html</t>
+  </si>
+  <si>
+    <t>260 000 €</t>
+  </si>
+  <si>
+    <t>32 ha.</t>
+  </si>
+  <si>
+    <t>42460020118</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jelgava-and-reg/kalnciems/cggfmf.html</t>
+  </si>
+  <si>
+    <t>3 000 €</t>
+  </si>
+  <si>
+    <t>Jelgava un raj.</t>
+  </si>
+  <si>
+    <t>54310030242</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/skultes-pag/biedf.html</t>
+  </si>
+  <si>
+    <t>72 000 €</t>
+  </si>
+  <si>
+    <t>66760160151</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/pelecu-pag/mmbxp.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/talsi-and-reg/laucienes-pag/injce.html</t>
+  </si>
+  <si>
+    <t>6.80 ha.</t>
+  </si>
+  <si>
+    <t>88700200012</t>
   </si>
 </sst>
 </file>
@@ -1966,7 +2011,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F167"/>
+  <dimension ref="A1:F170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5321,6 +5366,66 @@
       </c>
       <c r="F167" s="2">
         <v>45938.44861111111</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="C168" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D168" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E168" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="F168" s="2">
+        <v>45939.38125</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D169" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="E169" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="F169" s="2">
+        <v>45939.524305555555</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C170" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D170" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E170" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="F170" s="2">
+        <v>45938.941666666666</v>
       </c>
     </row>
   </sheetData>
@@ -5491,6 +5596,9 @@
     <hyperlink ref="A165" r:id="rId164"/>
     <hyperlink ref="A166" r:id="rId165"/>
     <hyperlink ref="A167" r:id="rId166"/>
+    <hyperlink ref="A168" r:id="rId167"/>
+    <hyperlink ref="A169" r:id="rId168"/>
+    <hyperlink ref="A170" r:id="rId169"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -5502,7 +5610,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5541,62 +5649,102 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>504</v>
+        <v>512</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>505</v>
+        <v>513</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>186</v>
+        <v>514</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>506</v>
+        <v>515</v>
       </c>
       <c r="F2" s="2">
-        <v>45939.38125</v>
+        <v>45940.37013888889</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>507</v>
+        <v>516</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>517</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>146</v>
+        <v>518</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>508</v>
+        <v>186</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>509</v>
+        <v>519</v>
       </c>
       <c r="F3" s="2">
-        <v>45939.524305555555</v>
+        <v>45939.76666666666</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>510</v>
+        <v>520</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>39</v>
+        <v>521</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>146</v>
+        <v>208</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>511</v>
+        <v>522</v>
       </c>
       <c r="F4" s="2">
-        <v>45938.941666666666</v>
+        <v>45940.37777777778</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>517</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45940.46736111111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45939.80416666667</v>
       </c>
     </row>
   </sheetData>
@@ -5604,6 +5752,8 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-10-13 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="535">
   <si>
     <t>link</t>
   </si>
@@ -1599,6 +1599,30 @@
   </si>
   <si>
     <t>88700200012</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/liepupes-pag/cgghen.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/lauderu-pag/bfixpm.html</t>
+  </si>
+  <si>
+    <t>68640060059</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/berzaunes-pag/jlbfo.html</t>
+  </si>
+  <si>
+    <t>70460010128</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/valmiera-and-reg/mazsalaca/cgbihd.html</t>
+  </si>
+  <si>
+    <t>110 000 €</t>
+  </si>
+  <si>
+    <t>96310010009</t>
   </si>
 </sst>
 </file>
@@ -2011,7 +2035,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F170"/>
+  <dimension ref="A1:F175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5426,6 +5450,106 @@
       </c>
       <c r="F170" s="2">
         <v>45938.941666666666</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="C171" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D171" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="E171" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="F171" s="2">
+        <v>45940.37013888889</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>517</v>
+      </c>
+      <c r="C172" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="D172" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E172" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="F172" s="2">
+        <v>45939.76666666666</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="C173" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D173" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E173" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="F173" s="2">
+        <v>45940.37777777778</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>517</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D174" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E174" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F174" s="2">
+        <v>45940.46736111111</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C175" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D175" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="E175" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="F175" s="2">
+        <v>45939.80416666667</v>
       </c>
     </row>
   </sheetData>
@@ -5599,6 +5723,11 @@
     <hyperlink ref="A168" r:id="rId167"/>
     <hyperlink ref="A169" r:id="rId168"/>
     <hyperlink ref="A170" r:id="rId169"/>
+    <hyperlink ref="A171" r:id="rId170"/>
+    <hyperlink ref="A172" r:id="rId171"/>
+    <hyperlink ref="A173" r:id="rId172"/>
+    <hyperlink ref="A174" r:id="rId173"/>
+    <hyperlink ref="A175" r:id="rId174"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -5610,7 +5739,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5649,102 +5778,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>512</v>
+        <v>527</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>513</v>
+        <v>461</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>63</v>
+        <v>208</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>514</v>
+        <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>515</v>
+        <v>463</v>
       </c>
       <c r="F2" s="2">
-        <v>45940.37013888889</v>
+        <v>45942.55763888889</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>516</v>
+        <v>528</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>517</v>
+        <v>268</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>518</v>
+        <v>234</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>186</v>
+        <v>75</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>519</v>
+        <v>529</v>
       </c>
       <c r="F3" s="2">
-        <v>45939.76666666666</v>
+        <v>45941.53055555555</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>521</v>
+        <v>116</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>208</v>
+        <v>256</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>24</v>
+        <v>186</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>522</v>
+        <v>531</v>
       </c>
       <c r="F4" s="2">
-        <v>45940.37777777778</v>
+        <v>45942.73888888889</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>523</v>
+        <v>532</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>517</v>
+        <v>533</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>284</v>
+        <v>396</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>272</v>
+        <v>82</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>25</v>
+        <v>534</v>
       </c>
       <c r="F5" s="2">
-        <v>45940.46736111111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>525</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>526</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45939.80416666667</v>
+        <v>45942.413194444445</v>
       </c>
     </row>
   </sheetData>
@@ -5753,7 +5862,6 @@
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-10-14 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="539">
   <si>
     <t>link</t>
   </si>
@@ -1623,6 +1623,18 @@
   </si>
   <si>
     <t>96310010009</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/naujenes-pag/achid.html</t>
+  </si>
+  <si>
+    <t>4 500 €</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jekabpils-and-reg/vipes-pag/odlhl.html</t>
+  </si>
+  <si>
+    <t>56960010027</t>
   </si>
 </sst>
 </file>
@@ -2035,7 +2047,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F175"/>
+  <dimension ref="A1:F179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5550,6 +5562,86 @@
       </c>
       <c r="F175" s="2">
         <v>45939.80416666667</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="C176" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D176" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E176" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="F176" s="2">
+        <v>45942.55763888889</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C177" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D177" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E177" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="F177" s="2">
+        <v>45941.53055555555</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C178" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D178" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E178" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="F178" s="2">
+        <v>45942.73888888889</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="C179" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="D179" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E179" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="F179" s="2">
+        <v>45942.413194444445</v>
       </c>
     </row>
   </sheetData>
@@ -5728,6 +5820,10 @@
     <hyperlink ref="A173" r:id="rId172"/>
     <hyperlink ref="A174" r:id="rId173"/>
     <hyperlink ref="A175" r:id="rId174"/>
+    <hyperlink ref="A176" r:id="rId175"/>
+    <hyperlink ref="A177" r:id="rId176"/>
+    <hyperlink ref="A178" r:id="rId177"/>
+    <hyperlink ref="A179" r:id="rId178"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -5739,7 +5835,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5778,90 +5874,48 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>461</v>
+        <v>536</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>208</v>
+        <v>74</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>13</v>
+        <v>272</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>463</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>45942.55763888889</v>
+        <v>45943.87986111111</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>528</v>
+        <v>537</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>268</v>
+        <v>204</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>234</v>
+        <v>127</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>529</v>
+        <v>538</v>
       </c>
       <c r="F3" s="2">
-        <v>45941.53055555555</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>530</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>531</v>
-      </c>
-      <c r="F4" s="2">
-        <v>45942.73888888889</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>532</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>533</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>534</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45942.413194444445</v>
+        <v>45944.61388888889</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-10-15 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="554">
   <si>
     <t>link</t>
   </si>
@@ -1635,6 +1635,51 @@
   </si>
   <si>
     <t>56960010027</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/gaujienas-pag/gebgx.html</t>
+  </si>
+  <si>
+    <t>26 900 €</t>
+  </si>
+  <si>
+    <t>4.90 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/salienas-pag/bccgkj.html</t>
+  </si>
+  <si>
+    <t>11.48 ha.</t>
+  </si>
+  <si>
+    <t>44840090024</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jekabpils-and-reg/rubenes-pag/indke.html</t>
+  </si>
+  <si>
+    <t>23 500 €</t>
+  </si>
+  <si>
+    <t>56820070009</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kalniesu-pag/iepek.html</t>
+  </si>
+  <si>
+    <t>21 000 €</t>
+  </si>
+  <si>
+    <t>60680010191</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/ledurgas-pag/djxgk.html</t>
+  </si>
+  <si>
+    <t>49 500 €</t>
+  </si>
+  <si>
+    <t>33 ha.</t>
   </si>
 </sst>
 </file>
@@ -2047,7 +2092,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F179"/>
+  <dimension ref="A1:F181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5642,6 +5687,46 @@
       </c>
       <c r="F179" s="2">
         <v>45942.413194444445</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="C180" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D180" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E180" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F180" s="2">
+        <v>45943.87986111111</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C181" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D181" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E181" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="F181" s="2">
+        <v>45944.61388888889</v>
       </c>
     </row>
   </sheetData>
@@ -5824,6 +5909,8 @@
     <hyperlink ref="A177" r:id="rId176"/>
     <hyperlink ref="A178" r:id="rId177"/>
     <hyperlink ref="A179" r:id="rId178"/>
+    <hyperlink ref="A180" r:id="rId179"/>
+    <hyperlink ref="A181" r:id="rId180"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -5835,7 +5922,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5874,48 +5961,111 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>74</v>
+        <v>435</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>272</v>
+        <v>541</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>45943.87986111111</v>
+        <v>45944.70833333333</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>204</v>
+        <v>106</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45944.8625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>538</v>
-      </c>
-      <c r="F3" s="2">
-        <v>45944.61388888889</v>
+      <c r="E4" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45945.43611111111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>550</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45944.65763888889</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>552</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45945.37638888889</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-10-16 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="564">
   <si>
     <t>link</t>
   </si>
@@ -1680,6 +1680,36 @@
   </si>
   <si>
     <t>33 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/malinovas-pag/mknjc.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/dobele-and-reg/berzes-pag/kkjpg.html</t>
+  </si>
+  <si>
+    <t>1 400 €</t>
+  </si>
+  <si>
+    <t>46520030087</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jelgava-and-reg/kalnciems/cfghfd.html</t>
+  </si>
+  <si>
+    <t>89 500 €</t>
+  </si>
+  <si>
+    <t>54310030137</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/valka-and-reg/blomes-pag/lkijb.html</t>
+  </si>
+  <si>
+    <t>123 456 €</t>
+  </si>
+  <si>
+    <t>94460010165</t>
   </si>
 </sst>
 </file>
@@ -2092,7 +2122,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F181"/>
+  <dimension ref="A1:F186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5727,6 +5757,106 @@
       </c>
       <c r="F181" s="2">
         <v>45944.61388888889</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="B182" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="C182" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D182" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="E182" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F182" s="2">
+        <v>45944.70833333333</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="B183" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C183" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D183" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="E183" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="F183" s="2">
+        <v>45944.8625</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="C184" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D184" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E184" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="F184" s="2">
+        <v>45945.43611111111</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="C185" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D185" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E185" s="4" t="s">
+        <v>550</v>
+      </c>
+      <c r="F185" s="2">
+        <v>45944.65763888889</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="B186" s="4" t="s">
+        <v>552</v>
+      </c>
+      <c r="C186" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D186" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="E186" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F186" s="2">
+        <v>45945.37638888889</v>
       </c>
     </row>
   </sheetData>
@@ -5911,6 +6041,11 @@
     <hyperlink ref="A179" r:id="rId178"/>
     <hyperlink ref="A180" r:id="rId179"/>
     <hyperlink ref="A181" r:id="rId180"/>
+    <hyperlink ref="A182" r:id="rId181"/>
+    <hyperlink ref="A183" r:id="rId182"/>
+    <hyperlink ref="A184" r:id="rId183"/>
+    <hyperlink ref="A185" r:id="rId184"/>
+    <hyperlink ref="A186" r:id="rId185"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -5922,7 +6057,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5961,102 +6096,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>539</v>
+        <v>554</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>540</v>
+        <v>313</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>435</v>
+        <v>74</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>541</v>
+        <v>36</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="F2" s="2">
-        <v>45944.70833333333</v>
+        <v>45946.60208333333</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>542</v>
+        <v>555</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>106</v>
+        <v>556</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>543</v>
+        <v>272</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>544</v>
+        <v>557</v>
       </c>
       <c r="F3" s="2">
-        <v>45944.8625</v>
+        <v>45946.40972222222</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>545</v>
+        <v>558</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>546</v>
+        <v>559</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>127</v>
+        <v>518</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>547</v>
+        <v>560</v>
       </c>
       <c r="F4" s="2">
-        <v>45945.43611111111</v>
+        <v>45946.49097222222</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>548</v>
+        <v>561</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>549</v>
+        <v>562</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>146</v>
+        <v>392</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>550</v>
+        <v>563</v>
       </c>
       <c r="F5" s="2">
-        <v>45944.65763888889</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>551</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>552</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>553</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45945.37638888889</v>
+        <v>45945.875</v>
       </c>
     </row>
   </sheetData>
@@ -6065,7 +6180,6 @@
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-10-17 12:17
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="572">
   <si>
     <t>link</t>
   </si>
@@ -1710,6 +1710,30 @@
   </si>
   <si>
     <t>94460010165</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/sarkanu-pag/iojbh.html</t>
+  </si>
+  <si>
+    <t>70900070024</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/berzaunes-pag/niefh.html</t>
+  </si>
+  <si>
+    <t>19 871 €</t>
+  </si>
+  <si>
+    <t>70460020031</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/tukums-and-reg/lapmezciema-nov/ocdgb.html</t>
+  </si>
+  <si>
+    <t>906600497</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/tukums-and-reg/lestenes-pag/bximhb.html</t>
   </si>
 </sst>
 </file>
@@ -2122,7 +2146,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F186"/>
+  <dimension ref="A1:F190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5857,6 +5881,86 @@
       </c>
       <c r="F186" s="2">
         <v>45945.37638888889</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="B187" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C187" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D187" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E187" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F187" s="2">
+        <v>45946.60208333333</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="B188" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="C188" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D188" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E188" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="F188" s="2">
+        <v>45946.40972222222</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="B189" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="C189" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="D189" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E189" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="F189" s="2">
+        <v>45946.49097222222</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B190" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="C190" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D190" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E190" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="F190" s="2">
+        <v>45945.875</v>
       </c>
     </row>
   </sheetData>
@@ -6046,6 +6150,10 @@
     <hyperlink ref="A184" r:id="rId183"/>
     <hyperlink ref="A185" r:id="rId184"/>
     <hyperlink ref="A186" r:id="rId185"/>
+    <hyperlink ref="A187" r:id="rId186"/>
+    <hyperlink ref="A188" r:id="rId187"/>
+    <hyperlink ref="A189" r:id="rId188"/>
+    <hyperlink ref="A190" r:id="rId189"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -6096,82 +6204,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>554</v>
+        <v>564</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>313</v>
+        <v>88</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>74</v>
+        <v>256</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>36</v>
+        <v>154</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>79</v>
+        <v>565</v>
       </c>
       <c r="F2" s="2">
-        <v>45946.60208333333</v>
+        <v>45947.54236111111</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>555</v>
+        <v>566</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>556</v>
+        <v>567</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>117</v>
+        <v>256</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>272</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>557</v>
+        <v>568</v>
       </c>
       <c r="F3" s="2">
-        <v>45946.40972222222</v>
+        <v>45946.975</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>558</v>
+        <v>569</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>559</v>
+        <v>47</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>518</v>
+        <v>376</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>560</v>
+        <v>570</v>
       </c>
       <c r="F4" s="2">
-        <v>45946.49097222222</v>
+        <v>45947.552777777775</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>561</v>
+        <v>571</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>562</v>
+        <v>185</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>563</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2">
-        <v>45945.875</v>
+        <v>45946.759722222225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update forests data - 2025-10-20 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="582">
   <si>
     <t>link</t>
   </si>
@@ -1734,6 +1734,36 @@
   </si>
   <si>
     <t>https://www.ss.com/msg/lv/real-estate/wood/tukums-and-reg/lestenes-pag/bximhb.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aizkraukle-and-reg/aizkraukles-pag/fppdj.html</t>
+  </si>
+  <si>
+    <t>32780050049</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aizkraukle-and-reg/aizkraukles-pag/ljdbo.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/mezvidu-pag/exmxd.html</t>
+  </si>
+  <si>
+    <t>6 000 €</t>
+  </si>
+  <si>
+    <t>68700050016</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ogre-and-reg/ledmanes-pag/jexbj.html</t>
+  </si>
+  <si>
+    <t>74640020009</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/cornajas-pag/afdcl.html</t>
+  </si>
+  <si>
+    <t>78460100069</t>
   </si>
 </sst>
 </file>
@@ -2146,7 +2176,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F190"/>
+  <dimension ref="A1:F194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5961,6 +5991,86 @@
       </c>
       <c r="F190" s="2">
         <v>45945.875</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="B191" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C191" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D191" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E191" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="F191" s="2">
+        <v>45947.54236111111</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="B192" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="C192" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D192" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E192" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="F192" s="2">
+        <v>45946.975</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B193" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C193" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D193" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E193" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="F193" s="2">
+        <v>45947.552777777775</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="B194" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C194" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D194" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E194" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F194" s="2">
+        <v>45946.759722222225</v>
       </c>
     </row>
   </sheetData>
@@ -6154,6 +6264,10 @@
     <hyperlink ref="A188" r:id="rId187"/>
     <hyperlink ref="A189" r:id="rId188"/>
     <hyperlink ref="A190" r:id="rId189"/>
+    <hyperlink ref="A191" r:id="rId190"/>
+    <hyperlink ref="A192" r:id="rId191"/>
+    <hyperlink ref="A193" r:id="rId192"/>
+    <hyperlink ref="A194" r:id="rId193"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -6165,7 +6279,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6204,82 +6318,102 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>564</v>
+        <v>572</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>88</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>256</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>565</v>
+        <v>573</v>
       </c>
       <c r="F2" s="2">
-        <v>45947.54236111111</v>
+        <v>45948.00208333333</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>566</v>
+        <v>574</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>567</v>
+        <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>256</v>
+        <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>272</v>
+        <v>186</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
       <c r="F3" s="2">
-        <v>45946.975</v>
+        <v>45948.00208333333</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>569</v>
+        <v>575</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>47</v>
+        <v>576</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>376</v>
+        <v>234</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>82</v>
+        <v>272</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>570</v>
+        <v>577</v>
       </c>
       <c r="F4" s="2">
-        <v>45947.552777777775</v>
+        <v>45949.69305555556</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>185</v>
+        <v>280</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>376</v>
+        <v>275</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>85</v>
+        <v>272</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>25</v>
+        <v>579</v>
       </c>
       <c r="F5" s="2">
-        <v>45946.759722222225</v>
+        <v>45949.60902777778</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45947.663888888885</v>
       </c>
     </row>
   </sheetData>
@@ -6288,6 +6422,7 @@
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-10-21 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="589">
   <si>
     <t>link</t>
   </si>
@@ -1764,6 +1764,27 @@
   </si>
   <si>
     <t>78460100069</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/pales-pag/iplcg.html</t>
+  </si>
+  <si>
+    <t>57 500 €</t>
+  </si>
+  <si>
+    <t>12.16 ha.</t>
+  </si>
+  <si>
+    <t>66680010347</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/sausnejas-pag/bepgl.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/tukums-and-reg/jaunsatu-pag/ohglb.html</t>
+  </si>
+  <si>
+    <t>90580070009</t>
   </si>
 </sst>
 </file>
@@ -2176,7 +2197,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F194"/>
+  <dimension ref="A1:F199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6071,6 +6092,106 @@
       </c>
       <c r="F194" s="2">
         <v>45946.759722222225</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="B195" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C195" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D195" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E195" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="F195" s="2">
+        <v>45948.00208333333</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="B196" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C196" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D196" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E196" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="F196" s="2">
+        <v>45948.00208333333</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="B197" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C197" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D197" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E197" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="F197" s="2">
+        <v>45949.69305555556</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="B198" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C198" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D198" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E198" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="F198" s="2">
+        <v>45949.60902777778</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="B199" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C199" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D199" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E199" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="F199" s="2">
+        <v>45947.663888888885</v>
       </c>
     </row>
   </sheetData>
@@ -6268,6 +6389,11 @@
     <hyperlink ref="A192" r:id="rId191"/>
     <hyperlink ref="A193" r:id="rId192"/>
     <hyperlink ref="A194" r:id="rId193"/>
+    <hyperlink ref="A195" r:id="rId194"/>
+    <hyperlink ref="A196" r:id="rId195"/>
+    <hyperlink ref="A197" r:id="rId196"/>
+    <hyperlink ref="A198" r:id="rId197"/>
+    <hyperlink ref="A199" r:id="rId198"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -6279,7 +6405,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6318,102 +6444,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>572</v>
+        <v>582</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>88</v>
+        <v>583</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>186</v>
+        <v>584</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>573</v>
+        <v>585</v>
       </c>
       <c r="F2" s="2">
-        <v>45948.00208333333</v>
+        <v>45951.570138888885</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>574</v>
+        <v>586</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>157</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>8</v>
+        <v>256</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>573</v>
+        <v>438</v>
       </c>
       <c r="F3" s="2">
-        <v>45948.00208333333</v>
+        <v>45950.648611111115</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>575</v>
+        <v>587</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>576</v>
+        <v>268</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>234</v>
+        <v>376</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>272</v>
+        <v>135</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="F4" s="2">
-        <v>45949.69305555556</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>578</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>579</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45949.60902777778</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>580</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>581</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45947.663888888885</v>
+        <v>45951.55416666667</v>
       </c>
     </row>
   </sheetData>
@@ -6421,8 +6507,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-10-22 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="603">
   <si>
     <t>link</t>
   </si>
@@ -1785,6 +1785,48 @@
   </si>
   <si>
     <t>90580070009</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/ziemera-pag/adhck.html</t>
+  </si>
+  <si>
+    <t>230 000 €</t>
+  </si>
+  <si>
+    <t>36960020096</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/liepnas-pag/oegon.html</t>
+  </si>
+  <si>
+    <t>2.53 ha.</t>
+  </si>
+  <si>
+    <t>36680010066</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kuldiga-and-reg/kurmales-pag/ahdem.html</t>
+  </si>
+  <si>
+    <t>57 000 €</t>
+  </si>
+  <si>
+    <t>62600100122</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/liepaja-and-reg/rucavas-pag/jddck.html</t>
+  </si>
+  <si>
+    <t>140 000 €</t>
+  </si>
+  <si>
+    <t>6484-005-0016/0015</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/laudonas-pag/gkdih.html</t>
+  </si>
+  <si>
+    <t>70700020007</t>
   </si>
 </sst>
 </file>
@@ -2197,7 +2239,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F199"/>
+  <dimension ref="A1:F202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6192,6 +6234,66 @@
       </c>
       <c r="F199" s="2">
         <v>45947.663888888885</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="B200" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="C200" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D200" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="E200" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="F200" s="2">
+        <v>45951.570138888885</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="B201" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C201" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D201" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E201" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="F201" s="2">
+        <v>45950.648611111115</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="B202" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C202" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D202" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E202" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="F202" s="2">
+        <v>45951.55416666667</v>
       </c>
     </row>
   </sheetData>
@@ -6394,6 +6496,9 @@
     <hyperlink ref="A197" r:id="rId196"/>
     <hyperlink ref="A198" r:id="rId197"/>
     <hyperlink ref="A199" r:id="rId198"/>
+    <hyperlink ref="A200" r:id="rId199"/>
+    <hyperlink ref="A201" r:id="rId200"/>
+    <hyperlink ref="A202" r:id="rId201"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -6405,7 +6510,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6444,62 +6549,102 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>583</v>
+        <v>590</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>208</v>
+        <v>435</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>584</v>
+        <v>253</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>585</v>
+        <v>591</v>
       </c>
       <c r="F2" s="2">
-        <v>45951.570138888885</v>
+        <v>45952.45486111111</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>586</v>
+        <v>592</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>256</v>
+        <v>435</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>162</v>
+        <v>593</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>438</v>
+        <v>594</v>
       </c>
       <c r="F3" s="2">
-        <v>45950.648611111115</v>
+        <v>45951.92152777778</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>587</v>
+        <v>595</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>268</v>
+        <v>596</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>376</v>
+        <v>424</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>135</v>
+        <v>44</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>588</v>
+        <v>597</v>
       </c>
       <c r="F4" s="2">
-        <v>45951.55416666667</v>
+        <v>45952.620833333334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45951.76597222222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45952.606944444444</v>
       </c>
     </row>
   </sheetData>
@@ -6507,6 +6652,8 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-10-23 12:17
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -2239,7 +2239,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F202"/>
+  <dimension ref="A1:F207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6294,6 +6294,106 @@
       </c>
       <c r="F202" s="2">
         <v>45951.55416666667</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="B203" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="C203" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D203" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E203" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="F203" s="2">
+        <v>45952.45486111111</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C204" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D204" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="E204" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="F204" s="2">
+        <v>45951.92152777778</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="B205" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="C205" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D205" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E205" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="F205" s="2">
+        <v>45952.620833333334</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="B206" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="C206" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D206" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E206" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="F206" s="2">
+        <v>45951.76597222222</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="B207" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="C207" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D207" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E207" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="F207" s="2">
+        <v>45952.606944444444</v>
       </c>
     </row>
   </sheetData>
@@ -6499,6 +6599,11 @@
     <hyperlink ref="A200" r:id="rId199"/>
     <hyperlink ref="A201" r:id="rId200"/>
     <hyperlink ref="A202" r:id="rId201"/>
+    <hyperlink ref="A203" r:id="rId202"/>
+    <hyperlink ref="A204" r:id="rId203"/>
+    <hyperlink ref="A205" r:id="rId204"/>
+    <hyperlink ref="A206" r:id="rId205"/>
+    <hyperlink ref="A207" r:id="rId206"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -6510,7 +6615,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6547,114 +6652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>589</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>590</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>591</v>
-      </c>
-      <c r="F2" s="2">
-        <v>45952.45486111111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>592</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>593</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>594</v>
-      </c>
-      <c r="F3" s="2">
-        <v>45951.92152777778</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>595</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>596</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>424</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>597</v>
-      </c>
-      <c r="F4" s="2">
-        <v>45952.620833333334</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>598</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>599</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>600</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45951.76597222222</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>601</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>440</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>602</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45952.606944444444</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forests data - 2025-10-24 12:17
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="610">
   <si>
     <t>link</t>
   </si>
@@ -1827,6 +1827,27 @@
   </si>
   <si>
     <t>70700020007</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/maltas-pag/gipgg.html</t>
+  </si>
+  <si>
+    <t>21 600 €</t>
+  </si>
+  <si>
+    <t>5.40 ha.</t>
+  </si>
+  <si>
+    <t>78700070207</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/tukums-and-reg/ceres-pag/ffcml.html</t>
+  </si>
+  <si>
+    <t>70 €</t>
+  </si>
+  <si>
+    <t>90440010002</t>
   </si>
 </sst>
 </file>
@@ -6615,7 +6636,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6652,7 +6673,51 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45954.56736111111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45953.91736111111</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forests data - 2025-10-27 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="631">
   <si>
     <t>link</t>
   </si>
@@ -1848,6 +1848,69 @@
   </si>
   <si>
     <t>90440010002</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/ziguru-pag/dfxge.html</t>
+  </si>
+  <si>
+    <t>38980010052</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/raunas-pag/jjxpi.html</t>
+  </si>
+  <si>
+    <t>42760080028</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jekabpils-and-reg/garsenes-pag/bxojlf.html</t>
+  </si>
+  <si>
+    <t>56620020013</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kalniesu-pag/jxgdk.html</t>
+  </si>
+  <si>
+    <t>60680040608</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/liepaja-and-reg/durbe/gdkpm.html</t>
+  </si>
+  <si>
+    <t>35 ha.</t>
+  </si>
+  <si>
+    <t>64270060039</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/livani/jlngb.html</t>
+  </si>
+  <si>
+    <t>22 500 €</t>
+  </si>
+  <si>
+    <t>76860070184</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/kaunatas-pag/npjbg.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/feimanu-pag/mhedc.html</t>
+  </si>
+  <si>
+    <t>11.83 ha.</t>
+  </si>
+  <si>
+    <t>78520030192</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/talsi-and-reg/kulciema-pag/cdlld.html</t>
+  </si>
+  <si>
+    <t>51 000 €</t>
+  </si>
+  <si>
+    <t>88640040079</t>
   </si>
 </sst>
 </file>
@@ -2260,7 +2323,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F207"/>
+  <dimension ref="A1:F209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6415,6 +6478,46 @@
       </c>
       <c r="F207" s="2">
         <v>45952.606944444444</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="B208" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="C208" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D208" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="E208" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="F208" s="2">
+        <v>45954.56736111111</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="B209" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="C209" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D209" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E209" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="F209" s="2">
+        <v>45953.91736111111</v>
       </c>
     </row>
   </sheetData>
@@ -6625,6 +6728,8 @@
     <hyperlink ref="A205" r:id="rId204"/>
     <hyperlink ref="A206" r:id="rId205"/>
     <hyperlink ref="A207" r:id="rId206"/>
+    <hyperlink ref="A208" r:id="rId207"/>
+    <hyperlink ref="A209" r:id="rId208"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -6636,7 +6741,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6675,48 +6780,195 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>603</v>
+        <v>610</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>604</v>
+        <v>417</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>294</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>605</v>
+        <v>272</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
       <c r="F2" s="2">
-        <v>45954.56736111111</v>
+        <v>45957.40625</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>608</v>
+        <v>52</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>376</v>
+        <v>63</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>186</v>
+        <v>36</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
       <c r="F3" s="2">
-        <v>45953.91736111111</v>
+        <v>45957.49444444444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45955.50069444445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45955.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>620</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45955.42152777778</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="F7" s="2">
+        <v>45957.44236111111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F8" s="2">
+        <v>45957.57430555555</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="F9" s="2">
+        <v>45957.46805555555</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>629</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="F10" s="2">
+        <v>45957.40833333333</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-10-28 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="636">
   <si>
     <t>link</t>
   </si>
@@ -1911,6 +1911,21 @@
   </si>
   <si>
     <t>88640040079</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/medumu-pag/conxg.html</t>
+  </si>
+  <si>
+    <t>23.60 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/udrisu-pag/jokck.html</t>
+  </si>
+  <si>
+    <t>60960050185</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/pasienes-pag/dmgxk.html</t>
   </si>
 </sst>
 </file>
@@ -2323,7 +2338,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F209"/>
+  <dimension ref="A1:F218"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6518,6 +6533,186 @@
       </c>
       <c r="F209" s="2">
         <v>45953.91736111111</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="B210" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C210" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D210" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E210" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="F210" s="2">
+        <v>45957.40625</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="B211" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C211" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D211" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E211" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="F211" s="2">
+        <v>45957.49444444444</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="B212" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="C212" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D212" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E212" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="F212" s="2">
+        <v>45955.50069444445</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="B213" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C213" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D213" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E213" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="F213" s="2">
+        <v>45955.45</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="B214" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C214" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D214" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="E214" s="4" t="s">
+        <v>620</v>
+      </c>
+      <c r="F214" s="2">
+        <v>45955.42152777778</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="B215" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="C215" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D215" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E215" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="F215" s="2">
+        <v>45957.44236111111</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="B216" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C216" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D216" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E216" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F216" s="2">
+        <v>45957.57430555555</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="B217" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C217" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D217" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="E217" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="F217" s="2">
+        <v>45957.46805555555</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="B218" s="4" t="s">
+        <v>629</v>
+      </c>
+      <c r="C218" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D218" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E218" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="F218" s="2">
+        <v>45957.40833333333</v>
       </c>
     </row>
   </sheetData>
@@ -6730,6 +6925,15 @@
     <hyperlink ref="A207" r:id="rId206"/>
     <hyperlink ref="A208" r:id="rId207"/>
     <hyperlink ref="A209" r:id="rId208"/>
+    <hyperlink ref="A210" r:id="rId209"/>
+    <hyperlink ref="A211" r:id="rId210"/>
+    <hyperlink ref="A212" r:id="rId211"/>
+    <hyperlink ref="A213" r:id="rId212"/>
+    <hyperlink ref="A214" r:id="rId213"/>
+    <hyperlink ref="A215" r:id="rId214"/>
+    <hyperlink ref="A216" r:id="rId215"/>
+    <hyperlink ref="A217" r:id="rId216"/>
+    <hyperlink ref="A218" r:id="rId217"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -6741,7 +6945,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6780,182 +6984,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>610</v>
+        <v>631</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>417</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>272</v>
+        <v>632</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>611</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>45957.40625</v>
+        <v>45958.38055555556</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>612</v>
+        <v>633</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>63</v>
+        <v>146</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>613</v>
+        <v>634</v>
       </c>
       <c r="F3" s="2">
-        <v>45957.49444444444</v>
+        <v>45957.61597222222</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>614</v>
+        <v>635</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>596</v>
+        <v>47</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>127</v>
+        <v>234</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>17</v>
+        <v>209</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>615</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2">
-        <v>45955.50069444445</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>616</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>617</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45955.45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>618</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>619</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>620</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45955.42152777778</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>621</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>622</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>623</v>
-      </c>
-      <c r="F7" s="2">
-        <v>45957.44236111111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>624</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="F8" s="2">
-        <v>45957.57430555555</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>625</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>626</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>627</v>
-      </c>
-      <c r="F9" s="2">
-        <v>45957.46805555555</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>628</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>629</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>630</v>
-      </c>
-      <c r="F10" s="2">
-        <v>45957.40833333333</v>
+        <v>45958.51388888889</v>
       </c>
     </row>
   </sheetData>
@@ -6963,12 +7047,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forests data - 2025-10-29 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -2338,7 +2338,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F218"/>
+  <dimension ref="A1:F221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6713,6 +6713,66 @@
       </c>
       <c r="F218" s="2">
         <v>45957.40833333333</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="B219" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C219" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D219" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="E219" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F219" s="2">
+        <v>45958.38055555556</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="B220" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C220" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D220" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E220" s="4" t="s">
+        <v>634</v>
+      </c>
+      <c r="F220" s="2">
+        <v>45957.61597222222</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="B221" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C221" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D221" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E221" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F221" s="2">
+        <v>45958.51388888889</v>
       </c>
     </row>
   </sheetData>
@@ -6934,6 +6994,9 @@
     <hyperlink ref="A216" r:id="rId215"/>
     <hyperlink ref="A217" r:id="rId216"/>
     <hyperlink ref="A218" r:id="rId217"/>
+    <hyperlink ref="A219" r:id="rId218"/>
+    <hyperlink ref="A220" r:id="rId219"/>
+    <hyperlink ref="A221" r:id="rId220"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -6945,7 +7008,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6982,72 +7045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>632</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="2">
-        <v>45958.38055555556</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>633</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>634</v>
-      </c>
-      <c r="F3" s="2">
-        <v>45957.61597222222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>635</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="2">
-        <v>45958.51388888889</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forests data - 2025-10-30 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="645">
   <si>
     <t>link</t>
   </si>
@@ -1926,6 +1926,33 @@
   </si>
   <si>
     <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/pasienes-pag/dmgxk.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aizkraukle-and-reg/bebru-pag/flpfk.html</t>
+  </si>
+  <si>
+    <t>44 000 €</t>
+  </si>
+  <si>
+    <t>9.40 ha.</t>
+  </si>
+  <si>
+    <t>32460010096</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/veclaicenes-pag/bbokfm.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/ape/mjild.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/other/cbxff.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/berzkalnes-pag/iepfl.html</t>
+  </si>
+  <si>
+    <t>38480030078</t>
   </si>
 </sst>
 </file>
@@ -7008,7 +7035,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7045,7 +7072,114 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>637</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>638</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45960.507638888885</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45959.925</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45959.67916666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45959.4875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>644</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45959.757638888885</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2025-10-31 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -2365,7 +2365,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F221"/>
+  <dimension ref="A1:F226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6800,6 +6800,106 @@
       </c>
       <c r="F221" s="2">
         <v>45958.51388888889</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="B222" s="4" t="s">
+        <v>637</v>
+      </c>
+      <c r="C222" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D222" s="4" t="s">
+        <v>638</v>
+      </c>
+      <c r="E222" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="F222" s="2">
+        <v>45960.507638888885</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="B223" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C223" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D223" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E223" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F223" s="2">
+        <v>45959.925</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="B224" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C224" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D224" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E224" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F224" s="2">
+        <v>45959.67916666667</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B225" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C225" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D225" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E225" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F225" s="2">
+        <v>45959.4875</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="B226" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C226" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D226" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E226" s="4" t="s">
+        <v>644</v>
+      </c>
+      <c r="F226" s="2">
+        <v>45959.757638888885</v>
       </c>
     </row>
   </sheetData>
@@ -7024,6 +7124,11 @@
     <hyperlink ref="A219" r:id="rId218"/>
     <hyperlink ref="A220" r:id="rId219"/>
     <hyperlink ref="A221" r:id="rId220"/>
+    <hyperlink ref="A222" r:id="rId221"/>
+    <hyperlink ref="A223" r:id="rId222"/>
+    <hyperlink ref="A224" r:id="rId223"/>
+    <hyperlink ref="A225" r:id="rId224"/>
+    <hyperlink ref="A226" r:id="rId225"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -7035,7 +7140,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7072,114 +7177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>636</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>637</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>638</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>639</v>
-      </c>
-      <c r="F2" s="2">
-        <v>45960.507638888885</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>640</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="2">
-        <v>45959.925</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>641</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="2">
-        <v>45959.67916666667</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>642</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45959.4875</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>644</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45959.757638888885</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2025-11-03 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="663">
   <si>
     <t>link</t>
   </si>
@@ -1953,6 +1953,60 @@
   </si>
   <si>
     <t>38480030078</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/susaju-pag/adhce.html</t>
+  </si>
+  <si>
+    <t>38780090009</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/zaubes-pag/hfoib.html</t>
+  </si>
+  <si>
+    <t>42960040023</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/gulbene-and-reg/ligo-pag/hkmoh.html</t>
+  </si>
+  <si>
+    <t>24 000 €</t>
+  </si>
+  <si>
+    <t>3.90 ha.</t>
+  </si>
+  <si>
+    <t>50760010181</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/madona/icelo.html</t>
+  </si>
+  <si>
+    <t>70860050034</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/barkavas-pag/exmih.html</t>
+  </si>
+  <si>
+    <t>43 210 €</t>
+  </si>
+  <si>
+    <t>70440010024</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/rozupes-pag/bfcbx.html</t>
+  </si>
+  <si>
+    <t>1.20 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ventspils-and-reg/usmas-pag/gfedj.html</t>
+  </si>
+  <si>
+    <t>5 100 €</t>
+  </si>
+  <si>
+    <t>98740060258</t>
   </si>
 </sst>
 </file>
@@ -7140,7 +7194,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7177,7 +7231,156 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45962.76180555555</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45964.41736111111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45964.55347222222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45964.53055555555</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45964.50069444445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="2">
+        <v>45961.898611111115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="F8" s="2">
+        <v>45964.34722222222</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2025-11-04 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -2419,7 +2419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F226"/>
+  <dimension ref="A1:F233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6954,6 +6954,146 @@
       </c>
       <c r="F226" s="2">
         <v>45959.757638888885</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="B227" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C227" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D227" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E227" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="F227" s="2">
+        <v>45962.76180555555</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="B228" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C228" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D228" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E228" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="F228" s="2">
+        <v>45964.41736111111</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="B229" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="C229" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D229" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="E229" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="F229" s="2">
+        <v>45964.55347222222</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="B230" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C230" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D230" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E230" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="F230" s="2">
+        <v>45964.53055555555</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="B231" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="C231" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D231" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E231" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="F231" s="2">
+        <v>45964.50069444445</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="B232" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C232" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D232" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="E232" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F232" s="2">
+        <v>45961.898611111115</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="B233" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="C233" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="D233" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E233" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="F233" s="2">
+        <v>45964.34722222222</v>
       </c>
     </row>
   </sheetData>
@@ -7183,6 +7323,13 @@
     <hyperlink ref="A224" r:id="rId223"/>
     <hyperlink ref="A225" r:id="rId224"/>
     <hyperlink ref="A226" r:id="rId225"/>
+    <hyperlink ref="A227" r:id="rId226"/>
+    <hyperlink ref="A228" r:id="rId227"/>
+    <hyperlink ref="A229" r:id="rId228"/>
+    <hyperlink ref="A230" r:id="rId229"/>
+    <hyperlink ref="A231" r:id="rId230"/>
+    <hyperlink ref="A232" r:id="rId231"/>
+    <hyperlink ref="A233" r:id="rId232"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -7194,7 +7341,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7231,156 +7378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>645</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>646</v>
-      </c>
-      <c r="F2" s="2">
-        <v>45962.76180555555</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>647</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>648</v>
-      </c>
-      <c r="F3" s="2">
-        <v>45964.41736111111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>649</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>650</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>651</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>652</v>
-      </c>
-      <c r="F4" s="2">
-        <v>45964.55347222222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>653</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>654</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45964.53055555555</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>655</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>656</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>657</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45964.50069444445</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>658</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>659</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="2">
-        <v>45961.898611111115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>660</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>661</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>662</v>
-      </c>
-      <c r="F8" s="2">
-        <v>45964.34722222222</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2025-11-05 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="668">
   <si>
     <t>link</t>
   </si>
@@ -2007,6 +2007,21 @@
   </si>
   <si>
     <t>98740060258</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/andzelu-pag/ahddd.html</t>
+  </si>
+  <si>
+    <t>60440050273</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/liepupes-pag/cghcmh.html</t>
+  </si>
+  <si>
+    <t>160 000 €</t>
+  </si>
+  <si>
+    <t>66600100005</t>
   </si>
 </sst>
 </file>
@@ -7341,7 +7356,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7378,7 +7393,51 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>664</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45966.46666666667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>666</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>667</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45965.868055555555</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2025-11-06 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="683">
   <si>
     <t>link</t>
   </si>
@@ -2022,6 +2022,51 @@
   </si>
   <si>
     <t>66600100005</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/nitaures-pag/ipbpn.html</t>
+  </si>
+  <si>
+    <t>275 000 €</t>
+  </si>
+  <si>
+    <t>49 ha.</t>
+  </si>
+  <si>
+    <t>42680070004</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/liepaja-and-reg/rucavas-pag/pcgli.html</t>
+  </si>
+  <si>
+    <t>115 000 €</t>
+  </si>
+  <si>
+    <t>64780230003</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/ciblas-pag/cxxhx.html</t>
+  </si>
+  <si>
+    <t>68480060001</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/laudonas-pag/hejed.html</t>
+  </si>
+  <si>
+    <t>70700070463</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/rusonas-pag/ghjgx.html</t>
+  </si>
+  <si>
+    <t>76700110070</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/rusonas-pag/ijexp.html</t>
+  </si>
+  <si>
+    <t>76700080013</t>
   </si>
 </sst>
 </file>
@@ -2434,7 +2479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F233"/>
+  <dimension ref="A1:F235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7109,6 +7154,46 @@
       </c>
       <c r="F233" s="2">
         <v>45964.34722222222</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="B234" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="C234" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D234" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E234" s="4" t="s">
+        <v>664</v>
+      </c>
+      <c r="F234" s="2">
+        <v>45966.46666666667</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="B235" s="4" t="s">
+        <v>666</v>
+      </c>
+      <c r="C235" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D235" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E235" s="4" t="s">
+        <v>667</v>
+      </c>
+      <c r="F235" s="2">
+        <v>45965.868055555555</v>
       </c>
     </row>
   </sheetData>
@@ -7345,6 +7430,8 @@
     <hyperlink ref="A231" r:id="rId230"/>
     <hyperlink ref="A232" r:id="rId231"/>
     <hyperlink ref="A233" r:id="rId232"/>
+    <hyperlink ref="A234" r:id="rId233"/>
+    <hyperlink ref="A235" r:id="rId234"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -7356,7 +7443,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7395,48 +7482,132 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>663</v>
+        <v>668</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>497</v>
+        <v>669</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>146</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>75</v>
+        <v>670</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>664</v>
+        <v>671</v>
       </c>
       <c r="F2" s="2">
-        <v>45966.46666666667</v>
+        <v>45966.61041666666</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>665</v>
+        <v>672</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>666</v>
+        <v>673</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>667</v>
+        <v>674</v>
       </c>
       <c r="F3" s="2">
-        <v>45965.868055555555</v>
+        <v>45966.66875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>676</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45967.46666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>678</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45966.620833333334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>680</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45967.476388888885</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="F7" s="2">
+        <v>45967.47361111111</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-11-07 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="688">
   <si>
     <t>link</t>
   </si>
@@ -2067,6 +2067,21 @@
   </si>
   <si>
     <t>76700080013</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/raunas-pag/ndcjg.html</t>
+  </si>
+  <si>
+    <t>116 000 €</t>
+  </si>
+  <si>
+    <t>42760010118,</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/salacgrivas-l-t/lcnpc.html</t>
+  </si>
+  <si>
+    <t>66720030013</t>
   </si>
 </sst>
 </file>
@@ -2479,7 +2494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F235"/>
+  <dimension ref="A1:F241"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7194,6 +7209,126 @@
       </c>
       <c r="F235" s="2">
         <v>45965.868055555555</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="B236" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="C236" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D236" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="E236" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="F236" s="2">
+        <v>45966.61041666666</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="B237" s="4" t="s">
+        <v>673</v>
+      </c>
+      <c r="C237" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D237" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E237" s="4" t="s">
+        <v>674</v>
+      </c>
+      <c r="F237" s="2">
+        <v>45966.66875</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="B238" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="C238" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D238" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E238" s="4" t="s">
+        <v>676</v>
+      </c>
+      <c r="F238" s="2">
+        <v>45967.46666666667</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A239" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="B239" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C239" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D239" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E239" s="4" t="s">
+        <v>678</v>
+      </c>
+      <c r="F239" s="2">
+        <v>45966.620833333334</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A240" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="B240" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C240" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D240" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E240" s="4" t="s">
+        <v>680</v>
+      </c>
+      <c r="F240" s="2">
+        <v>45967.476388888885</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="B241" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C241" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D241" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E241" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="F241" s="2">
+        <v>45967.47361111111</v>
       </c>
     </row>
   </sheetData>
@@ -7432,6 +7567,12 @@
     <hyperlink ref="A233" r:id="rId232"/>
     <hyperlink ref="A234" r:id="rId233"/>
     <hyperlink ref="A235" r:id="rId234"/>
+    <hyperlink ref="A236" r:id="rId235"/>
+    <hyperlink ref="A237" r:id="rId236"/>
+    <hyperlink ref="A238" r:id="rId237"/>
+    <hyperlink ref="A239" r:id="rId238"/>
+    <hyperlink ref="A240" r:id="rId239"/>
+    <hyperlink ref="A241" r:id="rId240"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -7443,7 +7584,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7482,132 +7623,48 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>668</v>
+        <v>683</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>669</v>
+        <v>684</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>670</v>
+        <v>71</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>671</v>
+        <v>685</v>
       </c>
       <c r="F2" s="2">
-        <v>45966.61041666666</v>
+        <v>45968.40625</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>672</v>
+        <v>686</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>673</v>
+        <v>217</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>674</v>
+        <v>687</v>
       </c>
       <c r="F3" s="2">
-        <v>45966.66875</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>675</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>650</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>676</v>
-      </c>
-      <c r="F4" s="2">
-        <v>45967.46666666667</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>678</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45966.620833333334</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>679</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>680</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45967.476388888885</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>681</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>682</v>
-      </c>
-      <c r="F7" s="2">
-        <v>45967.47361111111</v>
+        <v>45967.89583333333</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-11-10 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="697">
   <si>
     <t>link</t>
   </si>
@@ -2082,6 +2082,33 @@
   </si>
   <si>
     <t>66720030013</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/naujenes-pag/iokhx.html</t>
+  </si>
+  <si>
+    <t>44740090231</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kalniesu-pag/bexeig.html</t>
+  </si>
+  <si>
+    <t>60680040476</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/metrienas-pag/pglli.html</t>
+  </si>
+  <si>
+    <t>70760050003</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/cornajas-pag/ikbfo.html</t>
+  </si>
+  <si>
+    <t>11.50 ha.</t>
+  </si>
+  <si>
+    <t>78460090131</t>
   </si>
 </sst>
 </file>
@@ -2494,7 +2521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F241"/>
+  <dimension ref="A1:F243"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7329,6 +7356,46 @@
       </c>
       <c r="F241" s="2">
         <v>45967.47361111111</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="B242" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="C242" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D242" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E242" s="4" t="s">
+        <v>685</v>
+      </c>
+      <c r="F242" s="2">
+        <v>45968.40625</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="B243" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C243" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D243" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E243" s="4" t="s">
+        <v>687</v>
+      </c>
+      <c r="F243" s="2">
+        <v>45967.89583333333</v>
       </c>
     </row>
   </sheetData>
@@ -7573,6 +7640,8 @@
     <hyperlink ref="A239" r:id="rId238"/>
     <hyperlink ref="A240" r:id="rId239"/>
     <hyperlink ref="A241" r:id="rId240"/>
+    <hyperlink ref="A242" r:id="rId241"/>
+    <hyperlink ref="A243" r:id="rId242"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -7584,7 +7653,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7623,48 +7692,90 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>684</v>
+        <v>134</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>685</v>
+        <v>689</v>
       </c>
       <c r="F2" s="2">
-        <v>45968.40625</v>
+        <v>45968.709027777775</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>217</v>
+        <v>116</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>208</v>
+        <v>146</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>24</v>
+        <v>135</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>687</v>
+        <v>691</v>
       </c>
       <c r="F3" s="2">
-        <v>45967.89583333333</v>
+        <v>45968.99444444444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>693</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45970.81180555555</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>695</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45969.950694444444</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-11-11 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="706">
   <si>
     <t>link</t>
   </si>
@@ -2109,6 +2109,33 @@
   </si>
   <si>
     <t>78460090131</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/jaunlaicenes-pag/kldlj.html</t>
+  </si>
+  <si>
+    <t>692 000 €</t>
+  </si>
+  <si>
+    <t>30 ha.</t>
+  </si>
+  <si>
+    <t>36600010045</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/berzpils-pag/hiidj.html</t>
+  </si>
+  <si>
+    <t>1.85 ha.</t>
+  </si>
+  <si>
+    <t>38500050070</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kuldiga-and-reg/padures-pag/pefdd.html</t>
+  </si>
+  <si>
+    <t>62720010352</t>
   </si>
 </sst>
 </file>
@@ -2521,7 +2548,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F243"/>
+  <dimension ref="A1:F247"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7396,6 +7423,86 @@
       </c>
       <c r="F243" s="2">
         <v>45967.89583333333</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="B244" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C244" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D244" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E244" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="F244" s="2">
+        <v>45968.709027777775</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A245" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="B245" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C245" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D245" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E245" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="F245" s="2">
+        <v>45968.99444444444</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A246" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="B246" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C246" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D246" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E246" s="4" t="s">
+        <v>693</v>
+      </c>
+      <c r="F246" s="2">
+        <v>45970.81180555555</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A247" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="B247" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C247" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D247" s="4" t="s">
+        <v>695</v>
+      </c>
+      <c r="E247" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="F247" s="2">
+        <v>45969.950694444444</v>
       </c>
     </row>
   </sheetData>
@@ -7642,6 +7749,10 @@
     <hyperlink ref="A241" r:id="rId240"/>
     <hyperlink ref="A242" r:id="rId241"/>
     <hyperlink ref="A243" r:id="rId242"/>
+    <hyperlink ref="A244" r:id="rId243"/>
+    <hyperlink ref="A245" r:id="rId244"/>
+    <hyperlink ref="A246" r:id="rId245"/>
+    <hyperlink ref="A247" r:id="rId246"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -7653,7 +7764,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7692,82 +7803,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>688</v>
+        <v>697</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>134</v>
+        <v>698</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>74</v>
+        <v>435</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>82</v>
+        <v>699</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>689</v>
+        <v>700</v>
       </c>
       <c r="F2" s="2">
-        <v>45968.709027777775</v>
+        <v>45972.04791666666</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>690</v>
+        <v>701</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>116</v>
+        <v>355</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>146</v>
+        <v>28</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>135</v>
+        <v>702</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>691</v>
+        <v>703</v>
       </c>
       <c r="F3" s="2">
-        <v>45968.99444444444</v>
+        <v>45971.86388888889</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>692</v>
+        <v>704</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>467</v>
+        <v>116</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>256</v>
+        <v>424</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>186</v>
+        <v>272</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>693</v>
+        <v>705</v>
       </c>
       <c r="F4" s="2">
-        <v>45970.81180555555</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>694</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>695</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>696</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45969.950694444444</v>
+        <v>45971.941666666666</v>
       </c>
     </row>
   </sheetData>
@@ -7775,7 +7866,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-11-12 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="715">
   <si>
     <t>link</t>
   </si>
@@ -2136,6 +2136,33 @@
   </si>
   <si>
     <t>62720010352</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/varaklanu-pag/lhxco.html</t>
+  </si>
+  <si>
+    <t>17 000 €</t>
+  </si>
+  <si>
+    <t>70940030278</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ogre-and-reg/madlienas-pag/jnckk.html</t>
+  </si>
+  <si>
+    <t>74680050043</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/silukalna-pag/mpfce.html</t>
+  </si>
+  <si>
+    <t>76780010113</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/valmiera-and-reg/valmieras-pag/ipkdk.html</t>
+  </si>
+  <si>
+    <t>94540010130</t>
   </si>
 </sst>
 </file>
@@ -2548,7 +2575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F247"/>
+  <dimension ref="A1:F250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7503,6 +7530,66 @@
       </c>
       <c r="F247" s="2">
         <v>45969.950694444444</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A248" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="B248" s="4" t="s">
+        <v>698</v>
+      </c>
+      <c r="C248" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D248" s="4" t="s">
+        <v>699</v>
+      </c>
+      <c r="E248" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="F248" s="2">
+        <v>45972.04791666666</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="B249" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C249" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D249" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="E249" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="F249" s="2">
+        <v>45971.86388888889</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="B250" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C250" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D250" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E250" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="F250" s="2">
+        <v>45971.941666666666</v>
       </c>
     </row>
   </sheetData>
@@ -7753,6 +7840,9 @@
     <hyperlink ref="A245" r:id="rId244"/>
     <hyperlink ref="A246" r:id="rId245"/>
     <hyperlink ref="A247" r:id="rId246"/>
+    <hyperlink ref="A248" r:id="rId247"/>
+    <hyperlink ref="A249" r:id="rId248"/>
+    <hyperlink ref="A250" r:id="rId249"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -7764,7 +7854,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7803,62 +7893,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>697</v>
+        <v>706</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>698</v>
+        <v>707</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>435</v>
+        <v>256</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>699</v>
+        <v>186</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>700</v>
+        <v>708</v>
       </c>
       <c r="F2" s="2">
-        <v>45972.04791666666</v>
+        <v>45972.90486111111</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>701</v>
+        <v>709</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>355</v>
+        <v>150</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>28</v>
+        <v>275</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>702</v>
+        <v>36</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>703</v>
+        <v>710</v>
       </c>
       <c r="F3" s="2">
-        <v>45971.86388888889</v>
+        <v>45973.43402777778</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>704</v>
+        <v>711</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>116</v>
+        <v>31</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>424</v>
+        <v>284</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>272</v>
+        <v>82</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>705</v>
+        <v>712</v>
       </c>
       <c r="F4" s="2">
-        <v>45971.941666666666</v>
+        <v>45972.90347222222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>714</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45973.433333333334</v>
       </c>
     </row>
   </sheetData>
@@ -7866,6 +7976,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-11-13 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -2575,7 +2575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F250"/>
+  <dimension ref="A1:F254"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7590,6 +7590,86 @@
       </c>
       <c r="F250" s="2">
         <v>45971.941666666666</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="B251" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="C251" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D251" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E251" s="4" t="s">
+        <v>708</v>
+      </c>
+      <c r="F251" s="2">
+        <v>45972.90486111111</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="B252" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C252" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D252" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E252" s="4" t="s">
+        <v>710</v>
+      </c>
+      <c r="F252" s="2">
+        <v>45973.43402777778</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="B253" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C253" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D253" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E253" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="F253" s="2">
+        <v>45972.90347222222</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="B254" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C254" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="D254" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E254" s="4" t="s">
+        <v>714</v>
+      </c>
+      <c r="F254" s="2">
+        <v>45973.433333333334</v>
       </c>
     </row>
   </sheetData>
@@ -7843,6 +7923,10 @@
     <hyperlink ref="A248" r:id="rId247"/>
     <hyperlink ref="A249" r:id="rId248"/>
     <hyperlink ref="A250" r:id="rId249"/>
+    <hyperlink ref="A251" r:id="rId250"/>
+    <hyperlink ref="A252" r:id="rId251"/>
+    <hyperlink ref="A253" r:id="rId252"/>
+    <hyperlink ref="A254" r:id="rId253"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -7854,7 +7938,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7891,93 +7975,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>706</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>707</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>708</v>
-      </c>
-      <c r="F2" s="2">
-        <v>45972.90486111111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>709</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>710</v>
-      </c>
-      <c r="F3" s="2">
-        <v>45973.43402777778</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>711</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>712</v>
-      </c>
-      <c r="F4" s="2">
-        <v>45972.90347222222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>713</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>714</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45973.433333333334</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2025-11-14 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="720">
   <si>
     <t>link</t>
   </si>
@@ -2163,6 +2163,21 @@
   </si>
   <si>
     <t>94540010130</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/vectilzas-pag/jiedm.html</t>
+  </si>
+  <si>
+    <t>8.20 ha.</t>
+  </si>
+  <si>
+    <t>3890004066</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/liepaja-and-reg/dunikas-pag/dipeh.html</t>
+  </si>
+  <si>
+    <t>64520060019</t>
   </si>
 </sst>
 </file>
@@ -7938,7 +7953,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7975,7 +7990,51 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>717</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45974.81597222222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>719</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45975.43680555555</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2025-11-17 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="739">
   <si>
     <t>link</t>
   </si>
@@ -2178,6 +2178,63 @@
   </si>
   <si>
     <t>64520060019</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/ligatnes-pag/bgnghf.html</t>
+  </si>
+  <si>
+    <t>280 000 €</t>
+  </si>
+  <si>
+    <t>42620110056</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/laucesas-pag/adhnd.html</t>
+  </si>
+  <si>
+    <t>0.60 ha.</t>
+  </si>
+  <si>
+    <t>44640030164</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jekabpils-and-reg/dunavas-pag/mbdni.html</t>
+  </si>
+  <si>
+    <t>8.30 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kuldiga-and-reg/padures-pag/cghhpx.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/indranu-pag/bgcpkd.html</t>
+  </si>
+  <si>
+    <t>70580160044</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/erglu-pag/ekgnc.html</t>
+  </si>
+  <si>
+    <t>66 ha.</t>
+  </si>
+  <si>
+    <t>70540100032</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/turku-pag/cmcnb.html</t>
+  </si>
+  <si>
+    <t>76860060151</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/ozolmuizas-pag/blmkl.html</t>
+  </si>
+  <si>
+    <t>1.70 ha.</t>
+  </si>
+  <si>
+    <t>78780040220</t>
   </si>
 </sst>
 </file>
@@ -2590,7 +2647,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F254"/>
+  <dimension ref="A1:F256"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7685,6 +7742,46 @@
       </c>
       <c r="F254" s="2">
         <v>45973.433333333334</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="B255" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C255" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D255" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="E255" s="4" t="s">
+        <v>717</v>
+      </c>
+      <c r="F255" s="2">
+        <v>45974.81597222222</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="B256" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C256" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D256" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E256" s="4" t="s">
+        <v>719</v>
+      </c>
+      <c r="F256" s="2">
+        <v>45975.43680555555</v>
       </c>
     </row>
   </sheetData>
@@ -7942,6 +8039,8 @@
     <hyperlink ref="A252" r:id="rId251"/>
     <hyperlink ref="A253" r:id="rId252"/>
     <hyperlink ref="A254" r:id="rId253"/>
+    <hyperlink ref="A255" r:id="rId254"/>
+    <hyperlink ref="A256" r:id="rId255"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -7953,7 +8052,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7992,48 +8091,174 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>715</v>
+        <v>720</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>52</v>
+        <v>721</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>716</v>
+        <v>253</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>717</v>
+        <v>722</v>
       </c>
       <c r="F2" s="2">
-        <v>45974.81597222222</v>
+        <v>45977.620833333334</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>718</v>
+        <v>723</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>725</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45976.65694444445</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>727</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45977.53263888889</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>728</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45976.63402777778</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>719</v>
-      </c>
-      <c r="F3" s="2">
-        <v>45975.43680555555</v>
+      <c r="C6" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45976.81736111111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="F7" s="2">
+        <v>45975.68472222222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>735</v>
+      </c>
+      <c r="F8" s="2">
+        <v>45977.50902777778</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>737</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>738</v>
+      </c>
+      <c r="F9" s="2">
+        <v>45978.495833333334</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-11-18 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="740">
   <si>
     <t>link</t>
   </si>
@@ -2235,6 +2235,9 @@
   </si>
   <si>
     <t>78780040220</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/vecumu-pag/dkpmp.html</t>
   </si>
 </sst>
 </file>
@@ -2647,7 +2650,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F256"/>
+  <dimension ref="A1:F264"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7782,6 +7785,166 @@
       </c>
       <c r="F256" s="2">
         <v>45975.43680555555</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="B257" s="4" t="s">
+        <v>721</v>
+      </c>
+      <c r="C257" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D257" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E257" s="4" t="s">
+        <v>722</v>
+      </c>
+      <c r="F257" s="2">
+        <v>45977.620833333334</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A258" s="3" t="s">
+        <v>723</v>
+      </c>
+      <c r="B258" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C258" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D258" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="E258" s="4" t="s">
+        <v>725</v>
+      </c>
+      <c r="F258" s="2">
+        <v>45976.65694444445</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="B259" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C259" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D259" s="4" t="s">
+        <v>727</v>
+      </c>
+      <c r="E259" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F259" s="2">
+        <v>45977.53263888889</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260" s="3" t="s">
+        <v>728</v>
+      </c>
+      <c r="B260" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C260" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D260" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E260" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="F260" s="2">
+        <v>45976.63402777778</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="B261" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C261" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D261" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E261" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="F261" s="2">
+        <v>45976.81736111111</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="B262" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="C262" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D262" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="E262" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="F262" s="2">
+        <v>45975.68472222222</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="B263" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="C263" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D263" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="E263" s="4" t="s">
+        <v>735</v>
+      </c>
+      <c r="F263" s="2">
+        <v>45977.50902777778</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="B264" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C264" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D264" s="4" t="s">
+        <v>737</v>
+      </c>
+      <c r="E264" s="4" t="s">
+        <v>738</v>
+      </c>
+      <c r="F264" s="2">
+        <v>45978.495833333334</v>
       </c>
     </row>
   </sheetData>
@@ -8041,6 +8204,14 @@
     <hyperlink ref="A254" r:id="rId253"/>
     <hyperlink ref="A255" r:id="rId254"/>
     <hyperlink ref="A256" r:id="rId255"/>
+    <hyperlink ref="A257" r:id="rId256"/>
+    <hyperlink ref="A258" r:id="rId257"/>
+    <hyperlink ref="A259" r:id="rId258"/>
+    <hyperlink ref="A260" r:id="rId259"/>
+    <hyperlink ref="A261" r:id="rId260"/>
+    <hyperlink ref="A262" r:id="rId261"/>
+    <hyperlink ref="A263" r:id="rId262"/>
+    <hyperlink ref="A264" r:id="rId263"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -8052,7 +8223,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8091,174 +8262,27 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>720</v>
+        <v>739</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>721</v>
+        <v>52</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>253</v>
+        <v>702</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>722</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>45977.620833333334</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>723</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>576</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>724</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>725</v>
-      </c>
-      <c r="F3" s="2">
-        <v>45976.65694444445</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>726</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>727</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="2">
-        <v>45977.53263888889</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>728</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>424</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>468</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45976.63402777778</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>729</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>730</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45976.81736111111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>513</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>732</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>733</v>
-      </c>
-      <c r="F7" s="2">
-        <v>45975.68472222222</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>734</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>470</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>735</v>
-      </c>
-      <c r="F8" s="2">
-        <v>45977.50902777778</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>736</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>737</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>738</v>
-      </c>
-      <c r="F9" s="2">
-        <v>45978.495833333334</v>
+        <v>45978.76111111111</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-11-19 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="742">
   <si>
     <t>link</t>
   </si>
@@ -2238,6 +2238,12 @@
   </si>
   <si>
     <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/vecumu-pag/dkpmp.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/makonkalna-pag/ipcgg.html</t>
+  </si>
+  <si>
+    <t>78720020189</t>
   </si>
 </sst>
 </file>
@@ -2650,7 +2656,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F264"/>
+  <dimension ref="A1:F265"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7945,6 +7951,26 @@
       </c>
       <c r="F264" s="2">
         <v>45978.495833333334</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="B265" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C265" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D265" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="E265" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F265" s="2">
+        <v>45978.76111111111</v>
       </c>
     </row>
   </sheetData>
@@ -8212,6 +8238,7 @@
     <hyperlink ref="A262" r:id="rId261"/>
     <hyperlink ref="A263" r:id="rId262"/>
     <hyperlink ref="A264" r:id="rId263"/>
+    <hyperlink ref="A265" r:id="rId264"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -8262,22 +8289,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>52</v>
+        <v>134</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>294</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>702</v>
+        <v>67</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>741</v>
       </c>
       <c r="F2" s="2">
-        <v>45978.76111111111</v>
+        <v>45979.790972222225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update forest data - 2025-11-20 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="742">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="754">
   <si>
     <t>link</t>
   </si>
@@ -2244,6 +2244,42 @@
   </si>
   <si>
     <t>78720020189</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/raiskuma-pag/kkblb.html</t>
+  </si>
+  <si>
+    <t>42740020022</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/indras-pag/giidl.html</t>
+  </si>
+  <si>
+    <t>49 000 €</t>
+  </si>
+  <si>
+    <t>60620040186</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/jumurdas-pag/jimne.html</t>
+  </si>
+  <si>
+    <t>70600080001</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/talsi-and-reg/mersraga-pag/ljdbi.html</t>
+  </si>
+  <si>
+    <t>88780040262</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/tukums-and-reg/degoles-pag/fjjfk.html</t>
+  </si>
+  <si>
+    <t>12 600 €</t>
+  </si>
+  <si>
+    <t>90460040053</t>
   </si>
 </sst>
 </file>
@@ -2656,7 +2692,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F265"/>
+  <dimension ref="A1:F266"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7971,6 +8007,26 @@
       </c>
       <c r="F265" s="2">
         <v>45978.76111111111</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="B266" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C266" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D266" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E266" s="4" t="s">
+        <v>741</v>
+      </c>
+      <c r="F266" s="2">
+        <v>45979.790972222225</v>
       </c>
     </row>
   </sheetData>
@@ -8239,6 +8295,7 @@
     <hyperlink ref="A263" r:id="rId262"/>
     <hyperlink ref="A264" r:id="rId263"/>
     <hyperlink ref="A265" r:id="rId264"/>
+    <hyperlink ref="A266" r:id="rId265"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -8250,7 +8307,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8289,27 +8346,111 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>134</v>
+        <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>294</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="F2" s="2">
-        <v>45979.790972222225</v>
+        <v>45981.56805555556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>745</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>746</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45980.875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>748</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45980.62430555555</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>749</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45981.5625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>751</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>752</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>753</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45981.558333333334</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-11-21 12:18
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="758">
   <si>
     <t>link</t>
   </si>
@@ -2280,6 +2280,18 @@
   </si>
   <si>
     <t>90460040053</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/talsi-and-reg/dundagas-pag/mjdlj.html</t>
+  </si>
+  <si>
+    <t>169 000 €</t>
+  </si>
+  <si>
+    <t>59 ha.</t>
+  </si>
+  <si>
+    <t>88500020198</t>
   </si>
 </sst>
 </file>
@@ -2692,7 +2704,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F266"/>
+  <dimension ref="A1:F271"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8027,6 +8039,106 @@
       </c>
       <c r="F266" s="2">
         <v>45979.790972222225</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="B267" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C267" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D267" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E267" s="4" t="s">
+        <v>743</v>
+      </c>
+      <c r="F267" s="2">
+        <v>45981.56805555556</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="B268" s="4" t="s">
+        <v>745</v>
+      </c>
+      <c r="C268" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D268" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E268" s="4" t="s">
+        <v>746</v>
+      </c>
+      <c r="F268" s="2">
+        <v>45980.875</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B269" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C269" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D269" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="E269" s="4" t="s">
+        <v>748</v>
+      </c>
+      <c r="F269" s="2">
+        <v>45980.62430555555</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270" s="3" t="s">
+        <v>749</v>
+      </c>
+      <c r="B270" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C270" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D270" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E270" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="F270" s="2">
+        <v>45981.5625</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271" s="3" t="s">
+        <v>751</v>
+      </c>
+      <c r="B271" s="4" t="s">
+        <v>752</v>
+      </c>
+      <c r="C271" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D271" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E271" s="4" t="s">
+        <v>753</v>
+      </c>
+      <c r="F271" s="2">
+        <v>45981.558333333334</v>
       </c>
     </row>
   </sheetData>
@@ -8296,6 +8408,11 @@
     <hyperlink ref="A264" r:id="rId263"/>
     <hyperlink ref="A265" r:id="rId264"/>
     <hyperlink ref="A266" r:id="rId265"/>
+    <hyperlink ref="A267" r:id="rId266"/>
+    <hyperlink ref="A268" r:id="rId267"/>
+    <hyperlink ref="A269" r:id="rId268"/>
+    <hyperlink ref="A270" r:id="rId269"/>
+    <hyperlink ref="A271" r:id="rId270"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -8307,7 +8424,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8346,111 +8463,27 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>31</v>
+        <v>755</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>63</v>
+        <v>356</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>59</v>
+        <v>756</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>743</v>
+        <v>757</v>
       </c>
       <c r="F2" s="2">
-        <v>45981.56805555556</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>744</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>745</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>746</v>
-      </c>
-      <c r="F3" s="2">
-        <v>45980.875</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>747</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>748</v>
-      </c>
-      <c r="F4" s="2">
-        <v>45980.62430555555</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>749</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>750</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45981.5625</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>751</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>752</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>753</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45981.558333333334</v>
+        <v>45982.368055555555</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-11-24 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="776">
   <si>
     <t>link</t>
   </si>
@@ -2292,6 +2292,60 @@
   </si>
   <si>
     <t>88500020198</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/jaunlaicenes-pag/kxjph.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/berzpils-pag/hiidj.html?_gl=1*1u7cuf1*_up*MQ..*_ga*ODQ5MTg2ODA0LjE3NjM5ODY3Mzk.*_ga_ZCGHC71BQ2*czE3NjM5ODY3MzkkbzEkZzAkdDE3NjM5ODY3MzkkajYwJGwwJGgw</t>
+  </si>
+  <si>
+    <t>24 500 €</t>
+  </si>
+  <si>
+    <t>1.80 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/berzpils-pag/hbxpx.html?_gl=1*17t3g13*_up*MQ..*_ga*MTI2Mzg3NDExOS4xNzYzOTg2NzQw*_ga_ZCGHC71BQ2*czE3NjM5ODY3MzkkbzEkZzAkdDE3NjM5ODY3MzkkajYwJGwwJGgw</t>
+  </si>
+  <si>
+    <t>38500030175</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/gulbene-and-reg/litenes-pag/gmxfh.html</t>
+  </si>
+  <si>
+    <t>50680070035</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jekabpils-and-reg/atasienes-pag/cndok.html</t>
+  </si>
+  <si>
+    <t>56460030122</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/aulejas-pag/opgnm.html</t>
+  </si>
+  <si>
+    <t>60480030114</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/malnavas-pag/iiemg.html</t>
+  </si>
+  <si>
+    <t>68680060098</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/talsi-and-reg/ives-pag/bxkod.html</t>
+  </si>
+  <si>
+    <t>1 080 000 €</t>
+  </si>
+  <si>
+    <t>40 ha.</t>
+  </si>
+  <si>
+    <t>88580020037</t>
   </si>
 </sst>
 </file>
@@ -2704,7 +2758,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F271"/>
+  <dimension ref="A1:F272"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8139,6 +8193,26 @@
       </c>
       <c r="F271" s="2">
         <v>45981.558333333334</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="B272" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="C272" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D272" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="E272" s="4" t="s">
+        <v>757</v>
+      </c>
+      <c r="F272" s="2">
+        <v>45982.368055555555</v>
       </c>
     </row>
   </sheetData>
@@ -8413,6 +8487,7 @@
     <hyperlink ref="A269" r:id="rId268"/>
     <hyperlink ref="A270" r:id="rId269"/>
     <hyperlink ref="A271" r:id="rId270"/>
+    <hyperlink ref="A272" r:id="rId271"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -8424,7 +8499,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8463,27 +8538,174 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>755</v>
+        <v>698</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>699</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45984.62013888889</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>760</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>761</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45982.84305555555</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>762</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>763</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45982.70277777778</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>765</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45984.84722222222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>766</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>767</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45983.822222222225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>769</v>
+      </c>
+      <c r="F7" s="2">
+        <v>45985.59583333333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>770</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>771</v>
+      </c>
+      <c r="F8" s="2">
+        <v>45983.424305555556</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>773</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>756</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2" s="2">
-        <v>45982.368055555555</v>
+      <c r="D9" s="4" t="s">
+        <v>774</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>775</v>
+      </c>
+      <c r="F9" s="2">
+        <v>45983.527083333334</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-11-25 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="783">
   <si>
     <t>link</t>
   </si>
@@ -2346,6 +2346,27 @@
   </si>
   <si>
     <t>88580020037</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/balvu-pag/akimk.html</t>
+  </si>
+  <si>
+    <t>38460040026</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/dobele-and-reg/dobeles-pag/lfnll.html</t>
+  </si>
+  <si>
+    <t>46600010112</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/aronas-pag/cghlhb.html</t>
+  </si>
+  <si>
+    <t>80 000 €</t>
+  </si>
+  <si>
+    <t>137000 m²</t>
   </si>
 </sst>
 </file>
@@ -2758,7 +2779,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F272"/>
+  <dimension ref="A1:F280"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8213,6 +8234,166 @@
       </c>
       <c r="F272" s="2">
         <v>45982.368055555555</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="B273" s="4" t="s">
+        <v>698</v>
+      </c>
+      <c r="C273" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D273" s="4" t="s">
+        <v>699</v>
+      </c>
+      <c r="E273" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="F273" s="2">
+        <v>45984.62013888889</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="B274" s="4" t="s">
+        <v>760</v>
+      </c>
+      <c r="C274" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D274" s="4" t="s">
+        <v>761</v>
+      </c>
+      <c r="E274" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="F274" s="2">
+        <v>45982.84305555555</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A275" s="3" t="s">
+        <v>762</v>
+      </c>
+      <c r="B275" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C275" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D275" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E275" s="4" t="s">
+        <v>763</v>
+      </c>
+      <c r="F275" s="2">
+        <v>45982.70277777778</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A276" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="B276" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C276" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D276" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E276" s="4" t="s">
+        <v>765</v>
+      </c>
+      <c r="F276" s="2">
+        <v>45984.84722222222</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A277" s="3" t="s">
+        <v>766</v>
+      </c>
+      <c r="B277" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C277" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D277" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E277" s="4" t="s">
+        <v>767</v>
+      </c>
+      <c r="F277" s="2">
+        <v>45983.822222222225</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A278" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="B278" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C278" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D278" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E278" s="4" t="s">
+        <v>769</v>
+      </c>
+      <c r="F278" s="2">
+        <v>45985.59583333333</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279" s="3" t="s">
+        <v>770</v>
+      </c>
+      <c r="B279" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C279" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D279" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E279" s="4" t="s">
+        <v>771</v>
+      </c>
+      <c r="F279" s="2">
+        <v>45983.424305555556</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A280" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="B280" s="4" t="s">
+        <v>773</v>
+      </c>
+      <c r="C280" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D280" s="4" t="s">
+        <v>774</v>
+      </c>
+      <c r="E280" s="4" t="s">
+        <v>775</v>
+      </c>
+      <c r="F280" s="2">
+        <v>45983.527083333334</v>
       </c>
     </row>
   </sheetData>
@@ -8488,6 +8669,14 @@
     <hyperlink ref="A270" r:id="rId269"/>
     <hyperlink ref="A271" r:id="rId270"/>
     <hyperlink ref="A272" r:id="rId271"/>
+    <hyperlink ref="A273" r:id="rId272"/>
+    <hyperlink ref="A274" r:id="rId273"/>
+    <hyperlink ref="A275" r:id="rId274"/>
+    <hyperlink ref="A276" r:id="rId275"/>
+    <hyperlink ref="A277" r:id="rId276"/>
+    <hyperlink ref="A278" r:id="rId277"/>
+    <hyperlink ref="A279" r:id="rId278"/>
+    <hyperlink ref="A280" r:id="rId279"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -8499,7 +8688,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8538,162 +8727,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>758</v>
+        <v>776</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>698</v>
+        <v>131</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>435</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>699</v>
+        <v>272</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>700</v>
+        <v>777</v>
       </c>
       <c r="F2" s="2">
-        <v>45984.62013888889</v>
+        <v>45985.790972222225</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>759</v>
+        <v>778</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>760</v>
+        <v>204</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>28</v>
+        <v>117</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>761</v>
+        <v>59</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>703</v>
+        <v>779</v>
       </c>
       <c r="F3" s="2">
-        <v>45982.84305555555</v>
+        <v>45985.72777777778</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>762</v>
+        <v>780</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>290</v>
+        <v>781</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>28</v>
+        <v>256</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>59</v>
+        <v>782</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>763</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2">
-        <v>45982.70277777778</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>764</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>765</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45984.84722222222</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>766</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>767</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45983.822222222225</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>768</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>769</v>
-      </c>
-      <c r="F7" s="2">
-        <v>45985.59583333333</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>770</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>771</v>
-      </c>
-      <c r="F8" s="2">
-        <v>45983.424305555556</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>772</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>773</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>774</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>775</v>
-      </c>
-      <c r="F9" s="2">
-        <v>45983.527083333334</v>
+        <v>45985.65902777778</v>
       </c>
     </row>
   </sheetData>
@@ -8701,11 +8790,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-11-26 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="789">
   <si>
     <t>link</t>
   </si>
@@ -2367,6 +2367,24 @@
   </si>
   <si>
     <t>137000 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/susaju-pag/cixen.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/bauska-and-reg/davinu-pag/emmkl.html</t>
+  </si>
+  <si>
+    <t>40560070003</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/pusas-pag/okndh.html</t>
+  </si>
+  <si>
+    <t>4 400 €</t>
+  </si>
+  <si>
+    <t>78800040225</t>
   </si>
 </sst>
 </file>
@@ -2779,7 +2797,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F280"/>
+  <dimension ref="A1:F283"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8394,6 +8412,66 @@
       </c>
       <c r="F280" s="2">
         <v>45983.527083333334</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A281" s="3" t="s">
+        <v>776</v>
+      </c>
+      <c r="B281" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C281" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D281" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E281" s="4" t="s">
+        <v>777</v>
+      </c>
+      <c r="F281" s="2">
+        <v>45985.790972222225</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A282" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="B282" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C282" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D282" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E282" s="4" t="s">
+        <v>779</v>
+      </c>
+      <c r="F282" s="2">
+        <v>45985.72777777778</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A283" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="B283" s="4" t="s">
+        <v>781</v>
+      </c>
+      <c r="C283" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D283" s="4" t="s">
+        <v>782</v>
+      </c>
+      <c r="E283" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F283" s="2">
+        <v>45985.65902777778</v>
       </c>
     </row>
   </sheetData>
@@ -8677,6 +8755,9 @@
     <hyperlink ref="A278" r:id="rId277"/>
     <hyperlink ref="A279" r:id="rId278"/>
     <hyperlink ref="A280" r:id="rId279"/>
+    <hyperlink ref="A281" r:id="rId280"/>
+    <hyperlink ref="A282" r:id="rId281"/>
+    <hyperlink ref="A283" r:id="rId282"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -8727,10 +8808,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>776</v>
+        <v>783</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>131</v>
+        <v>576</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>28</v>
@@ -8739,50 +8820,50 @@
         <v>272</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>777</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>45985.790972222225</v>
+        <v>45986.88055555556</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>204</v>
+        <v>549</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>117</v>
+        <v>48</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>779</v>
+        <v>785</v>
       </c>
       <c r="F3" s="2">
-        <v>45985.72777777778</v>
+        <v>45987.43611111111</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>780</v>
+        <v>786</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>781</v>
+        <v>787</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>256</v>
+        <v>294</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>782</v>
+        <v>272</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>25</v>
+        <v>788</v>
       </c>
       <c r="F4" s="2">
-        <v>45985.65902777778</v>
+        <v>45986.683333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update forest data - 2025-11-27 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="795">
   <si>
     <t>link</t>
   </si>
@@ -2385,6 +2385,24 @@
   </si>
   <si>
     <t>78800040225</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/bauska-and-reg/vecsaules-pag/joxkg.html</t>
+  </si>
+  <si>
+    <t>40920020560</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/sausnejas-pag/jecom.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ogre-and-reg/taurupes-pag/jobib.html</t>
+  </si>
+  <si>
+    <t>14 000 €</t>
+  </si>
+  <si>
+    <t>74920100064</t>
   </si>
 </sst>
 </file>
@@ -2797,7 +2815,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F283"/>
+  <dimension ref="A1:F286"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8472,6 +8490,66 @@
       </c>
       <c r="F283" s="2">
         <v>45985.65902777778</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A284" s="3" t="s">
+        <v>783</v>
+      </c>
+      <c r="B284" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C284" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D284" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E284" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F284" s="2">
+        <v>45986.88055555556</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A285" s="3" t="s">
+        <v>784</v>
+      </c>
+      <c r="B285" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="C285" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D285" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E285" s="4" t="s">
+        <v>785</v>
+      </c>
+      <c r="F285" s="2">
+        <v>45987.43611111111</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A286" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="B286" s="4" t="s">
+        <v>787</v>
+      </c>
+      <c r="C286" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D286" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E286" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="F286" s="2">
+        <v>45986.683333333334</v>
       </c>
     </row>
   </sheetData>
@@ -8758,6 +8836,9 @@
     <hyperlink ref="A281" r:id="rId280"/>
     <hyperlink ref="A282" r:id="rId281"/>
     <hyperlink ref="A283" r:id="rId282"/>
+    <hyperlink ref="A284" r:id="rId283"/>
+    <hyperlink ref="A285" r:id="rId284"/>
+    <hyperlink ref="A286" r:id="rId285"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -8808,62 +8889,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>783</v>
+        <v>789</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>576</v>
+        <v>246</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>272</v>
+        <v>36</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>790</v>
       </c>
       <c r="F2" s="2">
-        <v>45986.88055555556</v>
+        <v>45988.425</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>784</v>
+        <v>791</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>549</v>
+        <v>174</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>48</v>
+        <v>256</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>162</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>785</v>
+        <v>438</v>
       </c>
       <c r="F3" s="2">
-        <v>45987.43611111111</v>
+        <v>45988.402083333334</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>786</v>
+        <v>792</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>787</v>
+        <v>793</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>272</v>
+        <v>59</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>788</v>
+        <v>794</v>
       </c>
       <c r="F4" s="2">
-        <v>45986.683333333334</v>
+        <v>45988.42708333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update forest data - 2025-11-28 12:27
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="813">
   <si>
     <t>link</t>
   </si>
@@ -2403,6 +2403,60 @@
   </si>
   <si>
     <t>74920100064</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/aluksne/alffx.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/malupes-pag/mkgjf.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/ziemera-pag/bdildi.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/pededzes-pag/bdildc.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/malupes-pag/bliehm.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/liepnas-pag/bbllhm.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/kalncempju-pag/bbokep.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/jaunaluksnes-pag/cghmmh.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/ilzenes-pag/bdxkxn.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/gaujienas-pag/bljonf.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/annas-pag/bhgjcl.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/alsviku-pag/bbllgg.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/ape/blkgik.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/aluksne/iiefg.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/ape/mjikj.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/bauska-and-reg/vecsaules-pag/cghmim.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/indras-pag/mhmhi.html</t>
+  </si>
+  <si>
+    <t>60620041116</t>
   </si>
 </sst>
 </file>
@@ -2815,7 +2869,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F286"/>
+  <dimension ref="A1:F289"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8550,6 +8604,66 @@
       </c>
       <c r="F286" s="2">
         <v>45986.683333333334</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A287" s="3" t="s">
+        <v>789</v>
+      </c>
+      <c r="B287" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C287" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D287" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E287" s="4" t="s">
+        <v>790</v>
+      </c>
+      <c r="F287" s="2">
+        <v>45988.425</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A288" s="3" t="s">
+        <v>791</v>
+      </c>
+      <c r="B288" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C288" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D288" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E288" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="F288" s="2">
+        <v>45988.402083333334</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A289" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="B289" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="C289" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D289" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E289" s="4" t="s">
+        <v>794</v>
+      </c>
+      <c r="F289" s="2">
+        <v>45988.42708333333</v>
       </c>
     </row>
   </sheetData>
@@ -8839,6 +8953,9 @@
     <hyperlink ref="A284" r:id="rId283"/>
     <hyperlink ref="A285" r:id="rId284"/>
     <hyperlink ref="A286" r:id="rId285"/>
+    <hyperlink ref="A287" r:id="rId286"/>
+    <hyperlink ref="A288" r:id="rId287"/>
+    <hyperlink ref="A289" r:id="rId288"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -8850,7 +8967,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8889,62 +9006,342 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>789</v>
+        <v>795</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>246</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>48</v>
+        <v>435</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>790</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>45988.425</v>
+        <v>45989.4375</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>791</v>
+        <v>796</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>174</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>256</v>
+        <v>435</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>162</v>
+        <v>25</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>438</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2">
-        <v>45988.402083333334</v>
+        <v>45989.39027777778</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>792</v>
+        <v>797</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>793</v>
+        <v>25</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>275</v>
+        <v>435</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>794</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2">
-        <v>45988.42708333333</v>
+        <v>45989.245833333334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45989.24513888889</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>799</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45989.24444444444</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="2">
+        <v>45989.24375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2">
+        <v>45989.243055555555</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="2">
+        <v>45989.242361111115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="2">
+        <v>45989.242361111115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>804</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="2">
+        <v>45989.24166666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="2">
+        <v>45989.24097222222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>806</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="2">
+        <v>45989.240277777775</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="2">
+        <v>45989.23958333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="2">
+        <v>45989.23888888889</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="2">
+        <v>45988.802777777775</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>810</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="2">
+        <v>45988.61944444444</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>812</v>
+      </c>
+      <c r="F18" s="2">
+        <v>45988.74861111111</v>
       </c>
     </row>
   </sheetData>
@@ -8952,6 +9349,20 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A13" r:id="rId12"/>
+    <hyperlink ref="A14" r:id="rId13"/>
+    <hyperlink ref="A15" r:id="rId14"/>
+    <hyperlink ref="A16" r:id="rId15"/>
+    <hyperlink ref="A17" r:id="rId16"/>
+    <hyperlink ref="A18" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-12-01 12:21
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="829">
   <si>
     <t>link</t>
   </si>
@@ -2457,6 +2457,54 @@
   </si>
   <si>
     <t>60620041116</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/aluksne/gnedm.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/pildas-pag/bbexhf.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ogre-and-reg/taurupes-pag/cfmhh.html</t>
+  </si>
+  <si>
+    <t>42 000 €</t>
+  </si>
+  <si>
+    <t>8.64 ha.</t>
+  </si>
+  <si>
+    <t>74920090122</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/griskanu-pag/cghxgj.html</t>
+  </si>
+  <si>
+    <t>78560040407</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/kaunatas-pag/bgnoig.html</t>
+  </si>
+  <si>
+    <t>7 800 €</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/saldus-and-reg/saldus-pag/lklod.html</t>
+  </si>
+  <si>
+    <t>84800040015</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/saldus-and-reg/saldus/jchdj.html</t>
+  </si>
+  <si>
+    <t>276 000 €</t>
+  </si>
+  <si>
+    <t>74 ha.</t>
+  </si>
+  <si>
+    <t>84620050240</t>
   </si>
 </sst>
 </file>
@@ -2869,7 +2917,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F289"/>
+  <dimension ref="A1:F306"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8664,6 +8712,346 @@
       </c>
       <c r="F289" s="2">
         <v>45988.42708333333</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A290" s="3" t="s">
+        <v>795</v>
+      </c>
+      <c r="B290" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C290" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D290" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E290" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F290" s="2">
+        <v>45989.4375</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A291" s="3" t="s">
+        <v>796</v>
+      </c>
+      <c r="B291" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C291" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D291" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E291" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F291" s="2">
+        <v>45989.39027777778</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A292" s="3" t="s">
+        <v>797</v>
+      </c>
+      <c r="B292" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C292" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D292" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E292" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F292" s="2">
+        <v>45989.245833333334</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A293" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="B293" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C293" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D293" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E293" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F293" s="2">
+        <v>45989.24513888889</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A294" s="3" t="s">
+        <v>799</v>
+      </c>
+      <c r="B294" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C294" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D294" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E294" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F294" s="2">
+        <v>45989.24444444444</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A295" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="B295" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C295" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D295" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E295" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F295" s="2">
+        <v>45989.24375</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A296" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="B296" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C296" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D296" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E296" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F296" s="2">
+        <v>45989.243055555555</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A297" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="B297" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C297" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D297" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E297" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F297" s="2">
+        <v>45989.242361111115</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A298" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="B298" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C298" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D298" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E298" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F298" s="2">
+        <v>45989.242361111115</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299" s="3" t="s">
+        <v>804</v>
+      </c>
+      <c r="B299" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C299" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D299" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E299" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F299" s="2">
+        <v>45989.24166666667</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A300" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="B300" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C300" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D300" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E300" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F300" s="2">
+        <v>45989.24097222222</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A301" s="3" t="s">
+        <v>806</v>
+      </c>
+      <c r="B301" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C301" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D301" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E301" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F301" s="2">
+        <v>45989.240277777775</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A302" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="B302" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C302" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D302" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E302" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F302" s="2">
+        <v>45989.23958333333</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A303" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="B303" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C303" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D303" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E303" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F303" s="2">
+        <v>45989.23888888889</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A304" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="B304" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C304" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D304" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E304" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F304" s="2">
+        <v>45988.802777777775</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A305" s="3" t="s">
+        <v>810</v>
+      </c>
+      <c r="B305" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C305" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D305" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E305" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F305" s="2">
+        <v>45988.61944444444</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A306" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="B306" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C306" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D306" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E306" s="4" t="s">
+        <v>812</v>
+      </c>
+      <c r="F306" s="2">
+        <v>45988.74861111111</v>
       </c>
     </row>
   </sheetData>
@@ -8956,6 +9344,23 @@
     <hyperlink ref="A287" r:id="rId286"/>
     <hyperlink ref="A288" r:id="rId287"/>
     <hyperlink ref="A289" r:id="rId288"/>
+    <hyperlink ref="A290" r:id="rId289"/>
+    <hyperlink ref="A291" r:id="rId290"/>
+    <hyperlink ref="A292" r:id="rId291"/>
+    <hyperlink ref="A293" r:id="rId292"/>
+    <hyperlink ref="A294" r:id="rId293"/>
+    <hyperlink ref="A295" r:id="rId294"/>
+    <hyperlink ref="A296" r:id="rId295"/>
+    <hyperlink ref="A297" r:id="rId296"/>
+    <hyperlink ref="A298" r:id="rId297"/>
+    <hyperlink ref="A299" r:id="rId298"/>
+    <hyperlink ref="A300" r:id="rId299"/>
+    <hyperlink ref="A301" r:id="rId300"/>
+    <hyperlink ref="A302" r:id="rId301"/>
+    <hyperlink ref="A303" r:id="rId302"/>
+    <hyperlink ref="A304" r:id="rId303"/>
+    <hyperlink ref="A305" r:id="rId304"/>
+    <hyperlink ref="A306" r:id="rId305"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -8967,7 +9372,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9006,7 +9411,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>795</v>
+        <v>813</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>25</v>
@@ -9021,327 +9426,127 @@
         <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>45989.4375</v>
+        <v>45992.4625</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>796</v>
+        <v>814</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>25</v>
+        <v>116</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>435</v>
+        <v>234</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2">
-        <v>45989.39027777778</v>
+        <v>45991.69583333333</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>797</v>
+        <v>815</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>25</v>
+        <v>816</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>435</v>
+        <v>275</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>25</v>
+        <v>817</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>25</v>
+        <v>818</v>
       </c>
       <c r="F4" s="2">
-        <v>45989.245833333334</v>
+        <v>45990.54375</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>798</v>
+        <v>819</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>25</v>
+        <v>268</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>435</v>
+        <v>294</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>25</v>
+        <v>820</v>
       </c>
       <c r="F5" s="2">
-        <v>45989.24513888889</v>
+        <v>45992.32777777778</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>799</v>
+        <v>821</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>25</v>
+        <v>822</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>435</v>
+        <v>294</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>25</v>
+        <v>186</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>25</v>
+        <v>342</v>
       </c>
       <c r="F6" s="2">
-        <v>45989.24444444444</v>
+        <v>45991.57291666667</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>800</v>
+        <v>823</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>25</v>
+        <v>174</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>435</v>
+        <v>346</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>25</v>
+        <v>824</v>
       </c>
       <c r="F7" s="2">
-        <v>45989.24375</v>
+        <v>45990.74166666667</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>801</v>
+        <v>825</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>25</v>
+        <v>826</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>435</v>
+        <v>346</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>25</v>
+        <v>827</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>25</v>
+        <v>828</v>
       </c>
       <c r="F8" s="2">
-        <v>45989.243055555555</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>802</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="2">
-        <v>45989.242361111115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>803</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="2">
-        <v>45989.242361111115</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>804</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="2">
-        <v>45989.24166666667</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>805</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="2">
-        <v>45989.24097222222</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>806</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="2">
-        <v>45989.240277777775</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>807</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="2">
-        <v>45989.23958333333</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>808</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="2">
-        <v>45989.23888888889</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>809</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="2">
-        <v>45988.802777777775</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>810</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="2">
-        <v>45988.61944444444</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>811</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>812</v>
-      </c>
-      <c r="F18" s="2">
-        <v>45988.74861111111</v>
+        <v>45989.75625</v>
       </c>
     </row>
   </sheetData>
@@ -9353,16 +9558,6 @@
     <hyperlink ref="A6" r:id="rId5"/>
     <hyperlink ref="A7" r:id="rId6"/>
     <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
-    <hyperlink ref="A12" r:id="rId11"/>
-    <hyperlink ref="A13" r:id="rId12"/>
-    <hyperlink ref="A14" r:id="rId13"/>
-    <hyperlink ref="A15" r:id="rId14"/>
-    <hyperlink ref="A16" r:id="rId15"/>
-    <hyperlink ref="A17" r:id="rId16"/>
-    <hyperlink ref="A18" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-12-02 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="829">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1587" uniqueCount="838">
   <si>
     <t>link</t>
   </si>
@@ -2505,6 +2505,33 @@
   </si>
   <si>
     <t>84620050240</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/aluksne/gxkjp.html</t>
+  </si>
+  <si>
+    <t>74 €</t>
+  </si>
+  <si>
+    <t>36960010013</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ventspils-and-reg/zleku-pag/booep.html</t>
+  </si>
+  <si>
+    <t>0.61 ha.</t>
+  </si>
+  <si>
+    <t>98940030050</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ventspils-and-reg/zleku-pag/bbkhx.html</t>
+  </si>
+  <si>
+    <t>3.98 ha.</t>
+  </si>
+  <si>
+    <t>98940030021</t>
   </si>
 </sst>
 </file>
@@ -2917,7 +2944,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F306"/>
+  <dimension ref="A1:F313"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9052,6 +9079,146 @@
       </c>
       <c r="F306" s="2">
         <v>45988.74861111111</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A307" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="B307" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C307" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D307" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E307" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F307" s="2">
+        <v>45992.4625</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A308" s="3" t="s">
+        <v>814</v>
+      </c>
+      <c r="B308" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C308" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D308" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E308" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F308" s="2">
+        <v>45991.69583333333</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A309" s="3" t="s">
+        <v>815</v>
+      </c>
+      <c r="B309" s="4" t="s">
+        <v>816</v>
+      </c>
+      <c r="C309" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D309" s="4" t="s">
+        <v>817</v>
+      </c>
+      <c r="E309" s="4" t="s">
+        <v>818</v>
+      </c>
+      <c r="F309" s="2">
+        <v>45990.54375</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A310" s="3" t="s">
+        <v>819</v>
+      </c>
+      <c r="B310" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C310" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D310" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E310" s="4" t="s">
+        <v>820</v>
+      </c>
+      <c r="F310" s="2">
+        <v>45992.32777777778</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A311" s="3" t="s">
+        <v>821</v>
+      </c>
+      <c r="B311" s="4" t="s">
+        <v>822</v>
+      </c>
+      <c r="C311" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D311" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E311" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="F311" s="2">
+        <v>45991.57291666667</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A312" s="3" t="s">
+        <v>823</v>
+      </c>
+      <c r="B312" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C312" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D312" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E312" s="4" t="s">
+        <v>824</v>
+      </c>
+      <c r="F312" s="2">
+        <v>45990.74166666667</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A313" s="3" t="s">
+        <v>825</v>
+      </c>
+      <c r="B313" s="4" t="s">
+        <v>826</v>
+      </c>
+      <c r="C313" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D313" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="E313" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="F313" s="2">
+        <v>45989.75625</v>
       </c>
     </row>
   </sheetData>
@@ -9361,6 +9528,13 @@
     <hyperlink ref="A304" r:id="rId303"/>
     <hyperlink ref="A305" r:id="rId304"/>
     <hyperlink ref="A306" r:id="rId305"/>
+    <hyperlink ref="A307" r:id="rId306"/>
+    <hyperlink ref="A308" r:id="rId307"/>
+    <hyperlink ref="A309" r:id="rId308"/>
+    <hyperlink ref="A310" r:id="rId309"/>
+    <hyperlink ref="A311" r:id="rId310"/>
+    <hyperlink ref="A312" r:id="rId311"/>
+    <hyperlink ref="A313" r:id="rId312"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -9372,7 +9546,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9411,142 +9585,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>813</v>
+        <v>829</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>830</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>435</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>831</v>
       </c>
       <c r="F2" s="2">
-        <v>45992.4625</v>
+        <v>45993.575694444444</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>814</v>
+        <v>832</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>116</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>234</v>
+        <v>404</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>36</v>
+        <v>833</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>25</v>
+        <v>834</v>
       </c>
       <c r="F3" s="2">
-        <v>45991.69583333333</v>
+        <v>45993.55416666667</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>815</v>
+        <v>835</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>816</v>
+        <v>116</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>275</v>
+        <v>404</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>817</v>
+        <v>836</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>818</v>
+        <v>837</v>
       </c>
       <c r="F4" s="2">
-        <v>45990.54375</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>819</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>820</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45992.32777777778</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>821</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>822</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45991.57291666667</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>823</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>824</v>
-      </c>
-      <c r="F7" s="2">
-        <v>45990.74166666667</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>825</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>826</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>827</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>828</v>
-      </c>
-      <c r="F8" s="2">
-        <v>45989.75625</v>
+        <v>45993.55416666667</v>
       </c>
     </row>
   </sheetData>
@@ -9554,10 +9648,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-12-03 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1587" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="850">
   <si>
     <t>link</t>
   </si>
@@ -2532,6 +2532,42 @@
   </si>
   <si>
     <t>98940030021</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jelgava-and-reg/valgundes-nov/cghpfg.html</t>
+  </si>
+  <si>
+    <t>54860020101</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jelgava-and-reg/livberzes-pag/ohbhg.html</t>
+  </si>
+  <si>
+    <t>54620090154</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jelgava-and-reg/valgundes-nov/egcjx.html</t>
+  </si>
+  <si>
+    <t>4 000 €</t>
+  </si>
+  <si>
+    <t>548600701105</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jelgava-and-reg/valgundes-nov/ecmgi.html</t>
+  </si>
+  <si>
+    <t>54860060066</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kuldiga-and-reg/varmes-pag/dpmoh.html</t>
+  </si>
+  <si>
+    <t>149 000 €</t>
+  </si>
+  <si>
+    <t>38 ha.</t>
   </si>
 </sst>
 </file>
@@ -2944,7 +2980,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F313"/>
+  <dimension ref="A1:F316"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9219,6 +9255,66 @@
       </c>
       <c r="F313" s="2">
         <v>45989.75625</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A314" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="B314" s="4" t="s">
+        <v>830</v>
+      </c>
+      <c r="C314" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D314" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E314" s="4" t="s">
+        <v>831</v>
+      </c>
+      <c r="F314" s="2">
+        <v>45993.575694444444</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A315" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="B315" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C315" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="D315" s="4" t="s">
+        <v>833</v>
+      </c>
+      <c r="E315" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="F315" s="2">
+        <v>45993.55416666667</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A316" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="B316" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C316" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="D316" s="4" t="s">
+        <v>836</v>
+      </c>
+      <c r="E316" s="4" t="s">
+        <v>837</v>
+      </c>
+      <c r="F316" s="2">
+        <v>45993.55416666667</v>
       </c>
     </row>
   </sheetData>
@@ -9535,6 +9631,9 @@
     <hyperlink ref="A311" r:id="rId310"/>
     <hyperlink ref="A312" r:id="rId311"/>
     <hyperlink ref="A313" r:id="rId312"/>
+    <hyperlink ref="A314" r:id="rId313"/>
+    <hyperlink ref="A315" r:id="rId314"/>
+    <hyperlink ref="A316" r:id="rId315"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -9546,7 +9645,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9585,62 +9684,102 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>829</v>
+        <v>838</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>830</v>
+        <v>246</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>435</v>
+        <v>518</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>82</v>
+        <v>186</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>831</v>
+        <v>839</v>
       </c>
       <c r="F2" s="2">
-        <v>45993.575694444444</v>
+        <v>45994.59513888889</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>832</v>
+        <v>840</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>116</v>
+        <v>536</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>404</v>
+        <v>518</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>833</v>
+        <v>272</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>834</v>
+        <v>841</v>
       </c>
       <c r="F3" s="2">
-        <v>45993.55416666667</v>
+        <v>45994.58333333333</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>835</v>
+        <v>842</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>116</v>
+        <v>843</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>404</v>
+        <v>518</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>836</v>
+        <v>272</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>837</v>
+        <v>844</v>
       </c>
       <c r="F4" s="2">
-        <v>45993.55416666667</v>
+        <v>45994.57708333334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>846</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45994.57152777778</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>847</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>848</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>849</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45993.70833333333</v>
       </c>
     </row>
   </sheetData>
@@ -9648,6 +9787,8 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-12-04 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -2980,7 +2980,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F316"/>
+  <dimension ref="A1:F321"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9315,6 +9315,106 @@
       </c>
       <c r="F316" s="2">
         <v>45993.55416666667</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A317" s="3" t="s">
+        <v>838</v>
+      </c>
+      <c r="B317" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C317" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="D317" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E317" s="4" t="s">
+        <v>839</v>
+      </c>
+      <c r="F317" s="2">
+        <v>45994.59513888889</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A318" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="B318" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="C318" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="D318" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E318" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="F318" s="2">
+        <v>45994.58333333333</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A319" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="B319" s="4" t="s">
+        <v>843</v>
+      </c>
+      <c r="C319" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="D319" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E319" s="4" t="s">
+        <v>844</v>
+      </c>
+      <c r="F319" s="2">
+        <v>45994.57708333334</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A320" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="B320" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C320" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="D320" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E320" s="4" t="s">
+        <v>846</v>
+      </c>
+      <c r="F320" s="2">
+        <v>45994.57152777778</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A321" s="3" t="s">
+        <v>847</v>
+      </c>
+      <c r="B321" s="4" t="s">
+        <v>848</v>
+      </c>
+      <c r="C321" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D321" s="4" t="s">
+        <v>849</v>
+      </c>
+      <c r="E321" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F321" s="2">
+        <v>45993.70833333333</v>
       </c>
     </row>
   </sheetData>
@@ -9634,6 +9734,11 @@
     <hyperlink ref="A314" r:id="rId313"/>
     <hyperlink ref="A315" r:id="rId314"/>
     <hyperlink ref="A316" r:id="rId315"/>
+    <hyperlink ref="A317" r:id="rId316"/>
+    <hyperlink ref="A318" r:id="rId317"/>
+    <hyperlink ref="A319" r:id="rId318"/>
+    <hyperlink ref="A320" r:id="rId319"/>
+    <hyperlink ref="A321" r:id="rId320"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -9645,7 +9750,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9682,114 +9787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>838</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>518</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>839</v>
-      </c>
-      <c r="F2" s="2">
-        <v>45994.59513888889</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>840</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>536</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>518</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>841</v>
-      </c>
-      <c r="F3" s="2">
-        <v>45994.58333333333</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>842</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>843</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>518</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>844</v>
-      </c>
-      <c r="F4" s="2">
-        <v>45994.57708333334</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>518</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>846</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45994.57152777778</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>847</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>848</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>424</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>849</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45993.70833333333</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2025-12-05 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="853">
   <si>
     <t>link</t>
   </si>
@@ -2568,6 +2568,15 @@
   </si>
   <si>
     <t>38 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/ledurgas-pag/obmbf.html</t>
+  </si>
+  <si>
+    <t>76 000 €</t>
+  </si>
+  <si>
+    <t>66560010200</t>
   </si>
 </sst>
 </file>
@@ -9750,7 +9759,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9787,7 +9796,30 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>851</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>852</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45995.77083333333</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2025-12-08 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="873">
   <si>
     <t>link</t>
   </si>
@@ -2577,6 +2577,66 @@
   </si>
   <si>
     <t>66560010200</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/vecumu-pag/cogdb.html</t>
+  </si>
+  <si>
+    <t>58 000 €</t>
+  </si>
+  <si>
+    <t>19.47 ha.</t>
+  </si>
+  <si>
+    <t>38920050109</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/vecumu-pag/amgxp.html</t>
+  </si>
+  <si>
+    <t>43 000 €</t>
+  </si>
+  <si>
+    <t>14.46 ha.</t>
+  </si>
+  <si>
+    <t>38920050232</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/bauska-and-reg/iecavas-nov/ijmhp.html</t>
+  </si>
+  <si>
+    <t>32 100 €</t>
+  </si>
+  <si>
+    <t>40640130163</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jekabpils-and-reg/aknistes-l-t/hfxcb.html</t>
+  </si>
+  <si>
+    <t>16.63 ha.</t>
+  </si>
+  <si>
+    <t>56250070275</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/brigu-pag/kniic.html</t>
+  </si>
+  <si>
+    <t>10.21 ha.</t>
+  </si>
+  <si>
+    <t>68460030011</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/merdzenes-pag/hmobk.html</t>
+  </si>
+  <si>
+    <t>5.60 ha.</t>
+  </si>
+  <si>
+    <t>68720020331</t>
   </si>
 </sst>
 </file>
@@ -2989,7 +3049,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F321"/>
+  <dimension ref="A1:F322"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9424,6 +9484,26 @@
       </c>
       <c r="F321" s="2">
         <v>45993.70833333333</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A322" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="B322" s="4" t="s">
+        <v>851</v>
+      </c>
+      <c r="C322" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D322" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="E322" s="4" t="s">
+        <v>852</v>
+      </c>
+      <c r="F322" s="2">
+        <v>45995.77083333333</v>
       </c>
     </row>
   </sheetData>
@@ -9748,6 +9828,7 @@
     <hyperlink ref="A319" r:id="rId318"/>
     <hyperlink ref="A320" r:id="rId319"/>
     <hyperlink ref="A321" r:id="rId320"/>
+    <hyperlink ref="A322" r:id="rId321"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -9759,7 +9840,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9798,27 +9879,132 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>850</v>
+        <v>853</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>851</v>
+        <v>854</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>208</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>619</v>
+        <v>855</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>852</v>
+        <v>856</v>
       </c>
       <c r="F2" s="2">
-        <v>45995.77083333333</v>
+        <v>45999.48402777778</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>857</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>858</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>859</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45999.45486111111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>861</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>862</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>863</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45998.55972222222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>864</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>865</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>866</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45999.459027777775</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>867</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>868</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>869</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45999.48888888889</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>871</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>872</v>
+      </c>
+      <c r="F7" s="2">
+        <v>45999.46319444444</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-12-09 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="878">
   <si>
     <t>link</t>
   </si>
@@ -2637,6 +2637,21 @@
   </si>
   <si>
     <t>68720020331</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/raunas-pag/kcjhx.html</t>
+  </si>
+  <si>
+    <t>42760020065</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/makonkalna-pag/gohej.html</t>
+  </si>
+  <si>
+    <t>190 000 €</t>
+  </si>
+  <si>
+    <t>78720020066</t>
   </si>
 </sst>
 </file>
@@ -3049,7 +3064,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F322"/>
+  <dimension ref="A1:F328"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9504,6 +9519,126 @@
       </c>
       <c r="F322" s="2">
         <v>45995.77083333333</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A323" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="B323" s="4" t="s">
+        <v>854</v>
+      </c>
+      <c r="C323" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D323" s="4" t="s">
+        <v>855</v>
+      </c>
+      <c r="E323" s="4" t="s">
+        <v>856</v>
+      </c>
+      <c r="F323" s="2">
+        <v>45999.48402777778</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A324" s="3" t="s">
+        <v>857</v>
+      </c>
+      <c r="B324" s="4" t="s">
+        <v>858</v>
+      </c>
+      <c r="C324" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D324" s="4" t="s">
+        <v>859</v>
+      </c>
+      <c r="E324" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="F324" s="2">
+        <v>45999.45486111111</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A325" s="3" t="s">
+        <v>861</v>
+      </c>
+      <c r="B325" s="4" t="s">
+        <v>862</v>
+      </c>
+      <c r="C325" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D325" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E325" s="4" t="s">
+        <v>863</v>
+      </c>
+      <c r="F325" s="2">
+        <v>45998.55972222222</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A326" s="3" t="s">
+        <v>864</v>
+      </c>
+      <c r="B326" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C326" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D326" s="4" t="s">
+        <v>865</v>
+      </c>
+      <c r="E326" s="4" t="s">
+        <v>866</v>
+      </c>
+      <c r="F326" s="2">
+        <v>45999.459027777775</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A327" s="3" t="s">
+        <v>867</v>
+      </c>
+      <c r="B327" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C327" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D327" s="4" t="s">
+        <v>868</v>
+      </c>
+      <c r="E327" s="4" t="s">
+        <v>869</v>
+      </c>
+      <c r="F327" s="2">
+        <v>45999.48888888889</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A328" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="B328" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C328" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D328" s="4" t="s">
+        <v>871</v>
+      </c>
+      <c r="E328" s="4" t="s">
+        <v>872</v>
+      </c>
+      <c r="F328" s="2">
+        <v>45999.46319444444</v>
       </c>
     </row>
   </sheetData>
@@ -9829,6 +9964,12 @@
     <hyperlink ref="A320" r:id="rId319"/>
     <hyperlink ref="A321" r:id="rId320"/>
     <hyperlink ref="A322" r:id="rId321"/>
+    <hyperlink ref="A323" r:id="rId322"/>
+    <hyperlink ref="A324" r:id="rId323"/>
+    <hyperlink ref="A325" r:id="rId324"/>
+    <hyperlink ref="A326" r:id="rId325"/>
+    <hyperlink ref="A327" r:id="rId326"/>
+    <hyperlink ref="A328" r:id="rId327"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -9840,7 +9981,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9879,132 +10020,48 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>853</v>
+        <v>873</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>854</v>
+        <v>62</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>855</v>
+        <v>44</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>856</v>
+        <v>874</v>
       </c>
       <c r="F2" s="2">
-        <v>45999.48402777778</v>
+        <v>46000.52291666667</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>857</v>
+        <v>875</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>858</v>
+        <v>876</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>28</v>
+        <v>294</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>859</v>
+        <v>302</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>860</v>
+        <v>877</v>
       </c>
       <c r="F3" s="2">
-        <v>45999.45486111111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>861</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>862</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>863</v>
-      </c>
-      <c r="F4" s="2">
-        <v>45998.55972222222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>864</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>865</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>866</v>
-      </c>
-      <c r="F5" s="2">
-        <v>45999.459027777775</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>867</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>868</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>869</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45999.48888888889</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>870</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>871</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>872</v>
-      </c>
-      <c r="F7" s="2">
-        <v>45999.46319444444</v>
+        <v>45999.61041666666</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-12-10 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="884">
   <si>
     <t>link</t>
   </si>
@@ -2652,6 +2652,24 @@
   </si>
   <si>
     <t>78720020066</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kuldiga-and-reg/turlavas-pag/bbknn.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/ilzeskalna-pag/fiblg.html</t>
+  </si>
+  <si>
+    <t>78580060216</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/ozolmuizas-pag/aghex.html</t>
+  </si>
+  <si>
+    <t>0.53 ha.</t>
+  </si>
+  <si>
+    <t>78780030511</t>
   </si>
 </sst>
 </file>
@@ -3064,7 +3082,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F328"/>
+  <dimension ref="A1:F330"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9639,6 +9657,46 @@
       </c>
       <c r="F328" s="2">
         <v>45999.46319444444</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A329" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="B329" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C329" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D329" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E329" s="4" t="s">
+        <v>874</v>
+      </c>
+      <c r="F329" s="2">
+        <v>46000.52291666667</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A330" s="3" t="s">
+        <v>875</v>
+      </c>
+      <c r="B330" s="4" t="s">
+        <v>876</v>
+      </c>
+      <c r="C330" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D330" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E330" s="4" t="s">
+        <v>877</v>
+      </c>
+      <c r="F330" s="2">
+        <v>45999.61041666666</v>
       </c>
     </row>
   </sheetData>
@@ -9970,6 +10028,8 @@
     <hyperlink ref="A326" r:id="rId325"/>
     <hyperlink ref="A327" r:id="rId326"/>
     <hyperlink ref="A328" r:id="rId327"/>
+    <hyperlink ref="A329" r:id="rId328"/>
+    <hyperlink ref="A330" r:id="rId329"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -9981,7 +10041,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10020,48 +10080,69 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>873</v>
+        <v>878</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>62</v>
+        <v>271</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>63</v>
+        <v>424</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>44</v>
+        <v>272</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>874</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>46000.52291666667</v>
+        <v>46001.45694444445</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>875</v>
+        <v>879</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>876</v>
+        <v>215</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>294</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>302</v>
+        <v>272</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>877</v>
+        <v>880</v>
       </c>
       <c r="F3" s="2">
-        <v>45999.61041666666</v>
+        <v>46001.33333333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>881</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>882</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>883</v>
+      </c>
+      <c r="F4" s="2">
+        <v>46000.617361111115</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-12-11 12:21
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="884">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="886">
   <si>
     <t>link</t>
   </si>
@@ -2670,6 +2670,12 @@
   </si>
   <si>
     <t>78780030511</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/liepaja-and-reg/vainodes-pag/kxikn.html</t>
+  </si>
+  <si>
+    <t>64920050035</t>
   </si>
 </sst>
 </file>
@@ -3082,7 +3088,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F330"/>
+  <dimension ref="A1:F333"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9697,6 +9703,66 @@
       </c>
       <c r="F330" s="2">
         <v>45999.61041666666</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A331" s="3" t="s">
+        <v>878</v>
+      </c>
+      <c r="B331" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C331" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D331" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E331" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F331" s="2">
+        <v>46001.45694444445</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A332" s="3" t="s">
+        <v>879</v>
+      </c>
+      <c r="B332" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C332" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D332" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E332" s="4" t="s">
+        <v>880</v>
+      </c>
+      <c r="F332" s="2">
+        <v>46001.33333333333</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A333" s="3" t="s">
+        <v>881</v>
+      </c>
+      <c r="B333" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C333" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D333" s="4" t="s">
+        <v>882</v>
+      </c>
+      <c r="E333" s="4" t="s">
+        <v>883</v>
+      </c>
+      <c r="F333" s="2">
+        <v>46000.617361111115</v>
       </c>
     </row>
   </sheetData>
@@ -10030,6 +10096,9 @@
     <hyperlink ref="A328" r:id="rId327"/>
     <hyperlink ref="A329" r:id="rId328"/>
     <hyperlink ref="A330" r:id="rId329"/>
+    <hyperlink ref="A331" r:id="rId330"/>
+    <hyperlink ref="A332" r:id="rId331"/>
+    <hyperlink ref="A333" r:id="rId332"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -10041,7 +10110,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10080,69 +10149,27 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>878</v>
+        <v>884</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>424</v>
+        <v>190</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>272</v>
+        <v>44</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>885</v>
       </c>
       <c r="F2" s="2">
-        <v>46001.45694444445</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>879</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>880</v>
-      </c>
-      <c r="F3" s="2">
-        <v>46001.33333333333</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>881</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>576</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>882</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>883</v>
-      </c>
-      <c r="F4" s="2">
-        <v>46000.617361111115</v>
+        <v>46001.70625</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-12-12 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -3088,7 +3088,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F333"/>
+  <dimension ref="A1:F334"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9763,6 +9763,26 @@
       </c>
       <c r="F333" s="2">
         <v>46000.617361111115</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A334" s="3" t="s">
+        <v>884</v>
+      </c>
+      <c r="B334" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C334" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D334" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E334" s="4" t="s">
+        <v>885</v>
+      </c>
+      <c r="F334" s="2">
+        <v>46001.70625</v>
       </c>
     </row>
   </sheetData>
@@ -10099,6 +10119,7 @@
     <hyperlink ref="A331" r:id="rId330"/>
     <hyperlink ref="A332" r:id="rId331"/>
     <hyperlink ref="A333" r:id="rId332"/>
+    <hyperlink ref="A334" r:id="rId333"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -10110,7 +10131,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10147,30 +10168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>884</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>885</v>
-      </c>
-      <c r="F2" s="2">
-        <v>46001.70625</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2025-12-15 12:21
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="899">
   <si>
     <t>link</t>
   </si>
@@ -2676,6 +2676,45 @@
   </si>
   <si>
     <t>64920050035</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/dzerbenes-pag/ihhmh.html</t>
+  </si>
+  <si>
+    <t>50 €</t>
+  </si>
+  <si>
+    <t>10.20 ha.</t>
+  </si>
+  <si>
+    <t>42500040011</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/vecpiebalgas-pag/alikx.html</t>
+  </si>
+  <si>
+    <t>3.51 ha.</t>
+  </si>
+  <si>
+    <t>42540020145</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/gulbene-and-reg/lejasciema-pag/lfkbg.html</t>
+  </si>
+  <si>
+    <t>26 400 €</t>
+  </si>
+  <si>
+    <t>50640020038</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/ciblas-pag/ggibg.html</t>
+  </si>
+  <si>
+    <t>15.70 ha.</t>
+  </si>
+  <si>
+    <t>68480030023</t>
   </si>
 </sst>
 </file>
@@ -10131,7 +10170,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10168,7 +10207,93 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>886</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>887</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>888</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>889</v>
+      </c>
+      <c r="F2" s="2">
+        <v>46006.506944444445</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>890</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>891</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>892</v>
+      </c>
+      <c r="F3" s="2">
+        <v>46005.57708333334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>894</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>895</v>
+      </c>
+      <c r="F4" s="2">
+        <v>46003.92222222222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>897</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>898</v>
+      </c>
+      <c r="F5" s="2">
+        <v>46003.8625</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2025-12-16 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="899">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="901">
   <si>
     <t>link</t>
   </si>
@@ -2715,6 +2715,12 @@
   </si>
   <si>
     <t>68480030023</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/kaunatas-pag/nnplp.html</t>
+  </si>
+  <si>
+    <t>78620020231</t>
   </si>
 </sst>
 </file>
@@ -3127,7 +3133,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F334"/>
+  <dimension ref="A1:F338"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9822,6 +9828,86 @@
       </c>
       <c r="F334" s="2">
         <v>46001.70625</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A335" s="3" t="s">
+        <v>886</v>
+      </c>
+      <c r="B335" s="4" t="s">
+        <v>887</v>
+      </c>
+      <c r="C335" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D335" s="4" t="s">
+        <v>888</v>
+      </c>
+      <c r="E335" s="4" t="s">
+        <v>889</v>
+      </c>
+      <c r="F335" s="2">
+        <v>46006.506944444445</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A336" s="3" t="s">
+        <v>890</v>
+      </c>
+      <c r="B336" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="C336" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D336" s="4" t="s">
+        <v>891</v>
+      </c>
+      <c r="E336" s="4" t="s">
+        <v>892</v>
+      </c>
+      <c r="F336" s="2">
+        <v>46005.57708333334</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A337" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="B337" s="4" t="s">
+        <v>894</v>
+      </c>
+      <c r="C337" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D337" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E337" s="4" t="s">
+        <v>895</v>
+      </c>
+      <c r="F337" s="2">
+        <v>46003.92222222222</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A338" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="B338" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C338" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D338" s="4" t="s">
+        <v>897</v>
+      </c>
+      <c r="E338" s="4" t="s">
+        <v>898</v>
+      </c>
+      <c r="F338" s="2">
+        <v>46003.8625</v>
       </c>
     </row>
   </sheetData>
@@ -10159,6 +10245,10 @@
     <hyperlink ref="A332" r:id="rId331"/>
     <hyperlink ref="A333" r:id="rId332"/>
     <hyperlink ref="A334" r:id="rId333"/>
+    <hyperlink ref="A335" r:id="rId334"/>
+    <hyperlink ref="A336" r:id="rId335"/>
+    <hyperlink ref="A337" r:id="rId336"/>
+    <hyperlink ref="A338" r:id="rId337"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -10170,7 +10260,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10209,90 +10299,27 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>886</v>
+        <v>899</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>887</v>
+        <v>52</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>63</v>
+        <v>294</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>888</v>
+        <v>82</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>889</v>
+        <v>900</v>
       </c>
       <c r="F2" s="2">
-        <v>46006.506944444445</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>890</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>549</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>891</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>892</v>
-      </c>
-      <c r="F3" s="2">
-        <v>46005.57708333334</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>893</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>894</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>895</v>
-      </c>
-      <c r="F4" s="2">
-        <v>46003.92222222222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>896</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>897</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>898</v>
-      </c>
-      <c r="F5" s="2">
-        <v>46003.8625</v>
+        <v>46006.62986111111</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-12-17 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="908">
   <si>
     <t>link</t>
   </si>
@@ -2721,6 +2721,27 @@
   </si>
   <si>
     <t>78620020231</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/skilbenu-pag/bckdgk.html</t>
+  </si>
+  <si>
+    <t>77 500 €</t>
+  </si>
+  <si>
+    <t>15 ha.</t>
+  </si>
+  <si>
+    <t>38820050098</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/praulienas-pag/fikle.html</t>
+  </si>
+  <si>
+    <t>47 000 €</t>
+  </si>
+  <si>
+    <t>70860080106</t>
   </si>
 </sst>
 </file>
@@ -3133,7 +3154,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F338"/>
+  <dimension ref="A1:F339"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9908,6 +9929,26 @@
       </c>
       <c r="F338" s="2">
         <v>46003.8625</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A339" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="B339" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C339" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D339" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E339" s="4" t="s">
+        <v>900</v>
+      </c>
+      <c r="F339" s="2">
+        <v>46006.62986111111</v>
       </c>
     </row>
   </sheetData>
@@ -10249,6 +10290,7 @@
     <hyperlink ref="A336" r:id="rId335"/>
     <hyperlink ref="A337" r:id="rId336"/>
     <hyperlink ref="A338" r:id="rId337"/>
+    <hyperlink ref="A339" r:id="rId338"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -10260,7 +10302,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10299,27 +10341,48 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>52</v>
+        <v>902</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>294</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>82</v>
+        <v>903</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>900</v>
+        <v>904</v>
       </c>
       <c r="F2" s="2">
-        <v>46006.62986111111</v>
+        <v>46008.56041666667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>905</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>906</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>907</v>
+      </c>
+      <c r="F3" s="2">
+        <v>46008.45138888889</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-12-18 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="910">
   <si>
     <t>link</t>
   </si>
@@ -2742,6 +2742,12 @@
   </si>
   <si>
     <t>70860080106</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/pales-pag/hdfxi.html</t>
+  </si>
+  <si>
+    <t>66680020029</t>
   </si>
 </sst>
 </file>
@@ -3154,7 +3160,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F339"/>
+  <dimension ref="A1:F341"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9949,6 +9955,46 @@
       </c>
       <c r="F339" s="2">
         <v>46006.62986111111</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A340" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="B340" s="4" t="s">
+        <v>902</v>
+      </c>
+      <c r="C340" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D340" s="4" t="s">
+        <v>903</v>
+      </c>
+      <c r="E340" s="4" t="s">
+        <v>904</v>
+      </c>
+      <c r="F340" s="2">
+        <v>46008.56041666667</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A341" s="3" t="s">
+        <v>905</v>
+      </c>
+      <c r="B341" s="4" t="s">
+        <v>906</v>
+      </c>
+      <c r="C341" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D341" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E341" s="4" t="s">
+        <v>907</v>
+      </c>
+      <c r="F341" s="2">
+        <v>46008.45138888889</v>
       </c>
     </row>
   </sheetData>
@@ -10291,6 +10337,8 @@
     <hyperlink ref="A337" r:id="rId336"/>
     <hyperlink ref="A338" r:id="rId337"/>
     <hyperlink ref="A339" r:id="rId338"/>
+    <hyperlink ref="A340" r:id="rId339"/>
+    <hyperlink ref="A341" r:id="rId340"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -10302,7 +10350,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10341,48 +10389,27 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>901</v>
+        <v>908</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>902</v>
+        <v>293</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>208</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>903</v>
+        <v>272</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>904</v>
+        <v>909</v>
       </c>
       <c r="F2" s="2">
-        <v>46008.56041666667</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>905</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>906</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>907</v>
-      </c>
-      <c r="F3" s="2">
-        <v>46008.45138888889</v>
+        <v>46009.43958333333</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-12-19 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="913">
   <si>
     <t>link</t>
   </si>
@@ -2748,6 +2748,15 @@
   </si>
   <si>
     <t>66680020029</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/pelecu-pag/liecc.html</t>
+  </si>
+  <si>
+    <t>5.30 ha.</t>
+  </si>
+  <si>
+    <t>76560050122</t>
   </si>
 </sst>
 </file>
@@ -3160,7 +3169,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F341"/>
+  <dimension ref="A1:F342"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9995,6 +10004,26 @@
       </c>
       <c r="F341" s="2">
         <v>46008.45138888889</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A342" s="3" t="s">
+        <v>908</v>
+      </c>
+      <c r="B342" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C342" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D342" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E342" s="4" t="s">
+        <v>909</v>
+      </c>
+      <c r="F342" s="2">
+        <v>46009.43958333333</v>
       </c>
     </row>
   </sheetData>
@@ -10339,6 +10368,7 @@
     <hyperlink ref="A339" r:id="rId338"/>
     <hyperlink ref="A340" r:id="rId339"/>
     <hyperlink ref="A341" r:id="rId340"/>
+    <hyperlink ref="A342" r:id="rId341"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -10389,22 +10419,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>293</v>
+        <v>268</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>208</v>
+        <v>284</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>272</v>
+        <v>911</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>909</v>
+        <v>912</v>
       </c>
       <c r="F2" s="2">
-        <v>46009.43958333333</v>
+        <v>46010.01875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update forest data - 2025-12-22 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="926">
   <si>
     <t>link</t>
   </si>
@@ -2757,6 +2757,45 @@
   </si>
   <si>
     <t>76560050122</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/bauska-and-reg/vecumnieku-pag/lebhx.html</t>
+  </si>
+  <si>
+    <t>9 800 €</t>
+  </si>
+  <si>
+    <t>3.32 ha.</t>
+  </si>
+  <si>
+    <t>40940130127</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/piedrujas-pag/kjohf.html</t>
+  </si>
+  <si>
+    <t>9.50 ha.</t>
+  </si>
+  <si>
+    <t>60840050087, 162</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/tukums-and-reg/smardes-pag/dcegf.html</t>
+  </si>
+  <si>
+    <t>2 200 €</t>
+  </si>
+  <si>
+    <t>0.08 ha.</t>
+  </si>
+  <si>
+    <t>90820050176</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/tukums-and-reg/smardes-pag/kecid.html</t>
+  </si>
+  <si>
+    <t>90820050174</t>
   </si>
 </sst>
 </file>
@@ -3169,7 +3208,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F342"/>
+  <dimension ref="A1:F343"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10024,6 +10063,26 @@
       </c>
       <c r="F342" s="2">
         <v>46009.43958333333</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A343" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="B343" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C343" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D343" s="4" t="s">
+        <v>911</v>
+      </c>
+      <c r="E343" s="4" t="s">
+        <v>912</v>
+      </c>
+      <c r="F343" s="2">
+        <v>46010.01875</v>
       </c>
     </row>
   </sheetData>
@@ -10369,6 +10428,7 @@
     <hyperlink ref="A340" r:id="rId339"/>
     <hyperlink ref="A341" r:id="rId340"/>
     <hyperlink ref="A342" r:id="rId341"/>
+    <hyperlink ref="A343" r:id="rId342"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -10380,7 +10440,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10419,27 +10479,90 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>268</v>
+        <v>914</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>284</v>
+        <v>48</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>911</v>
+        <v>915</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>912</v>
+        <v>916</v>
       </c>
       <c r="F2" s="2">
-        <v>46010.01875</v>
+        <v>46013.58541666667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>917</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>637</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>918</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>919</v>
+      </c>
+      <c r="F3" s="2">
+        <v>46010.92638888889</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>921</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>922</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>923</v>
+      </c>
+      <c r="F4" s="2">
+        <v>46012.92291666666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>924</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>925</v>
+      </c>
+      <c r="F5" s="2">
+        <v>46012.92152777778</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-12-23 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="929">
   <si>
     <t>link</t>
   </si>
@@ -2796,6 +2796,15 @@
   </si>
   <si>
     <t>90820050174</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/pilskalnes-pag/lfcem.html</t>
+  </si>
+  <si>
+    <t>7 500 €</t>
+  </si>
+  <si>
+    <t>17000 m²</t>
   </si>
 </sst>
 </file>
@@ -3208,7 +3217,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F343"/>
+  <dimension ref="A1:F347"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10083,6 +10092,86 @@
       </c>
       <c r="F343" s="2">
         <v>46010.01875</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A344" s="3" t="s">
+        <v>913</v>
+      </c>
+      <c r="B344" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="C344" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D344" s="4" t="s">
+        <v>915</v>
+      </c>
+      <c r="E344" s="4" t="s">
+        <v>916</v>
+      </c>
+      <c r="F344" s="2">
+        <v>46013.58541666667</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A345" s="3" t="s">
+        <v>917</v>
+      </c>
+      <c r="B345" s="4" t="s">
+        <v>637</v>
+      </c>
+      <c r="C345" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D345" s="4" t="s">
+        <v>918</v>
+      </c>
+      <c r="E345" s="4" t="s">
+        <v>919</v>
+      </c>
+      <c r="F345" s="2">
+        <v>46010.92638888889</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A346" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="B346" s="4" t="s">
+        <v>921</v>
+      </c>
+      <c r="C346" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D346" s="4" t="s">
+        <v>922</v>
+      </c>
+      <c r="E346" s="4" t="s">
+        <v>923</v>
+      </c>
+      <c r="F346" s="2">
+        <v>46012.92291666666</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A347" s="3" t="s">
+        <v>924</v>
+      </c>
+      <c r="B347" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C347" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D347" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E347" s="4" t="s">
+        <v>925</v>
+      </c>
+      <c r="F347" s="2">
+        <v>46012.92152777778</v>
       </c>
     </row>
   </sheetData>
@@ -10429,6 +10518,10 @@
     <hyperlink ref="A341" r:id="rId340"/>
     <hyperlink ref="A342" r:id="rId341"/>
     <hyperlink ref="A343" r:id="rId342"/>
+    <hyperlink ref="A344" r:id="rId343"/>
+    <hyperlink ref="A345" r:id="rId344"/>
+    <hyperlink ref="A346" r:id="rId345"/>
+    <hyperlink ref="A347" r:id="rId346"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -10440,7 +10533,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10479,90 +10572,27 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>913</v>
+        <v>926</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>914</v>
+        <v>927</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>915</v>
+        <v>928</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>916</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>46013.58541666667</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>917</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>637</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>918</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>919</v>
-      </c>
-      <c r="F3" s="2">
-        <v>46010.92638888889</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>920</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>921</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>922</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>923</v>
-      </c>
-      <c r="F4" s="2">
-        <v>46012.92291666666</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>924</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>925</v>
-      </c>
-      <c r="F5" s="2">
-        <v>46012.92152777778</v>
+        <v>46014.59444444445</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2025-12-24 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -3217,7 +3217,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F347"/>
+  <dimension ref="A1:F348"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10172,6 +10172,26 @@
       </c>
       <c r="F347" s="2">
         <v>46012.92152777778</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A348" s="3" t="s">
+        <v>926</v>
+      </c>
+      <c r="B348" s="4" t="s">
+        <v>927</v>
+      </c>
+      <c r="C348" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D348" s="4" t="s">
+        <v>928</v>
+      </c>
+      <c r="E348" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F348" s="2">
+        <v>46014.59444444445</v>
       </c>
     </row>
   </sheetData>
@@ -10522,6 +10542,7 @@
     <hyperlink ref="A345" r:id="rId344"/>
     <hyperlink ref="A346" r:id="rId345"/>
     <hyperlink ref="A347" r:id="rId346"/>
+    <hyperlink ref="A348" r:id="rId347"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -10533,7 +10554,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10570,30 +10591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>926</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>927</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>928</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="2">
-        <v>46014.59444444445</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2025-12-29 12:21
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="931">
   <si>
     <t>link</t>
   </si>
@@ -2805,6 +2805,12 @@
   </si>
   <si>
     <t>17000 m²</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/drustu-pag/fjcee.html</t>
+  </si>
+  <si>
+    <t>2.50 ha.</t>
   </si>
 </sst>
 </file>
@@ -10554,7 +10560,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10591,7 +10597,30 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>929</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>930</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2">
+        <v>46018.663194444445</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2025-12-30 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="932">
   <si>
     <t>link</t>
   </si>
@@ -2811,6 +2811,9 @@
   </si>
   <si>
     <t>2.50 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/zvirgzdenes-pag/pmnmj.html</t>
   </si>
 </sst>
 </file>
@@ -3223,7 +3226,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F348"/>
+  <dimension ref="A1:F349"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10198,6 +10201,26 @@
       </c>
       <c r="F348" s="2">
         <v>46014.59444444445</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A349" s="3" t="s">
+        <v>929</v>
+      </c>
+      <c r="B349" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C349" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D349" s="4" t="s">
+        <v>930</v>
+      </c>
+      <c r="E349" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F349" s="2">
+        <v>46018.663194444445</v>
       </c>
     </row>
   </sheetData>
@@ -10549,6 +10572,7 @@
     <hyperlink ref="A346" r:id="rId345"/>
     <hyperlink ref="A347" r:id="rId346"/>
     <hyperlink ref="A348" r:id="rId347"/>
+    <hyperlink ref="A349" r:id="rId348"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -10599,22 +10623,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>467</v>
+        <v>666</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>63</v>
+        <v>234</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>930</v>
+        <v>17</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>46018.663194444445</v>
+        <v>46020.83472222222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update forest data - 2025-12-31 12:21
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="932">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="936">
   <si>
     <t>link</t>
   </si>
@@ -2814,6 +2814,18 @@
   </si>
   <si>
     <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/zvirgzdenes-pag/pmnmj.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/aluksne/bchdfd.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ogre-and-reg/ledmanes-pag/jexlx.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/saldus-and-reg/novadnieku-pag/nmdkd.html</t>
+  </si>
+  <si>
+    <t>84720080179</t>
   </si>
 </sst>
 </file>
@@ -3226,7 +3238,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F349"/>
+  <dimension ref="A1:F350"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10221,6 +10233,26 @@
       </c>
       <c r="F349" s="2">
         <v>46018.663194444445</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A350" s="3" t="s">
+        <v>931</v>
+      </c>
+      <c r="B350" s="4" t="s">
+        <v>666</v>
+      </c>
+      <c r="C350" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D350" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E350" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F350" s="2">
+        <v>46020.83472222222</v>
       </c>
     </row>
   </sheetData>
@@ -10573,6 +10605,7 @@
     <hyperlink ref="A347" r:id="rId346"/>
     <hyperlink ref="A348" r:id="rId347"/>
     <hyperlink ref="A349" r:id="rId348"/>
+    <hyperlink ref="A350" r:id="rId349"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -10584,7 +10617,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10623,27 +10656,69 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>666</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>234</v>
+        <v>435</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>46020.83472222222</v>
+        <v>46021.68263888889</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>933</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="F3" s="2">
+        <v>46022.59722222222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>934</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>935</v>
+      </c>
+      <c r="F4" s="2">
+        <v>46021.74722222222</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-01 12:21
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -3238,7 +3238,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F350"/>
+  <dimension ref="A1:F353"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10253,6 +10253,66 @@
       </c>
       <c r="F350" s="2">
         <v>46020.83472222222</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A351" s="3" t="s">
+        <v>932</v>
+      </c>
+      <c r="B351" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C351" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D351" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E351" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F351" s="2">
+        <v>46021.68263888889</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A352" s="3" t="s">
+        <v>933</v>
+      </c>
+      <c r="B352" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C352" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D352" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E352" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="F352" s="2">
+        <v>46022.59722222222</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A353" s="3" t="s">
+        <v>934</v>
+      </c>
+      <c r="B353" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C353" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D353" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E353" s="4" t="s">
+        <v>935</v>
+      </c>
+      <c r="F353" s="2">
+        <v>46021.74722222222</v>
       </c>
     </row>
   </sheetData>
@@ -10606,6 +10666,9 @@
     <hyperlink ref="A348" r:id="rId347"/>
     <hyperlink ref="A349" r:id="rId348"/>
     <hyperlink ref="A350" r:id="rId349"/>
+    <hyperlink ref="A351" r:id="rId350"/>
+    <hyperlink ref="A352" r:id="rId351"/>
+    <hyperlink ref="A353" r:id="rId352"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -10617,7 +10680,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10654,72 +10717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>932</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="2">
-        <v>46021.68263888889</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>933</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>579</v>
-      </c>
-      <c r="F3" s="2">
-        <v>46022.59722222222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>934</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>935</v>
-      </c>
-      <c r="F4" s="2">
-        <v>46021.74722222222</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2026-01-02 12:19
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1777" uniqueCount="938">
   <si>
     <t>link</t>
   </si>
@@ -2826,6 +2826,12 @@
   </si>
   <si>
     <t>84720080179</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/berzpils-pag/mnmcj.html</t>
+  </si>
+  <si>
+    <t>38500050160</t>
   </si>
 </sst>
 </file>
@@ -10680,7 +10686,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10717,7 +10723,30 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>936</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>937</v>
+      </c>
+      <c r="F2" s="2">
+        <v>46024.558333333334</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2026-01-05 12:21
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1777" uniqueCount="938">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="951">
   <si>
     <t>link</t>
   </si>
@@ -2832,6 +2832,45 @@
   </si>
   <si>
     <t>38500050160</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/bauska-and-reg/islices-pag/ofhki.html</t>
+  </si>
+  <si>
+    <t>6 300 €</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jekabpils-and-reg/krustpils-pag/jmnen.html</t>
+  </si>
+  <si>
+    <t>3.65 ha.</t>
+  </si>
+  <si>
+    <t>56680060283</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jekabpils-and-reg/krustpils-pag/kfdjl.html</t>
+  </si>
+  <si>
+    <t>56680060573</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/audrinu-pag/cxdpb.html</t>
+  </si>
+  <si>
+    <t>6 200 €</t>
+  </si>
+  <si>
+    <t>1.10 ha.</t>
+  </si>
+  <si>
+    <t>78420020154</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/lendzu-pag/blmofi.html</t>
+  </si>
+  <si>
+    <t>78660040107</t>
   </si>
 </sst>
 </file>
@@ -3244,7 +3283,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F353"/>
+  <dimension ref="A1:F354"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10319,6 +10358,26 @@
       </c>
       <c r="F353" s="2">
         <v>46021.74722222222</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354" s="3" t="s">
+        <v>936</v>
+      </c>
+      <c r="B354" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C354" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D354" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E354" s="4" t="s">
+        <v>937</v>
+      </c>
+      <c r="F354" s="2">
+        <v>46024.558333333334</v>
       </c>
     </row>
   </sheetData>
@@ -10675,6 +10734,7 @@
     <hyperlink ref="A351" r:id="rId350"/>
     <hyperlink ref="A352" r:id="rId351"/>
     <hyperlink ref="A353" r:id="rId352"/>
+    <hyperlink ref="A354" r:id="rId353"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -10686,7 +10746,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10725,27 +10785,111 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>112</v>
+        <v>939</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>186</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>937</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>46024.558333333334</v>
+        <v>46025.58194444445</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>940</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>941</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>942</v>
+      </c>
+      <c r="F3" s="2">
+        <v>46025.65763888889</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>944</v>
+      </c>
+      <c r="F4" s="2">
+        <v>46025.64722222222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>945</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>946</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>947</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="F5" s="2">
+        <v>46026.76736111111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>949</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>950</v>
+      </c>
+      <c r="F6" s="2">
+        <v>46026.73541666666</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-06 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="951">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1822" uniqueCount="960">
   <si>
     <t>link</t>
   </si>
@@ -2871,6 +2871,33 @@
   </si>
   <si>
     <t>78660040107</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/priekulu-pag/bdjkcx.html</t>
+  </si>
+  <si>
+    <t>42720030144</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/liepas-pag/lkdcm.html</t>
+  </si>
+  <si>
+    <t>42600030079</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/gulbene-and-reg/galgauskas-pag/khelk.html</t>
+  </si>
+  <si>
+    <t>29 600 €</t>
+  </si>
+  <si>
+    <t>50560060064</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/liepupes-pag/hoxnl.html</t>
+  </si>
+  <si>
+    <t>4.60 ha.</t>
   </si>
 </sst>
 </file>
@@ -3283,7 +3310,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F354"/>
+  <dimension ref="A1:F359"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10378,6 +10405,106 @@
       </c>
       <c r="F354" s="2">
         <v>46024.558333333334</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A355" s="3" t="s">
+        <v>938</v>
+      </c>
+      <c r="B355" s="4" t="s">
+        <v>939</v>
+      </c>
+      <c r="C355" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D355" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E355" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F355" s="2">
+        <v>46025.58194444445</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A356" s="3" t="s">
+        <v>940</v>
+      </c>
+      <c r="B356" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C356" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D356" s="4" t="s">
+        <v>941</v>
+      </c>
+      <c r="E356" s="4" t="s">
+        <v>942</v>
+      </c>
+      <c r="F356" s="2">
+        <v>46025.65763888889</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A357" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="B357" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C357" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D357" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E357" s="4" t="s">
+        <v>944</v>
+      </c>
+      <c r="F357" s="2">
+        <v>46025.64722222222</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A358" s="3" t="s">
+        <v>945</v>
+      </c>
+      <c r="B358" s="4" t="s">
+        <v>946</v>
+      </c>
+      <c r="C358" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D358" s="4" t="s">
+        <v>947</v>
+      </c>
+      <c r="E358" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="F358" s="2">
+        <v>46026.76736111111</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A359" s="3" t="s">
+        <v>949</v>
+      </c>
+      <c r="B359" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C359" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D359" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E359" s="4" t="s">
+        <v>950</v>
+      </c>
+      <c r="F359" s="2">
+        <v>46026.73541666666</v>
       </c>
     </row>
   </sheetData>
@@ -10735,6 +10862,11 @@
     <hyperlink ref="A352" r:id="rId351"/>
     <hyperlink ref="A353" r:id="rId352"/>
     <hyperlink ref="A354" r:id="rId353"/>
+    <hyperlink ref="A355" r:id="rId354"/>
+    <hyperlink ref="A356" r:id="rId355"/>
+    <hyperlink ref="A357" r:id="rId356"/>
+    <hyperlink ref="A358" r:id="rId357"/>
+    <hyperlink ref="A359" r:id="rId358"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -10746,7 +10878,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10785,102 +10917,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>938</v>
+        <v>951</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>939</v>
+        <v>58</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>186</v>
+        <v>32</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>952</v>
       </c>
       <c r="F2" s="2">
-        <v>46025.58194444445</v>
+        <v>46028.57847222222</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>940</v>
+        <v>953</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>88</v>
+        <v>437</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>941</v>
+        <v>209</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>942</v>
+        <v>954</v>
       </c>
       <c r="F3" s="2">
-        <v>46025.65763888889</v>
+        <v>46027.75486111111</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>943</v>
+        <v>955</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>106</v>
+        <v>956</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>944</v>
+        <v>957</v>
       </c>
       <c r="F4" s="2">
-        <v>46025.64722222222</v>
+        <v>46028.57847222222</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>945</v>
+        <v>958</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>946</v>
+        <v>854</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>294</v>
+        <v>208</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>947</v>
+        <v>959</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>948</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2">
-        <v>46026.76736111111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>949</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>950</v>
-      </c>
-      <c r="F6" s="2">
-        <v>46026.73541666666</v>
+        <v>46028.51527777778</v>
       </c>
     </row>
   </sheetData>
@@ -10889,7 +11001,6 @@
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-07 12:21
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1822" uniqueCount="960">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="962">
   <si>
     <t>link</t>
   </si>
@@ -2898,6 +2898,12 @@
   </si>
   <si>
     <t>4.60 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/other/deobg.html</t>
+  </si>
+  <si>
+    <t>42760030110</t>
   </si>
 </sst>
 </file>
@@ -3310,7 +3316,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F359"/>
+  <dimension ref="A1:F363"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10505,6 +10511,86 @@
       </c>
       <c r="F359" s="2">
         <v>46026.73541666666</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A360" s="3" t="s">
+        <v>951</v>
+      </c>
+      <c r="B360" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C360" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D360" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E360" s="4" t="s">
+        <v>952</v>
+      </c>
+      <c r="F360" s="2">
+        <v>46028.57847222222</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A361" s="3" t="s">
+        <v>953</v>
+      </c>
+      <c r="B361" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="C361" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D361" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E361" s="4" t="s">
+        <v>954</v>
+      </c>
+      <c r="F361" s="2">
+        <v>46027.75486111111</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A362" s="3" t="s">
+        <v>955</v>
+      </c>
+      <c r="B362" s="4" t="s">
+        <v>956</v>
+      </c>
+      <c r="C362" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D362" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E362" s="4" t="s">
+        <v>957</v>
+      </c>
+      <c r="F362" s="2">
+        <v>46028.57847222222</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A363" s="3" t="s">
+        <v>958</v>
+      </c>
+      <c r="B363" s="4" t="s">
+        <v>854</v>
+      </c>
+      <c r="C363" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D363" s="4" t="s">
+        <v>959</v>
+      </c>
+      <c r="E363" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F363" s="2">
+        <v>46028.51527777778</v>
       </c>
     </row>
   </sheetData>
@@ -10867,6 +10953,10 @@
     <hyperlink ref="A357" r:id="rId356"/>
     <hyperlink ref="A358" r:id="rId357"/>
     <hyperlink ref="A359" r:id="rId358"/>
+    <hyperlink ref="A360" r:id="rId359"/>
+    <hyperlink ref="A361" r:id="rId360"/>
+    <hyperlink ref="A362" r:id="rId361"/>
+    <hyperlink ref="A363" r:id="rId362"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -10878,7 +10968,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10917,90 +11007,27 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>951</v>
+        <v>960</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>58</v>
+        <v>417</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>952</v>
+        <v>961</v>
       </c>
       <c r="F2" s="2">
-        <v>46028.57847222222</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>953</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>954</v>
-      </c>
-      <c r="F3" s="2">
-        <v>46027.75486111111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>955</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>956</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>957</v>
-      </c>
-      <c r="F4" s="2">
-        <v>46028.57847222222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>958</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>854</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>959</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2">
-        <v>46028.51527777778</v>
+        <v>46028.9125</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-08 12:21
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="962">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="968">
   <si>
     <t>link</t>
   </si>
@@ -2904,6 +2904,24 @@
   </si>
   <si>
     <t>42760030110</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kuldiga-and-reg/edoles-pag/bdjiih.html</t>
+  </si>
+  <si>
+    <t>62460060188</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/tukums-and-reg/engures-pag/dckfd.html</t>
+  </si>
+  <si>
+    <t>90500070062</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ventspils-and-reg/piltenes-l-t/ndjxx.html</t>
+  </si>
+  <si>
+    <t>98700090069</t>
   </si>
 </sst>
 </file>
@@ -3316,7 +3334,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F363"/>
+  <dimension ref="A1:F364"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10591,6 +10609,26 @@
       </c>
       <c r="F363" s="2">
         <v>46028.51527777778</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A364" s="3" t="s">
+        <v>960</v>
+      </c>
+      <c r="B364" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C364" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D364" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E364" s="4" t="s">
+        <v>961</v>
+      </c>
+      <c r="F364" s="2">
+        <v>46028.9125</v>
       </c>
     </row>
   </sheetData>
@@ -10957,6 +10995,7 @@
     <hyperlink ref="A361" r:id="rId360"/>
     <hyperlink ref="A362" r:id="rId361"/>
     <hyperlink ref="A363" r:id="rId362"/>
+    <hyperlink ref="A364" r:id="rId363"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -10968,7 +11007,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11007,27 +11046,69 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>417</v>
+        <v>185</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>25</v>
+        <v>424</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>82</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="F2" s="2">
-        <v>46028.9125</v>
+        <v>46030.59097222222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>964</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>965</v>
+      </c>
+      <c r="F3" s="2">
+        <v>46030.35972222222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>967</v>
+      </c>
+      <c r="F4" s="2">
+        <v>46030.49652777778</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-09 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="977">
   <si>
     <t>link</t>
   </si>
@@ -2922,6 +2922,33 @@
   </si>
   <si>
     <t>98700090069</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/zaubes-pag/eofpk.html</t>
+  </si>
+  <si>
+    <t>100 €</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/demenes-pag/adhng.html</t>
+  </si>
+  <si>
+    <t>53 000 €</t>
+  </si>
+  <si>
+    <t>44660060012</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/liepaja-and-reg/nicas-pag/jlbcm.html</t>
+  </si>
+  <si>
+    <t>123 €</t>
+  </si>
+  <si>
+    <t>64780120056</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/cesvaines-l-t/ildep.html</t>
   </si>
 </sst>
 </file>
@@ -3334,7 +3361,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F364"/>
+  <dimension ref="A1:F367"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10629,6 +10656,66 @@
       </c>
       <c r="F364" s="2">
         <v>46028.9125</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A365" s="3" t="s">
+        <v>962</v>
+      </c>
+      <c r="B365" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C365" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D365" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E365" s="4" t="s">
+        <v>963</v>
+      </c>
+      <c r="F365" s="2">
+        <v>46030.59097222222</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A366" s="3" t="s">
+        <v>964</v>
+      </c>
+      <c r="B366" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C366" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D366" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E366" s="4" t="s">
+        <v>965</v>
+      </c>
+      <c r="F366" s="2">
+        <v>46030.35972222222</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A367" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="B367" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C367" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="D367" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E367" s="4" t="s">
+        <v>967</v>
+      </c>
+      <c r="F367" s="2">
+        <v>46030.49652777778</v>
       </c>
     </row>
   </sheetData>
@@ -10996,6 +11083,9 @@
     <hyperlink ref="A362" r:id="rId361"/>
     <hyperlink ref="A363" r:id="rId362"/>
     <hyperlink ref="A364" r:id="rId363"/>
+    <hyperlink ref="A365" r:id="rId364"/>
+    <hyperlink ref="A366" r:id="rId365"/>
+    <hyperlink ref="A367" r:id="rId366"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -11007,7 +11097,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11046,62 +11136,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>962</v>
+        <v>968</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>185</v>
+        <v>969</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>424</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>82</v>
+        <v>272</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>963</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>46030.59097222222</v>
+        <v>46031.59513888889</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>964</v>
+        <v>970</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>576</v>
+        <v>971</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>376</v>
+        <v>74</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>272</v>
+        <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>965</v>
+        <v>972</v>
       </c>
       <c r="F3" s="2">
-        <v>46030.35972222222</v>
+        <v>46030.69305555556</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>966</v>
+        <v>973</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>274</v>
+        <v>974</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>404</v>
+        <v>190</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>186</v>
+        <v>272</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>967</v>
+        <v>975</v>
       </c>
       <c r="F4" s="2">
-        <v>46030.49652777778</v>
+        <v>46031.47777777778</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>976</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>928</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2">
+        <v>46030.740277777775</v>
       </c>
     </row>
   </sheetData>
@@ -11109,6 +11219,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-12 12:22
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="978">
   <si>
     <t>link</t>
   </si>
@@ -2949,6 +2949,9 @@
   </si>
   <si>
     <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/cesvaines-l-t/ildep.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/aronas-pag/fepkb.html</t>
   </si>
 </sst>
 </file>
@@ -3361,7 +3364,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F367"/>
+  <dimension ref="A1:F371"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10716,6 +10719,86 @@
       </c>
       <c r="F367" s="2">
         <v>46030.49652777778</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A368" s="3" t="s">
+        <v>968</v>
+      </c>
+      <c r="B368" s="4" t="s">
+        <v>969</v>
+      </c>
+      <c r="C368" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D368" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E368" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F368" s="2">
+        <v>46031.59513888889</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A369" s="3" t="s">
+        <v>970</v>
+      </c>
+      <c r="B369" s="4" t="s">
+        <v>971</v>
+      </c>
+      <c r="C369" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D369" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E369" s="4" t="s">
+        <v>972</v>
+      </c>
+      <c r="F369" s="2">
+        <v>46030.69305555556</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A370" s="3" t="s">
+        <v>973</v>
+      </c>
+      <c r="B370" s="4" t="s">
+        <v>974</v>
+      </c>
+      <c r="C370" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D370" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E370" s="4" t="s">
+        <v>975</v>
+      </c>
+      <c r="F370" s="2">
+        <v>46031.47777777778</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A371" s="3" t="s">
+        <v>976</v>
+      </c>
+      <c r="B371" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C371" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D371" s="4" t="s">
+        <v>928</v>
+      </c>
+      <c r="E371" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F371" s="2">
+        <v>46030.740277777775</v>
       </c>
     </row>
   </sheetData>
@@ -11086,6 +11169,10 @@
     <hyperlink ref="A365" r:id="rId364"/>
     <hyperlink ref="A366" r:id="rId365"/>
     <hyperlink ref="A367" r:id="rId366"/>
+    <hyperlink ref="A368" r:id="rId367"/>
+    <hyperlink ref="A369" r:id="rId368"/>
+    <hyperlink ref="A370" r:id="rId369"/>
+    <hyperlink ref="A371" r:id="rId370"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -11097,7 +11184,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11136,90 +11223,27 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>968</v>
+        <v>977</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>969</v>
+        <v>684</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>63</v>
+        <v>256</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>272</v>
+        <v>514</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>46031.59513888889</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>970</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>971</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>972</v>
-      </c>
-      <c r="F3" s="2">
-        <v>46030.69305555556</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>973</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>974</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>975</v>
-      </c>
-      <c r="F4" s="2">
-        <v>46031.47777777778</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>976</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>928</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2">
-        <v>46030.740277777775</v>
+        <v>46034.5125</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-13 12:21
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="998">
   <si>
     <t>link</t>
   </si>
@@ -2952,6 +2952,66 @@
   </si>
   <si>
     <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/aronas-pag/fepkb.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/mednevas-pag/kmhkk.html</t>
+  </si>
+  <si>
+    <t>7 000 €</t>
+  </si>
+  <si>
+    <t>38700050022</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/vecumu-pag/amgxp.html?_gl=1*1ccqz2i*_up*MQ..*_ga*NzY1NzgzMzgxLjE3NjgzMDY4NzA.*_ga_ZCGHC71BQ2*czE3NjgzMDY4NzAkbzEkZzAkdDE3NjgzMDY4NzAkajYwJGwwJGgw</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/vecumu-pag/cogdb.html?_gl=1*1wjyijr*_up*MQ..*_ga*NDI1NDA0MjIuMTc2ODMwNjg3MQ..*_ga_ZCGHC71BQ2*czE3NjgzMDY4NzAkbzEkZzAkdDE3NjgzMDY4NzAkajYwJGwwJGgw</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/bauska-and-reg/iecavas-nov/ibjpl.html</t>
+  </si>
+  <si>
+    <t>14800 m²</t>
+  </si>
+  <si>
+    <t>Xxxxx</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/bauska-and-reg/vecumnieku-pag/fjcij.html?_gl=1*109865b*_up*MQ..*_ga*ODg0NjQwNTgwLjE3NjgzMDY4NzM.*_ga_ZCGHC71BQ2*czE3NjgzMDY4NzMkbzEkZzAkdDE3NjgzMDY4NzMkajYwJGwwJGgw</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/bauska-and-reg/vecsaules-pag/cghmim.html?_gl=1*1bnjiy0*_up*MQ..*_ga*MTc4NzYwODE5OC4xNzY4MzA2ODc0*_ga_ZCGHC71BQ2*czE3NjgzMDY4NzMkbzEkZzAkdDE3NjgzMDY4NzMkajYwJGwwJGgw</t>
+  </si>
+  <si>
+    <t>23 000 €</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/izvaltas-pag/moomc.html</t>
+  </si>
+  <si>
+    <t>6064 003 0113</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/graveru-pag/mkdfj.html?_gl=1*13ntlob*_up*MQ..*_ga*MTgyNjQ1NTcxNy4xNzY4MzA2ODgz*_ga_ZCGHC71BQ2*czE3NjgzMDY4ODIkbzEkZzAkdDE3NjgzMDY4ODIkajYwJGwwJGgw</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/istras-pag/legmj.html</t>
+  </si>
+  <si>
+    <t>14.00 ha.</t>
+  </si>
+  <si>
+    <t>68600080094</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/malnavas-pag/jxmfo.html?_gl=1*16pucbi*_up*MQ..*_ga*MTM3NTQzNDg0OS4xNzY4MzA2ODg3*_ga_ZCGHC71BQ2*czE3NjgzMDY4ODckbzEkZzAkdDE3NjgzMDY4ODckajYwJGwwJGgw</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/merdzenes-pag/hmobk.html?_gl=1*1tkluhh*_up*MQ..*_ga*NTU3ODE2Njg3LjE3NjgzMDY4ODg.*_ga_ZCGHC71BQ2*czE3NjgzMDY4ODgkbzEkZzAkdDE3NjgzMDY4ODgkajYwJGwwJGgw</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/brigu-pag/kniic.html?_gl=1*f2vnos*_up*MQ..*_ga*MTMzMzI1MTgxNS4xNzY4MzA2ODg5*_ga_ZCGHC71BQ2*czE3NjgzMDY4ODgkbzEkZzAkdDE3NjgzMDY4ODgkajYwJGwwJGgw</t>
   </si>
 </sst>
 </file>
@@ -3364,7 +3424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F371"/>
+  <dimension ref="A1:F372"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10799,6 +10859,26 @@
       </c>
       <c r="F371" s="2">
         <v>46030.740277777775</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A372" s="3" t="s">
+        <v>977</v>
+      </c>
+      <c r="B372" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="C372" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D372" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="E372" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F372" s="2">
+        <v>46034.5125</v>
       </c>
     </row>
   </sheetData>
@@ -11173,6 +11253,7 @@
     <hyperlink ref="A369" r:id="rId368"/>
     <hyperlink ref="A370" r:id="rId369"/>
     <hyperlink ref="A371" r:id="rId370"/>
+    <hyperlink ref="A372" r:id="rId371"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -11184,7 +11265,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11223,27 +11304,258 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>684</v>
+        <v>979</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>256</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>514</v>
+        <v>272</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>980</v>
       </c>
       <c r="F2" s="2">
-        <v>46034.5125</v>
+        <v>46034.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>858</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>859</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="F3" s="2">
+        <v>46034.481944444444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>854</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>855</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>856</v>
+      </c>
+      <c r="F4" s="2">
+        <v>46034.481944444444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>984</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>985</v>
+      </c>
+      <c r="F5" s="2">
+        <v>46035.45833333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>986</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="2">
+        <v>46034.518055555556</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>987</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>988</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="2">
+        <v>46034.48263888889</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>989</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="F8" s="2">
+        <v>46035.49097222222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>991</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F9" s="2">
+        <v>46034.54722222222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>673</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>993</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>994</v>
+      </c>
+      <c r="F10" s="2">
+        <v>46034.73611111111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="F11" s="2">
+        <v>46034.481944444444</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>871</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>872</v>
+      </c>
+      <c r="F12" s="2">
+        <v>46034.481944444444</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>997</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>868</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>869</v>
+      </c>
+      <c r="F13" s="2">
+        <v>46034.481944444444</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A13" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-14 12:21
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="998">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="1003">
   <si>
     <t>link</t>
   </si>
@@ -3012,6 +3012,21 @@
   </si>
   <si>
     <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/brigu-pag/kniic.html?_gl=1*f2vnos*_up*MQ..*_ga*MTMzMzI1MTgxNS4xNzY4MzA2ODg5*_ga_ZCGHC71BQ2*czE3NjgzMDY4ODgkbzEkZzAkdDE3NjgzMDY4ODgkajYwJGwwJGgw</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jelgava-and-reg/valgundes-nov/glifp.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/robeznieku-pag/nnbfx.html</t>
+  </si>
+  <si>
+    <t>60860030283</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/feimanu-pag/aomnd.html</t>
+  </si>
+  <si>
+    <t>78520040087</t>
   </si>
 </sst>
 </file>
@@ -3424,7 +3439,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F372"/>
+  <dimension ref="A1:F384"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -10879,6 +10894,246 @@
       </c>
       <c r="F372" s="2">
         <v>46034.5125</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A373" s="3" t="s">
+        <v>978</v>
+      </c>
+      <c r="B373" s="4" t="s">
+        <v>979</v>
+      </c>
+      <c r="C373" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D373" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E373" s="4" t="s">
+        <v>980</v>
+      </c>
+      <c r="F373" s="2">
+        <v>46034.8</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A374" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B374" s="4" t="s">
+        <v>858</v>
+      </c>
+      <c r="C374" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D374" s="4" t="s">
+        <v>859</v>
+      </c>
+      <c r="E374" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="F374" s="2">
+        <v>46034.481944444444</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A375" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="B375" s="4" t="s">
+        <v>854</v>
+      </c>
+      <c r="C375" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D375" s="4" t="s">
+        <v>855</v>
+      </c>
+      <c r="E375" s="4" t="s">
+        <v>856</v>
+      </c>
+      <c r="F375" s="2">
+        <v>46034.481944444444</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A376" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="B376" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C376" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D376" s="4" t="s">
+        <v>984</v>
+      </c>
+      <c r="E376" s="4" t="s">
+        <v>985</v>
+      </c>
+      <c r="F376" s="2">
+        <v>46035.45833333333</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A377" s="3" t="s">
+        <v>986</v>
+      </c>
+      <c r="B377" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C377" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D377" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E377" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F377" s="2">
+        <v>46034.518055555556</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A378" s="3" t="s">
+        <v>987</v>
+      </c>
+      <c r="B378" s="4" t="s">
+        <v>988</v>
+      </c>
+      <c r="C378" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D378" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E378" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F378" s="2">
+        <v>46034.48263888889</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A379" s="3" t="s">
+        <v>989</v>
+      </c>
+      <c r="B379" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C379" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D379" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E379" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="F379" s="2">
+        <v>46035.49097222222</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A380" s="3" t="s">
+        <v>991</v>
+      </c>
+      <c r="B380" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C380" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D380" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E380" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F380" s="2">
+        <v>46034.54722222222</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A381" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="B381" s="4" t="s">
+        <v>673</v>
+      </c>
+      <c r="C381" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D381" s="4" t="s">
+        <v>993</v>
+      </c>
+      <c r="E381" s="4" t="s">
+        <v>994</v>
+      </c>
+      <c r="F381" s="2">
+        <v>46034.73611111111</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A382" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="B382" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C382" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D382" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E382" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="F382" s="2">
+        <v>46034.481944444444</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A383" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="B383" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C383" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D383" s="4" t="s">
+        <v>871</v>
+      </c>
+      <c r="E383" s="4" t="s">
+        <v>872</v>
+      </c>
+      <c r="F383" s="2">
+        <v>46034.481944444444</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A384" s="3" t="s">
+        <v>997</v>
+      </c>
+      <c r="B384" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C384" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D384" s="4" t="s">
+        <v>868</v>
+      </c>
+      <c r="E384" s="4" t="s">
+        <v>869</v>
+      </c>
+      <c r="F384" s="2">
+        <v>46034.481944444444</v>
       </c>
     </row>
   </sheetData>
@@ -11254,6 +11509,18 @@
     <hyperlink ref="A370" r:id="rId369"/>
     <hyperlink ref="A371" r:id="rId370"/>
     <hyperlink ref="A372" r:id="rId371"/>
+    <hyperlink ref="A373" r:id="rId372"/>
+    <hyperlink ref="A374" r:id="rId373"/>
+    <hyperlink ref="A375" r:id="rId374"/>
+    <hyperlink ref="A376" r:id="rId375"/>
+    <hyperlink ref="A377" r:id="rId376"/>
+    <hyperlink ref="A378" r:id="rId377"/>
+    <hyperlink ref="A379" r:id="rId378"/>
+    <hyperlink ref="A380" r:id="rId379"/>
+    <hyperlink ref="A381" r:id="rId380"/>
+    <hyperlink ref="A382" r:id="rId381"/>
+    <hyperlink ref="A383" r:id="rId382"/>
+    <hyperlink ref="A384" r:id="rId383"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -11265,7 +11532,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11304,242 +11571,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>978</v>
+        <v>998</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>979</v>
+        <v>204</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>518</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>272</v>
+        <v>162</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>980</v>
+        <v>846</v>
       </c>
       <c r="F2" s="2">
-        <v>46034.8</v>
+        <v>46036.575</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>981</v>
+        <v>999</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>858</v>
+        <v>88</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>28</v>
+        <v>146</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>859</v>
+        <v>186</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>860</v>
+        <v>1000</v>
       </c>
       <c r="F3" s="2">
-        <v>46034.481944444444</v>
+        <v>46035.96597222222</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>982</v>
+        <v>1001</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>854</v>
+        <v>576</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>28</v>
+        <v>294</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>855</v>
+        <v>147</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>856</v>
+        <v>1002</v>
       </c>
       <c r="F4" s="2">
-        <v>46034.481944444444</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>983</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>984</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>985</v>
-      </c>
-      <c r="F5" s="2">
-        <v>46035.45833333333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>986</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="2">
-        <v>46034.518055555556</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>987</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>988</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="2">
-        <v>46034.48263888889</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>989</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>990</v>
-      </c>
-      <c r="F8" s="2">
-        <v>46035.49097222222</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>991</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F9" s="2">
-        <v>46034.54722222222</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>992</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>673</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>993</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>994</v>
-      </c>
-      <c r="F10" s="2">
-        <v>46034.73611111111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>995</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="F11" s="2">
-        <v>46034.481944444444</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>996</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>871</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>872</v>
-      </c>
-      <c r="F12" s="2">
-        <v>46034.481944444444</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>997</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>868</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>869</v>
-      </c>
-      <c r="F13" s="2">
-        <v>46034.481944444444</v>
+        <v>46035.910416666666</v>
       </c>
     </row>
   </sheetData>
@@ -11547,15 +11634,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
-    <hyperlink ref="A12" r:id="rId11"/>
-    <hyperlink ref="A13" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-15 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -3439,7 +3439,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F384"/>
+  <dimension ref="A1:F387"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11134,6 +11134,66 @@
       </c>
       <c r="F384" s="2">
         <v>46034.481944444444</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A385" s="3" t="s">
+        <v>998</v>
+      </c>
+      <c r="B385" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C385" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="D385" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E385" s="4" t="s">
+        <v>846</v>
+      </c>
+      <c r="F385" s="2">
+        <v>46036.575</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A386" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="B386" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C386" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D386" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E386" s="4" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F386" s="2">
+        <v>46035.96597222222</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A387" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B387" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C387" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D387" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E387" s="4" t="s">
+        <v>1002</v>
+      </c>
+      <c r="F387" s="2">
+        <v>46035.910416666666</v>
       </c>
     </row>
   </sheetData>
@@ -11521,6 +11581,9 @@
     <hyperlink ref="A382" r:id="rId381"/>
     <hyperlink ref="A383" r:id="rId382"/>
     <hyperlink ref="A384" r:id="rId383"/>
+    <hyperlink ref="A385" r:id="rId384"/>
+    <hyperlink ref="A386" r:id="rId385"/>
+    <hyperlink ref="A387" r:id="rId386"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -11532,7 +11595,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11569,72 +11632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>998</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>518</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>846</v>
-      </c>
-      <c r="F2" s="2">
-        <v>46036.575</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>999</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>1000</v>
-      </c>
-      <c r="F3" s="2">
-        <v>46035.96597222222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1001</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>576</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>1002</v>
-      </c>
-      <c r="F4" s="2">
-        <v>46035.910416666666</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2026-01-16 12:20
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="1003">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="1032">
   <si>
     <t>link</t>
   </si>
@@ -3027,6 +3027,93 @@
   </si>
   <si>
     <t>78520040087</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/briezuciema-pag/gcflj.html</t>
+  </si>
+  <si>
+    <t>38520040022</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/ligatnes-pag/ldcxl.html</t>
+  </si>
+  <si>
+    <t>240 000 €</t>
+  </si>
+  <si>
+    <t>29 ha.</t>
+  </si>
+  <si>
+    <t>42620090040</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/ambelu-pag/geihe.html</t>
+  </si>
+  <si>
+    <t>19 800 €</t>
+  </si>
+  <si>
+    <t>6.60 ha.</t>
+  </si>
+  <si>
+    <t>44420040492</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/other/mlcgi.html</t>
+  </si>
+  <si>
+    <t>48 000 €</t>
+  </si>
+  <si>
+    <t>44350080055</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jekabpils-and-reg/mezares-pag/kxihc.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kraslavas-pag/cgimnm.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/braslavas-pag/amjnp.html</t>
+  </si>
+  <si>
+    <t>195 000 €</t>
+  </si>
+  <si>
+    <t>66440020142</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/staiceles-l-t/bpcdk.html</t>
+  </si>
+  <si>
+    <t>42.10 ha.</t>
+  </si>
+  <si>
+    <t>66370020046</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/nautrenu-pag/lbbjd.html</t>
+  </si>
+  <si>
+    <t>68760050071</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/sakstagala-pag/hnxfl.html</t>
+  </si>
+  <si>
+    <t>5 800 €</t>
+  </si>
+  <si>
+    <t>78860020587</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/valmiera-and-reg/valmieras-pag/hcjig.html</t>
+  </si>
+  <si>
+    <t>1 200 €</t>
+  </si>
+  <si>
+    <t>96900100060</t>
   </si>
 </sst>
 </file>
@@ -11595,7 +11682,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11632,7 +11719,240 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F2" s="2">
+        <v>46038.52986111111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F3" s="2">
+        <v>46037.84583333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F4" s="2">
+        <v>46037.73888888889</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="F5" s="2">
+        <v>46037.71527777778</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="2">
+        <v>46037.711805555555</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F7" s="2">
+        <v>46037.62430555555</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F8" s="2">
+        <v>46038.43680555555</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>1023</v>
+      </c>
+      <c r="F9" s="2">
+        <v>46037.78125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F10" s="2">
+        <v>46037.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F11" s="2">
+        <v>46037.71944444445</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>699</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F12" s="2">
+        <v>46038.59236111111</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update forest data - 2026-01-19 12:22
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="1032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2047" uniqueCount="1053">
   <si>
     <t>link</t>
   </si>
@@ -3114,6 +3114,69 @@
   </si>
   <si>
     <t>96900100060</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/briezuciema-pag/gcflj.html?_gl=1*10ch8fw*_up*MQ..*_ga*MTE3OTMzODg4OC4xNzY4ODI1MzI4*_ga_ZCGHC71BQ2*czE3Njg4MjUzMjckbzEkZzAkdDE3Njg4MjUzMjckajYwJGwwJGgw</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/liksnas-pag/jbkdf.html</t>
+  </si>
+  <si>
+    <t>2.10 ha.</t>
+  </si>
+  <si>
+    <t>4468-003-0052.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/vaboles-pag/fnlmn.html?_gl=1*1x3xgsa*_up*MQ..*_ga*MzI2Njc2MjczLjE3Njg4MjUzMzI.*_ga_ZCGHC71BQ2*czE3Njg4MjUzMzIkbzEkZzAkdDE3Njg4MjUzMzIkajYwJGwwJGgw</t>
+  </si>
+  <si>
+    <t>44940040060</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kalniesu-pag/becgme.html?_gl=1*dxn890*_up*MQ..*_ga*NzQwMjU1NDQyLjE3Njg4MjUzNDA.*_ga_ZCGHC71BQ2*czE3Njg4MjUzMzkkbzEkZzAkdDE3Njg4MjUzMzkkajYwJGwwJGgw</t>
+  </si>
+  <si>
+    <t>11.38 ha.</t>
+  </si>
+  <si>
+    <t>60680050169</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kalniesu-pag/ckmid.html?_gl=1*jgpqtw*_up*MQ..*_ga*OTY4MTIyNTI2LjE3Njg4MjUzNDA.*_ga_ZCGHC71BQ2*czE3Njg4MjUzNDAkbzEkZzAkdDE3Njg4MjUzNDAkajYwJGwwJGgw</t>
+  </si>
+  <si>
+    <t>60680070094</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kuldiga-and-reg/nikraces-pag/fjdgj.html</t>
+  </si>
+  <si>
+    <t>62680040114</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kuldiga-and-reg/varmes-pag/dpmoh.html?_gl=1*ybwt8d*_up*MQ..*_ga*NDQ0ODE1MjcuMTc2ODgyNTM0Mw..*_ga_ZCGHC71BQ2*czE3Njg4MjUzNDIkbzEkZzAkdDE3Njg4MjUzNDIkajYwJGwwJGgw</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/pildas-pag/hloec.html</t>
+  </si>
+  <si>
+    <t>68860050279</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/valka-and-reg/ergemes-pag/amefd.html</t>
+  </si>
+  <si>
+    <t>46 ha.</t>
+  </si>
+  <si>
+    <t>94520110156</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ventspils-and-reg/targales-pag/mfjgl.html</t>
+  </si>
+  <si>
+    <t>11 €</t>
   </si>
 </sst>
 </file>
@@ -3526,7 +3589,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F387"/>
+  <dimension ref="A1:F398"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11281,6 +11344,226 @@
       </c>
       <c r="F387" s="2">
         <v>46035.910416666666</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A388" s="3" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B388" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C388" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D388" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E388" s="4" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F388" s="2">
+        <v>46038.52986111111</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A389" s="3" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B389" s="4" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C389" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D389" s="4" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E389" s="4" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F389" s="2">
+        <v>46037.84583333333</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A390" s="3" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B390" s="4" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C390" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D390" s="4" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E390" s="4" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F390" s="2">
+        <v>46037.73888888889</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A391" s="3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B391" s="4" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C391" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D391" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E391" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="F391" s="2">
+        <v>46037.71527777778</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A392" s="3" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B392" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C392" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D392" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E392" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F392" s="2">
+        <v>46037.711805555555</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A393" s="3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B393" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C393" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D393" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E393" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F393" s="2">
+        <v>46037.62430555555</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A394" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B394" s="4" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C394" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D394" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="E394" s="4" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F394" s="2">
+        <v>46038.43680555555</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A395" s="3" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B395" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="C395" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D395" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E395" s="4" t="s">
+        <v>1023</v>
+      </c>
+      <c r="F395" s="2">
+        <v>46037.78125</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A396" s="3" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B396" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C396" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D396" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E396" s="4" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F396" s="2">
+        <v>46037.75</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A397" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B397" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C397" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D397" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E397" s="4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F397" s="2">
+        <v>46037.71944444445</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A398" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B398" s="4" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C398" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="D398" s="4" t="s">
+        <v>699</v>
+      </c>
+      <c r="E398" s="4" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F398" s="2">
+        <v>46038.59236111111</v>
       </c>
     </row>
   </sheetData>
@@ -11671,6 +11954,17 @@
     <hyperlink ref="A385" r:id="rId384"/>
     <hyperlink ref="A386" r:id="rId385"/>
     <hyperlink ref="A387" r:id="rId386"/>
+    <hyperlink ref="A388" r:id="rId387"/>
+    <hyperlink ref="A389" r:id="rId388"/>
+    <hyperlink ref="A390" r:id="rId389"/>
+    <hyperlink ref="A391" r:id="rId390"/>
+    <hyperlink ref="A392" r:id="rId391"/>
+    <hyperlink ref="A393" r:id="rId392"/>
+    <hyperlink ref="A394" r:id="rId393"/>
+    <hyperlink ref="A395" r:id="rId394"/>
+    <hyperlink ref="A396" r:id="rId395"/>
+    <hyperlink ref="A397" r:id="rId396"/>
+    <hyperlink ref="A398" r:id="rId397"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -11682,7 +11976,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11721,7 +12015,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1003</v>
+        <v>1032</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>467</v>
@@ -11741,202 +12035,182 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1005</v>
+        <v>1033</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1006</v>
+        <v>246</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>1007</v>
+        <v>1034</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1008</v>
+        <v>1035</v>
       </c>
       <c r="F3" s="2">
-        <v>46037.84583333333</v>
+        <v>46041.54166666667</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1009</v>
+        <v>1036</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1010</v>
+        <v>27</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>1011</v>
+        <v>903</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>1012</v>
+        <v>1037</v>
       </c>
       <c r="F4" s="2">
-        <v>46037.73888888889</v>
+        <v>46039.41666666667</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1013</v>
+        <v>1038</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1014</v>
+        <v>781</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>74</v>
+        <v>146</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>103</v>
+        <v>1039</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>1015</v>
+        <v>1040</v>
       </c>
       <c r="F5" s="2">
-        <v>46037.71527777778</v>
+        <v>46039.65833333333</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1016</v>
+        <v>1041</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>116</v>
+        <v>43</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>272</v>
+        <v>186</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>25</v>
+        <v>1042</v>
       </c>
       <c r="F6" s="2">
-        <v>46037.711805555555</v>
+        <v>46039.356944444444</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>1017</v>
+        <v>1043</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>146</v>
+        <v>424</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>175</v>
+        <v>260</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>176</v>
+        <v>1044</v>
       </c>
       <c r="F7" s="2">
-        <v>46037.62430555555</v>
+        <v>46041.50208333333</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>1018</v>
+        <v>1045</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1019</v>
+        <v>848</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>208</v>
+        <v>424</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>260</v>
+        <v>849</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>1020</v>
+        <v>25</v>
       </c>
       <c r="F8" s="2">
-        <v>46038.43680555555</v>
+        <v>46039.75625</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>1021</v>
+        <v>1046</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>590</v>
+        <v>88</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>1022</v>
+        <v>761</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>1023</v>
+        <v>1047</v>
       </c>
       <c r="F9" s="2">
-        <v>46037.78125</v>
+        <v>46041.55069444445</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>1024</v>
+        <v>1048</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>161</v>
+        <v>793</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>294</v>
+        <v>392</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>162</v>
+        <v>1049</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>1025</v>
+        <v>1050</v>
       </c>
       <c r="F10" s="2">
-        <v>46037.75</v>
+        <v>46039.47430555556</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>1026</v>
+        <v>1051</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>1027</v>
+        <v>1052</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>294</v>
+        <v>404</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>186</v>
+        <v>272</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>1028</v>
+        <v>25</v>
       </c>
       <c r="F11" s="2">
-        <v>46037.71944444445</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>1029</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>1030</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>699</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>1031</v>
-      </c>
-      <c r="F12" s="2">
-        <v>46038.59236111111</v>
+        <v>46041.513194444444</v>
       </c>
     </row>
   </sheetData>
@@ -11951,7 +12225,6 @@
     <hyperlink ref="A9" r:id="rId8"/>
     <hyperlink ref="A10" r:id="rId9"/>
     <hyperlink ref="A11" r:id="rId10"/>
-    <hyperlink ref="A12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-20 12:22
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2047" uniqueCount="1053">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="1066">
   <si>
     <t>link</t>
   </si>
@@ -3177,6 +3177,45 @@
   </si>
   <si>
     <t>11 €</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/kalupes-pag/nlcoe.html</t>
+  </si>
+  <si>
+    <t>44620030081</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kastulinas-pag/mfcbj.html</t>
+  </si>
+  <si>
+    <t>6072007039</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/izvaltas-pag/bxnjfe.html</t>
+  </si>
+  <si>
+    <t>60640040044</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/izvaltas-pag/bxnjdh.html</t>
+  </si>
+  <si>
+    <t>60640050017</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/valmiera-and-reg/valmieras-pag/ebojd.html</t>
+  </si>
+  <si>
+    <t>96880060034</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/valmiera-and-reg/jeru-pag/bhkbik.html</t>
+  </si>
+  <si>
+    <t>6.40 ha.</t>
+  </si>
+  <si>
+    <t>96580060060</t>
   </si>
 </sst>
 </file>
@@ -3589,7 +3628,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F398"/>
+  <dimension ref="A1:F408"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11564,6 +11603,206 @@
       </c>
       <c r="F398" s="2">
         <v>46038.59236111111</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A399" s="3" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B399" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C399" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D399" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E399" s="4" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F399" s="2">
+        <v>46038.52986111111</v>
+      </c>
+    </row>
+    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A400" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B400" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C400" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D400" s="4" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E400" s="4" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F400" s="2">
+        <v>46041.54166666667</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A401" s="3" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B401" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C401" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D401" s="4" t="s">
+        <v>903</v>
+      </c>
+      <c r="E401" s="4" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F401" s="2">
+        <v>46039.41666666667</v>
+      </c>
+    </row>
+    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A402" s="3" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B402" s="4" t="s">
+        <v>781</v>
+      </c>
+      <c r="C402" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D402" s="4" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E402" s="4" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F402" s="2">
+        <v>46039.65833333333</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A403" s="3" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B403" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C403" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D403" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E403" s="4" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F403" s="2">
+        <v>46039.356944444444</v>
+      </c>
+    </row>
+    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A404" s="3" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B404" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C404" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D404" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="E404" s="4" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F404" s="2">
+        <v>46041.50208333333</v>
+      </c>
+    </row>
+    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A405" s="3" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B405" s="4" t="s">
+        <v>848</v>
+      </c>
+      <c r="C405" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D405" s="4" t="s">
+        <v>849</v>
+      </c>
+      <c r="E405" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F405" s="2">
+        <v>46039.75625</v>
+      </c>
+    </row>
+    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A406" s="3" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B406" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C406" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D406" s="4" t="s">
+        <v>761</v>
+      </c>
+      <c r="E406" s="4" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F406" s="2">
+        <v>46041.55069444445</v>
+      </c>
+    </row>
+    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A407" s="3" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B407" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="C407" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D407" s="4" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E407" s="4" t="s">
+        <v>1050</v>
+      </c>
+      <c r="F407" s="2">
+        <v>46039.47430555556</v>
+      </c>
+    </row>
+    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A408" s="3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B408" s="4" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C408" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="D408" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E408" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F408" s="2">
+        <v>46041.513194444444</v>
       </c>
     </row>
   </sheetData>
@@ -11965,6 +12204,16 @@
     <hyperlink ref="A396" r:id="rId395"/>
     <hyperlink ref="A397" r:id="rId396"/>
     <hyperlink ref="A398" r:id="rId397"/>
+    <hyperlink ref="A399" r:id="rId398"/>
+    <hyperlink ref="A400" r:id="rId399"/>
+    <hyperlink ref="A401" r:id="rId400"/>
+    <hyperlink ref="A402" r:id="rId401"/>
+    <hyperlink ref="A403" r:id="rId402"/>
+    <hyperlink ref="A404" r:id="rId403"/>
+    <hyperlink ref="A405" r:id="rId404"/>
+    <hyperlink ref="A406" r:id="rId405"/>
+    <hyperlink ref="A407" r:id="rId406"/>
+    <hyperlink ref="A408" r:id="rId407"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -11976,7 +12225,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -12015,202 +12264,122 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1032</v>
+        <v>1053</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>467</v>
+        <v>204</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>272</v>
+        <v>154</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1004</v>
+        <v>1054</v>
       </c>
       <c r="F2" s="2">
-        <v>46038.52986111111</v>
+        <v>46042.59097222222</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1033</v>
+        <v>1055</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>246</v>
+        <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>74</v>
+        <v>146</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>1034</v>
+        <v>36</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1035</v>
+        <v>1056</v>
       </c>
       <c r="F3" s="2">
-        <v>46041.54166666667</v>
+        <v>46041.87847222222</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1036</v>
+        <v>1057</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>27</v>
+        <v>131</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>74</v>
+        <v>146</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>903</v>
+        <v>94</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>1037</v>
+        <v>1058</v>
       </c>
       <c r="F4" s="2">
-        <v>46039.41666666667</v>
+        <v>46041.728472222225</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1038</v>
+        <v>1059</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>781</v>
+        <v>157</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>1039</v>
+        <v>36</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>1040</v>
+        <v>1060</v>
       </c>
       <c r="F5" s="2">
-        <v>46039.65833333333</v>
+        <v>46041.70763888889</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1041</v>
+        <v>1061</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>43</v>
+        <v>1014</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>146</v>
+        <v>396</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>186</v>
+        <v>75</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>1042</v>
+        <v>1062</v>
       </c>
       <c r="F6" s="2">
-        <v>46039.356944444444</v>
+        <v>46041.80972222222</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>1043</v>
+        <v>1063</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>424</v>
+        <v>396</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>260</v>
+        <v>1064</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>1044</v>
+        <v>1065</v>
       </c>
       <c r="F7" s="2">
-        <v>46041.50208333333</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>1045</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>848</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>424</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>849</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="2">
-        <v>46039.75625</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>1046</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>761</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>1047</v>
-      </c>
-      <c r="F9" s="2">
-        <v>46041.55069444445</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>1048</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>793</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>1049</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>1050</v>
-      </c>
-      <c r="F10" s="2">
-        <v>46039.47430555556</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>1051</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>1052</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="2">
-        <v>46041.513194444444</v>
+        <v>46041.59930555556</v>
       </c>
     </row>
   </sheetData>
@@ -12221,10 +12390,6 @@
     <hyperlink ref="A5" r:id="rId4"/>
     <hyperlink ref="A6" r:id="rId5"/>
     <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-21 12:22
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="1066">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="1078">
   <si>
     <t>link</t>
   </si>
@@ -3216,6 +3216,42 @@
   </si>
   <si>
     <t>96580060060</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/susaju-pag/bbhej.html</t>
+  </si>
+  <si>
+    <t>166 000 €</t>
+  </si>
+  <si>
+    <t>39 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/raiskuma-pag/jfbdi.html</t>
+  </si>
+  <si>
+    <t>42740110037</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/sventes-pag/felde.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/salnavas-pag/ebhmd.html</t>
+  </si>
+  <si>
+    <t>68940010054</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/talsi-and-reg/vandzenes-pag/hidji.html</t>
+  </si>
+  <si>
+    <t>2 000 €</t>
+  </si>
+  <si>
+    <t>0.54 ha.</t>
+  </si>
+  <si>
+    <t>88940050034</t>
   </si>
 </sst>
 </file>
@@ -3628,7 +3664,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F408"/>
+  <dimension ref="A1:F414"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11803,6 +11839,126 @@
       </c>
       <c r="F408" s="2">
         <v>46041.513194444444</v>
+      </c>
+    </row>
+    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A409" s="3" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B409" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C409" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D409" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E409" s="4" t="s">
+        <v>1054</v>
+      </c>
+      <c r="F409" s="2">
+        <v>46042.59097222222</v>
+      </c>
+    </row>
+    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A410" s="3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B410" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C410" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D410" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E410" s="4" t="s">
+        <v>1056</v>
+      </c>
+      <c r="F410" s="2">
+        <v>46041.87847222222</v>
+      </c>
+    </row>
+    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A411" s="3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B411" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C411" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D411" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E411" s="4" t="s">
+        <v>1058</v>
+      </c>
+      <c r="F411" s="2">
+        <v>46041.728472222225</v>
+      </c>
+    </row>
+    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A412" s="3" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B412" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C412" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D412" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E412" s="4" t="s">
+        <v>1060</v>
+      </c>
+      <c r="F412" s="2">
+        <v>46041.70763888889</v>
+      </c>
+    </row>
+    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A413" s="3" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B413" s="4" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C413" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="D413" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E413" s="4" t="s">
+        <v>1062</v>
+      </c>
+      <c r="F413" s="2">
+        <v>46041.80972222222</v>
+      </c>
+    </row>
+    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A414" s="3" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B414" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C414" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="D414" s="4" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E414" s="4" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F414" s="2">
+        <v>46041.59930555556</v>
       </c>
     </row>
   </sheetData>
@@ -12214,6 +12370,12 @@
     <hyperlink ref="A406" r:id="rId405"/>
     <hyperlink ref="A407" r:id="rId406"/>
     <hyperlink ref="A408" r:id="rId407"/>
+    <hyperlink ref="A409" r:id="rId408"/>
+    <hyperlink ref="A410" r:id="rId409"/>
+    <hyperlink ref="A411" r:id="rId410"/>
+    <hyperlink ref="A412" r:id="rId411"/>
+    <hyperlink ref="A413" r:id="rId412"/>
+    <hyperlink ref="A414" r:id="rId413"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -12225,7 +12387,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -12264,122 +12426,102 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1053</v>
+        <v>1066</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>204</v>
+        <v>1067</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>154</v>
+        <v>1068</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1054</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>46042.59097222222</v>
+        <v>46042.68125</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1055</v>
+        <v>1069</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>274</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>146</v>
+        <v>63</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1056</v>
+        <v>1070</v>
       </c>
       <c r="F3" s="2">
-        <v>46041.87847222222</v>
+        <v>46042.847916666666</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1057</v>
+        <v>1071</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>131</v>
+        <v>549</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>146</v>
+        <v>74</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>1058</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2">
-        <v>46041.728472222225</v>
+        <v>46042.73333333334</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1059</v>
+        <v>1072</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>157</v>
+        <v>334</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>146</v>
+        <v>234</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>36</v>
+        <v>272</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>1060</v>
+        <v>1073</v>
       </c>
       <c r="F5" s="2">
-        <v>46041.70763888889</v>
+        <v>46042.74166666667</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1061</v>
+        <v>1074</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1014</v>
+        <v>1075</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>396</v>
+        <v>356</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>75</v>
+        <v>1076</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>1062</v>
+        <v>1077</v>
       </c>
       <c r="F6" s="2">
-        <v>46041.80972222222</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1063</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>1065</v>
-      </c>
-      <c r="F7" s="2">
-        <v>46041.59930555556</v>
+        <v>46042.700694444444</v>
       </c>
     </row>
   </sheetData>
@@ -12389,7 +12531,6 @@
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
     <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-22 12:23
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="1078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="1086">
   <si>
     <t>link</t>
   </si>
@@ -3252,6 +3252,30 @@
   </si>
   <si>
     <t>88940050034</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aizkraukle-and-reg/aizkraukles/ikfjj.html</t>
+  </si>
+  <si>
+    <t>32780070152</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/alsviku-pag/bnxil.html</t>
+  </si>
+  <si>
+    <t>14.10 ha.</t>
+  </si>
+  <si>
+    <t>36420120063</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/mezvidu-pag/hlcnn.html</t>
+  </si>
+  <si>
+    <t>2.39 ha.</t>
+  </si>
+  <si>
+    <t>68700050186</t>
   </si>
 </sst>
 </file>
@@ -3664,7 +3688,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F414"/>
+  <dimension ref="A1:F419"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11959,6 +11983,106 @@
       </c>
       <c r="F414" s="2">
         <v>46041.59930555556</v>
+      </c>
+    </row>
+    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A415" s="3" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B415" s="4" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C415" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D415" s="4" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E415" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F415" s="2">
+        <v>46042.68125</v>
+      </c>
+    </row>
+    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A416" s="3" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B416" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C416" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D416" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E416" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F416" s="2">
+        <v>46042.847916666666</v>
+      </c>
+    </row>
+    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A417" s="3" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B417" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="C417" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D417" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E417" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F417" s="2">
+        <v>46042.73333333334</v>
+      </c>
+    </row>
+    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A418" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B418" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C418" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D418" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E418" s="4" t="s">
+        <v>1073</v>
+      </c>
+      <c r="F418" s="2">
+        <v>46042.74166666667</v>
+      </c>
+    </row>
+    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A419" s="3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B419" s="4" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C419" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D419" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E419" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F419" s="2">
+        <v>46042.700694444444</v>
       </c>
     </row>
   </sheetData>
@@ -12376,6 +12500,11 @@
     <hyperlink ref="A412" r:id="rId411"/>
     <hyperlink ref="A413" r:id="rId412"/>
     <hyperlink ref="A414" r:id="rId413"/>
+    <hyperlink ref="A415" r:id="rId414"/>
+    <hyperlink ref="A416" r:id="rId415"/>
+    <hyperlink ref="A417" r:id="rId416"/>
+    <hyperlink ref="A418" r:id="rId417"/>
+    <hyperlink ref="A419" r:id="rId418"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -12387,7 +12516,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -12426,102 +12555,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1066</v>
+        <v>1078</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1067</v>
+        <v>246</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1068</v>
+        <v>82</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>1079</v>
       </c>
       <c r="F2" s="2">
-        <v>46042.68125</v>
+        <v>46044.56736111111</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1069</v>
+        <v>1080</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>63</v>
+        <v>435</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>162</v>
+        <v>1081</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1070</v>
+        <v>1082</v>
       </c>
       <c r="F3" s="2">
-        <v>46042.847916666666</v>
+        <v>46043.68888888889</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1071</v>
+        <v>1083</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>549</v>
+        <v>131</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>74</v>
+        <v>234</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>82</v>
+        <v>1084</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>25</v>
+        <v>1085</v>
       </c>
       <c r="F4" s="2">
-        <v>46042.73333333334</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>1072</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>1073</v>
-      </c>
-      <c r="F5" s="2">
-        <v>46042.74166666667</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>1074</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>1075</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>1077</v>
-      </c>
-      <c r="F6" s="2">
-        <v>46042.700694444444</v>
+        <v>46043.6125</v>
       </c>
     </row>
   </sheetData>
@@ -12529,8 +12618,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-23 12:22
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="1086">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2147" uniqueCount="1099">
   <si>
     <t>link</t>
   </si>
@@ -3276,6 +3276,45 @@
   </si>
   <si>
     <t>68700050186</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jekabpils-and-reg/jekabpils/ckbgp.html</t>
+  </si>
+  <si>
+    <t>56720110036</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/svarinu-pag/ixhpl.html</t>
+  </si>
+  <si>
+    <t>60900020075</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kombulu-pag/kofeb.html</t>
+  </si>
+  <si>
+    <t>60740020222</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/limbazu-pag/bebid.html</t>
+  </si>
+  <si>
+    <t>7.52 ha.</t>
+  </si>
+  <si>
+    <t>66640100023</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/isnaudas-pag/aobmi.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/valka-and-reg/varinu-pag/bbeepp.html</t>
+  </si>
+  <si>
+    <t>550 000 €</t>
+  </si>
+  <si>
+    <t>94900030021</t>
   </si>
 </sst>
 </file>
@@ -3688,7 +3727,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F419"/>
+  <dimension ref="A1:F422"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -12083,6 +12122,66 @@
       </c>
       <c r="F419" s="2">
         <v>46042.700694444444</v>
+      </c>
+    </row>
+    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A420" s="3" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B420" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C420" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D420" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E420" s="4" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F420" s="2">
+        <v>46044.56736111111</v>
+      </c>
+    </row>
+    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A421" s="3" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B421" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C421" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D421" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E421" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F421" s="2">
+        <v>46043.68888888889</v>
+      </c>
+    </row>
+    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A422" s="3" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B422" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C422" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D422" s="4" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E422" s="4" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F422" s="2">
+        <v>46043.6125</v>
       </c>
     </row>
   </sheetData>
@@ -12505,6 +12604,9 @@
     <hyperlink ref="A417" r:id="rId416"/>
     <hyperlink ref="A418" r:id="rId417"/>
     <hyperlink ref="A419" r:id="rId418"/>
+    <hyperlink ref="A420" r:id="rId419"/>
+    <hyperlink ref="A421" r:id="rId420"/>
+    <hyperlink ref="A422" r:id="rId421"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -12516,7 +12618,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -12555,62 +12657,122 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1078</v>
+        <v>1086</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>246</v>
+        <v>174</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1079</v>
+        <v>1087</v>
       </c>
       <c r="F2" s="2">
-        <v>46044.56736111111</v>
+        <v>46044.73472222222</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1080</v>
+        <v>1088</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>290</v>
+        <v>43</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>435</v>
+        <v>146</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>1081</v>
+        <v>36</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1082</v>
+        <v>1089</v>
       </c>
       <c r="F3" s="2">
-        <v>46043.68888888889</v>
+        <v>46045.350694444445</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1083</v>
+        <v>1090</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>131</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F4" s="2">
+        <v>46044.78472222222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="F5" s="2">
+        <v>46045.40972222222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>1085</v>
-      </c>
-      <c r="F4" s="2">
-        <v>46043.6125</v>
+      <c r="D6" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="2">
+        <v>46045.396527777775</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="F7" s="2">
+        <v>46045.37152777778</v>
       </c>
     </row>
   </sheetData>
@@ -12618,6 +12780,9 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-26 12:22
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2147" uniqueCount="1099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="1110">
   <si>
     <t>link</t>
   </si>
@@ -3315,6 +3315,39 @@
   </si>
   <si>
     <t>94900030021</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/bikernieku-pag/jpblk.html</t>
+  </si>
+  <si>
+    <t>44740040036</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/jekabpils-and-reg/rubenes-pag/noegf.html</t>
+  </si>
+  <si>
+    <t>56820010016</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kalniesu-pag/becgme.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/liepaja-and-reg/lazas-pag/nfpce.html</t>
+  </si>
+  <si>
+    <t>64720060002</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/aronas-pag/cgdklc.html</t>
+  </si>
+  <si>
+    <t>70420080028</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/tukums-and-reg/jaunsatu-pag/ockkd.html</t>
+  </si>
+  <si>
+    <t>90580030043</t>
   </si>
 </sst>
 </file>
@@ -3727,7 +3760,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F422"/>
+  <dimension ref="A1:F428"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -12182,6 +12215,126 @@
       </c>
       <c r="F422" s="2">
         <v>46043.6125</v>
+      </c>
+    </row>
+    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A423" s="3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B423" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C423" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D423" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E423" s="4" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F423" s="2">
+        <v>46044.73472222222</v>
+      </c>
+    </row>
+    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A424" s="3" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B424" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C424" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D424" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E424" s="4" t="s">
+        <v>1089</v>
+      </c>
+      <c r="F424" s="2">
+        <v>46045.350694444445</v>
+      </c>
+    </row>
+    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A425" s="3" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B425" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C425" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D425" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E425" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F425" s="2">
+        <v>46044.78472222222</v>
+      </c>
+    </row>
+    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A426" s="3" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B426" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C426" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D426" s="4" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E426" s="4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="F426" s="2">
+        <v>46045.40972222222</v>
+      </c>
+    </row>
+    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A427" s="3" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B427" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C427" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D427" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E427" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F427" s="2">
+        <v>46045.396527777775</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A428" s="3" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B428" s="4" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C428" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D428" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E428" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="F428" s="2">
+        <v>46045.37152777778</v>
       </c>
     </row>
   </sheetData>
@@ -12607,6 +12760,12 @@
     <hyperlink ref="A420" r:id="rId419"/>
     <hyperlink ref="A421" r:id="rId420"/>
     <hyperlink ref="A422" r:id="rId421"/>
+    <hyperlink ref="A423" r:id="rId422"/>
+    <hyperlink ref="A424" r:id="rId423"/>
+    <hyperlink ref="A425" r:id="rId424"/>
+    <hyperlink ref="A426" r:id="rId425"/>
+    <hyperlink ref="A427" r:id="rId426"/>
+    <hyperlink ref="A428" r:id="rId427"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -12657,122 +12816,122 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1086</v>
+        <v>1099</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>174</v>
+        <v>211</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>127</v>
+        <v>74</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1087</v>
+        <v>1100</v>
       </c>
       <c r="F2" s="2">
-        <v>46044.73472222222</v>
+        <v>46047.665972222225</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1088</v>
+        <v>1101</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1089</v>
+        <v>1102</v>
       </c>
       <c r="F3" s="2">
-        <v>46045.350694444445</v>
+        <v>46048.427777777775</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1090</v>
+        <v>1103</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>162</v>
+        <v>32</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>1091</v>
+        <v>1040</v>
       </c>
       <c r="F4" s="2">
-        <v>46044.78472222222</v>
+        <v>46047.51597222222</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1092</v>
+        <v>1104</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>274</v>
+        <v>650</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>1093</v>
+        <v>59</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>1094</v>
+        <v>1105</v>
       </c>
       <c r="F5" s="2">
-        <v>46045.40972222222</v>
+        <v>46048.32986111111</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1095</v>
+        <v>1106</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>185</v>
+        <v>271</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>234</v>
+        <v>256</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>186</v>
+        <v>272</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>25</v>
+        <v>1107</v>
       </c>
       <c r="F6" s="2">
-        <v>46045.396527777775</v>
+        <v>46048.33333333333</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>1096</v>
+        <v>1108</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1097</v>
+        <v>274</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>186</v>
+        <v>82</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>1098</v>
+        <v>1109</v>
       </c>
       <c r="F7" s="2">
-        <v>46045.37152777778</v>
+        <v>46045.603472222225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update forest data - 2026-01-27 12:22
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="1110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2202" uniqueCount="1120">
   <si>
     <t>link</t>
   </si>
@@ -3348,6 +3348,36 @@
   </si>
   <si>
     <t>90580030043</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/balvu-pag/hhgfc.html</t>
+  </si>
+  <si>
+    <t>36480010023</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/susaju-pag/adfpm.html</t>
+  </si>
+  <si>
+    <t>38780090085</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/bauska-and-reg/vecumnieku-pag/dbnld.html</t>
+  </si>
+  <si>
+    <t>5 900 €</t>
+  </si>
+  <si>
+    <t>40940120749</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/istras-pag/legnh.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/istras-pag/nkpgf.html</t>
+  </si>
+  <si>
+    <t>6860 008 0094</t>
   </si>
 </sst>
 </file>
@@ -3760,7 +3790,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F428"/>
+  <dimension ref="A1:F434"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -12335,6 +12365,126 @@
       </c>
       <c r="F428" s="2">
         <v>46045.37152777778</v>
+      </c>
+    </row>
+    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A429" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B429" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C429" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D429" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E429" s="4" t="s">
+        <v>1100</v>
+      </c>
+      <c r="F429" s="2">
+        <v>46047.665972222225</v>
+      </c>
+    </row>
+    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A430" s="3" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B430" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C430" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D430" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E430" s="4" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F430" s="2">
+        <v>46048.427777777775</v>
+      </c>
+    </row>
+    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A431" s="3" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B431" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C431" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D431" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E431" s="4" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F431" s="2">
+        <v>46047.51597222222</v>
+      </c>
+    </row>
+    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A432" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B432" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="C432" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D432" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E432" s="4" t="s">
+        <v>1105</v>
+      </c>
+      <c r="F432" s="2">
+        <v>46048.32986111111</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A433" s="3" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B433" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C433" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D433" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E433" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="F433" s="2">
+        <v>46048.33333333333</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A434" s="3" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B434" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C434" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D434" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E434" s="4" t="s">
+        <v>1109</v>
+      </c>
+      <c r="F434" s="2">
+        <v>46045.603472222225</v>
       </c>
     </row>
   </sheetData>
@@ -12766,6 +12916,12 @@
     <hyperlink ref="A426" r:id="rId425"/>
     <hyperlink ref="A427" r:id="rId426"/>
     <hyperlink ref="A428" r:id="rId427"/>
+    <hyperlink ref="A429" r:id="rId428"/>
+    <hyperlink ref="A430" r:id="rId429"/>
+    <hyperlink ref="A431" r:id="rId430"/>
+    <hyperlink ref="A432" r:id="rId431"/>
+    <hyperlink ref="A433" r:id="rId432"/>
+    <hyperlink ref="A434" r:id="rId433"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -12777,7 +12933,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -12816,122 +12972,102 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1099</v>
+        <v>1110</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>211</v>
+        <v>70</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1100</v>
+        <v>1111</v>
       </c>
       <c r="F2" s="2">
-        <v>46047.665972222225</v>
+        <v>46049.521527777775</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1101</v>
+        <v>1112</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>127</v>
+        <v>28</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>85</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1102</v>
+        <v>1113</v>
       </c>
       <c r="F3" s="2">
-        <v>46048.427777777775</v>
+        <v>46049.433333333334</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1103</v>
+        <v>1114</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>1115</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>146</v>
+        <v>48</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>1040</v>
+        <v>1116</v>
       </c>
       <c r="F4" s="2">
-        <v>46047.51597222222</v>
+        <v>46048.88333333333</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1104</v>
+        <v>1117</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>650</v>
+        <v>106</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>190</v>
+        <v>234</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>1105</v>
+        <v>994</v>
       </c>
       <c r="F5" s="2">
-        <v>46048.32986111111</v>
+        <v>46048.799305555556</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1106</v>
+        <v>1118</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>271</v>
+        <v>781</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>256</v>
+        <v>234</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>272</v>
+        <v>24</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>1107</v>
+        <v>1119</v>
       </c>
       <c r="F6" s="2">
-        <v>46048.33333333333</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1108</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>1109</v>
-      </c>
-      <c r="F7" s="2">
-        <v>46045.603472222225</v>
+        <v>46048.79027777778</v>
       </c>
     </row>
   </sheetData>
@@ -12941,7 +13077,6 @@
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
     <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-28 12:23
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2202" uniqueCount="1120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2212" uniqueCount="1125">
   <si>
     <t>link</t>
   </si>
@@ -3378,6 +3378,21 @@
   </si>
   <si>
     <t>6860 008 0094</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/jersikas-pag/fpncc.html</t>
+  </si>
+  <si>
+    <t>7652 004 0129</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/saldus-and-reg/zvardes-pag/kjfkn.html</t>
+  </si>
+  <si>
+    <t>89 000 €</t>
+  </si>
+  <si>
+    <t>84980020059</t>
   </si>
 </sst>
 </file>
@@ -3790,7 +3805,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F434"/>
+  <dimension ref="A1:F439"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -12485,6 +12500,106 @@
       </c>
       <c r="F434" s="2">
         <v>46045.603472222225</v>
+      </c>
+    </row>
+    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A435" s="3" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B435" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C435" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D435" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E435" s="4" t="s">
+        <v>1111</v>
+      </c>
+      <c r="F435" s="2">
+        <v>46049.521527777775</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A436" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B436" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C436" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D436" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E436" s="4" t="s">
+        <v>1113</v>
+      </c>
+      <c r="F436" s="2">
+        <v>46049.433333333334</v>
+      </c>
+    </row>
+    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A437" s="3" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B437" s="4" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C437" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D437" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E437" s="4" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F437" s="2">
+        <v>46048.88333333333</v>
+      </c>
+    </row>
+    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A438" s="3" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B438" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C438" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D438" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E438" s="4" t="s">
+        <v>994</v>
+      </c>
+      <c r="F438" s="2">
+        <v>46048.799305555556</v>
+      </c>
+    </row>
+    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A439" s="3" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B439" s="4" t="s">
+        <v>781</v>
+      </c>
+      <c r="C439" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D439" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E439" s="4" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F439" s="2">
+        <v>46048.79027777778</v>
       </c>
     </row>
   </sheetData>
@@ -12922,6 +13037,11 @@
     <hyperlink ref="A432" r:id="rId431"/>
     <hyperlink ref="A433" r:id="rId432"/>
     <hyperlink ref="A434" r:id="rId433"/>
+    <hyperlink ref="A435" r:id="rId434"/>
+    <hyperlink ref="A436" r:id="rId435"/>
+    <hyperlink ref="A437" r:id="rId436"/>
+    <hyperlink ref="A438" r:id="rId437"/>
+    <hyperlink ref="A439" r:id="rId438"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -12933,7 +13053,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -12972,111 +13092,48 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1110</v>
+        <v>1120</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>70</v>
+        <v>334</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>284</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>71</v>
+        <v>930</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1111</v>
+        <v>1121</v>
       </c>
       <c r="F2" s="2">
-        <v>46049.521527777775</v>
+        <v>46050.56597222222</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1112</v>
+        <v>1122</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>131</v>
+        <v>1123</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>28</v>
+        <v>346</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1113</v>
+        <v>1124</v>
       </c>
       <c r="F3" s="2">
-        <v>46049.433333333334</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1114</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>1115</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>1116</v>
-      </c>
-      <c r="F4" s="2">
-        <v>46048.88333333333</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>1117</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>994</v>
-      </c>
-      <c r="F5" s="2">
-        <v>46048.799305555556</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>1118</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>781</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>1119</v>
-      </c>
-      <c r="F6" s="2">
-        <v>46048.79027777778</v>
+        <v>46050.527083333334</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-29 12:29
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2212" uniqueCount="1125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2242" uniqueCount="1141">
   <si>
     <t>link</t>
   </si>
@@ -3393,6 +3393,54 @@
   </si>
   <si>
     <t>84980020059</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/lazdukalna-pag/gboid.html</t>
+  </si>
+  <si>
+    <t>38640090004</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/bauska-and-reg/iecavas-nov/mbgnx.html</t>
+  </si>
+  <si>
+    <t>40640110604</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/salienas-pag/ojhkp.html</t>
+  </si>
+  <si>
+    <t>12 800 €</t>
+  </si>
+  <si>
+    <t>44840040659</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/gulbene-and-reg/belavas-pag/bxxehb.html</t>
+  </si>
+  <si>
+    <t>50440070082</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/gulbene-and-reg/belavas-pag/injkh.html</t>
+  </si>
+  <si>
+    <t>43 ha.</t>
+  </si>
+  <si>
+    <t>50440060014</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/rusonas-pag/ixeng.html</t>
+  </si>
+  <si>
+    <t>211 000 €</t>
+  </si>
+  <si>
+    <t>91 ha.</t>
+  </si>
+  <si>
+    <t>7670 011 0032 011 00</t>
   </si>
 </sst>
 </file>
@@ -3805,7 +3853,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F439"/>
+  <dimension ref="A1:F441"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -12600,6 +12648,46 @@
       </c>
       <c r="F439" s="2">
         <v>46048.79027777778</v>
+      </c>
+    </row>
+    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A440" s="3" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B440" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C440" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D440" s="4" t="s">
+        <v>930</v>
+      </c>
+      <c r="E440" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="F440" s="2">
+        <v>46050.56597222222</v>
+      </c>
+    </row>
+    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A441" s="3" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B441" s="4" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C441" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D441" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E441" s="4" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F441" s="2">
+        <v>46050.527083333334</v>
       </c>
     </row>
   </sheetData>
@@ -13042,6 +13130,8 @@
     <hyperlink ref="A437" r:id="rId436"/>
     <hyperlink ref="A438" r:id="rId437"/>
     <hyperlink ref="A439" r:id="rId438"/>
+    <hyperlink ref="A440" r:id="rId439"/>
+    <hyperlink ref="A441" r:id="rId440"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -13053,7 +13143,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -13092,48 +13182,132 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1120</v>
+        <v>1125</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>334</v>
+        <v>131</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>284</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>930</v>
+        <v>186</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1121</v>
+        <v>1126</v>
       </c>
       <c r="F2" s="2">
-        <v>46050.56597222222</v>
+        <v>46050.70763888889</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1122</v>
+        <v>1127</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1123</v>
+        <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>346</v>
+        <v>48</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1124</v>
+        <v>1128</v>
       </c>
       <c r="F3" s="2">
-        <v>46050.527083333334</v>
+        <v>46051.54236111111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>1131</v>
+      </c>
+      <c r="F4" s="2">
+        <v>46050.72222222222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F5" s="2">
+        <v>46050.71736111111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F6" s="2">
+        <v>46050.70972222222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F7" s="2">
+        <v>46051.17083333334</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-01-30 12:27
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2242" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2272" uniqueCount="1154">
   <si>
     <t>link</t>
   </si>
@@ -3441,6 +3441,45 @@
   </si>
   <si>
     <t>7670 011 0032 011 00</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/stalbes-pag/hkpmm.html</t>
+  </si>
+  <si>
+    <t>42800050052</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/zosenu-pag/chebn.html</t>
+  </si>
+  <si>
+    <t>39 900 €</t>
+  </si>
+  <si>
+    <t>42980020111</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/bebrenes-pag/hljhk.html</t>
+  </si>
+  <si>
+    <t>1.51 ha.</t>
+  </si>
+  <si>
+    <t>44440020017</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kalniesu-pag/bebfkn.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/indras-pag/beplxd.html</t>
+  </si>
+  <si>
+    <t>6062002037</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/silmalas-pag/ljeii.html</t>
+  </si>
+  <si>
+    <t>78880010003</t>
   </si>
 </sst>
 </file>
@@ -3853,7 +3892,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F441"/>
+  <dimension ref="A1:F447"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -12688,6 +12727,126 @@
       </c>
       <c r="F441" s="2">
         <v>46050.527083333334</v>
+      </c>
+    </row>
+    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A442" s="3" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B442" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C442" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D442" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E442" s="4" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F442" s="2">
+        <v>46050.70763888889</v>
+      </c>
+    </row>
+    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A443" s="3" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B443" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C443" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D443" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E443" s="4" t="s">
+        <v>1128</v>
+      </c>
+      <c r="F443" s="2">
+        <v>46051.54236111111</v>
+      </c>
+    </row>
+    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A444" s="3" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B444" s="4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C444" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D444" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E444" s="4" t="s">
+        <v>1131</v>
+      </c>
+      <c r="F444" s="2">
+        <v>46050.72222222222</v>
+      </c>
+    </row>
+    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A445" s="3" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B445" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C445" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D445" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E445" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F445" s="2">
+        <v>46050.71736111111</v>
+      </c>
+    </row>
+    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A446" s="3" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B446" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="C446" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D446" s="4" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E446" s="4" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F446" s="2">
+        <v>46050.70972222222</v>
+      </c>
+    </row>
+    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A447" s="3" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B447" s="4" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C447" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D447" s="4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E447" s="4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F447" s="2">
+        <v>46051.17083333334</v>
       </c>
     </row>
   </sheetData>
@@ -13132,6 +13291,12 @@
     <hyperlink ref="A439" r:id="rId438"/>
     <hyperlink ref="A440" r:id="rId439"/>
     <hyperlink ref="A441" r:id="rId440"/>
+    <hyperlink ref="A442" r:id="rId441"/>
+    <hyperlink ref="A443" r:id="rId442"/>
+    <hyperlink ref="A444" r:id="rId443"/>
+    <hyperlink ref="A445" r:id="rId444"/>
+    <hyperlink ref="A446" r:id="rId445"/>
+    <hyperlink ref="A447" r:id="rId446"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -13182,122 +13347,122 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1125</v>
+        <v>1141</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>131</v>
+        <v>650</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>186</v>
+        <v>85</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1126</v>
+        <v>1142</v>
       </c>
       <c r="F2" s="2">
-        <v>46050.70763888889</v>
+        <v>46051.91736111111</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1127</v>
+        <v>1143</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>1144</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1128</v>
+        <v>1145</v>
       </c>
       <c r="F3" s="2">
-        <v>46051.54236111111</v>
+        <v>46051.81597222222</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1129</v>
+        <v>1146</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1130</v>
+        <v>1075</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>272</v>
+        <v>1147</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>1131</v>
+        <v>1148</v>
       </c>
       <c r="F4" s="2">
-        <v>46050.72222222222</v>
+        <v>46051.76666666666</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1132</v>
+        <v>1149</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>211</v>
+        <v>549</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>1133</v>
+        <v>550</v>
       </c>
       <c r="F5" s="2">
-        <v>46050.71736111111</v>
+        <v>46051.6375</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1134</v>
+        <v>1150</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>599</v>
+        <v>368</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>1135</v>
+        <v>36</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>1136</v>
+        <v>1151</v>
       </c>
       <c r="F6" s="2">
-        <v>46050.70972222222</v>
+        <v>46051.61944444444</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>1137</v>
+        <v>1152</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1138</v>
+        <v>204</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>1139</v>
+        <v>59</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>1140</v>
+        <v>1153</v>
       </c>
       <c r="F7" s="2">
-        <v>46051.17083333334</v>
+        <v>46051.61597222222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update forest data - 2026-02-02 12:30
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2272" uniqueCount="1154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2307" uniqueCount="1170">
   <si>
     <t>link</t>
   </si>
@@ -3480,6 +3480,54 @@
   </si>
   <si>
     <t>78880010003</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aizkraukle-and-reg/plavinas/mfgbj.html</t>
+  </si>
+  <si>
+    <t>32420090035</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aluksne-and-reg/jaunaluksnes-pag/inghf.html</t>
+  </si>
+  <si>
+    <t>36560130028</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/izvaltas-pag/hmlmn.html</t>
+  </si>
+  <si>
+    <t>60640020120</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kuldiga-and-reg/kurmales-pag/chgio.html</t>
+  </si>
+  <si>
+    <t>13 900 €</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/blontu-pag/dioce.html</t>
+  </si>
+  <si>
+    <t>41 000 €</t>
+  </si>
+  <si>
+    <t>68440050028</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ogre-and-reg/lielvardes-l-t/lhlxf.html</t>
+  </si>
+  <si>
+    <t>74840070028</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/saldus-and-reg/saldus/kgkjn.html</t>
+  </si>
+  <si>
+    <t>1.35 ha.</t>
+  </si>
+  <si>
+    <t>84480060140</t>
   </si>
 </sst>
 </file>
@@ -3892,7 +3940,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F447"/>
+  <dimension ref="A1:F453"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -12847,6 +12895,126 @@
       </c>
       <c r="F447" s="2">
         <v>46051.17083333334</v>
+      </c>
+    </row>
+    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A448" s="3" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B448" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="C448" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D448" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E448" s="4" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F448" s="2">
+        <v>46051.91736111111</v>
+      </c>
+    </row>
+    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A449" s="3" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B449" s="4" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C449" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D449" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E449" s="4" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F449" s="2">
+        <v>46051.81597222222</v>
+      </c>
+    </row>
+    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A450" s="3" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B450" s="4" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C450" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D450" s="4" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E450" s="4" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F450" s="2">
+        <v>46051.76666666666</v>
+      </c>
+    </row>
+    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A451" s="3" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B451" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="C451" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D451" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E451" s="4" t="s">
+        <v>550</v>
+      </c>
+      <c r="F451" s="2">
+        <v>46051.6375</v>
+      </c>
+    </row>
+    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A452" s="3" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B452" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="C452" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D452" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E452" s="4" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F452" s="2">
+        <v>46051.61944444444</v>
+      </c>
+    </row>
+    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A453" s="3" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B453" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C453" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D453" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E453" s="4" t="s">
+        <v>1153</v>
+      </c>
+      <c r="F453" s="2">
+        <v>46051.61597222222</v>
       </c>
     </row>
   </sheetData>
@@ -13297,6 +13465,12 @@
     <hyperlink ref="A445" r:id="rId444"/>
     <hyperlink ref="A446" r:id="rId445"/>
     <hyperlink ref="A447" r:id="rId446"/>
+    <hyperlink ref="A448" r:id="rId447"/>
+    <hyperlink ref="A449" r:id="rId448"/>
+    <hyperlink ref="A450" r:id="rId449"/>
+    <hyperlink ref="A451" r:id="rId450"/>
+    <hyperlink ref="A452" r:id="rId451"/>
+    <hyperlink ref="A453" r:id="rId452"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -13308,7 +13482,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -13347,122 +13521,142 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1141</v>
+        <v>1154</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>650</v>
+        <v>576</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>85</v>
+        <v>272</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1142</v>
+        <v>1155</v>
       </c>
       <c r="F2" s="2">
-        <v>46051.91736111111</v>
+        <v>46055.46388888889</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1143</v>
+        <v>1156</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1144</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>63</v>
+        <v>435</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1145</v>
+        <v>1157</v>
       </c>
       <c r="F3" s="2">
-        <v>46051.81597222222</v>
+        <v>46055.36041666666</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1146</v>
+        <v>1158</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1075</v>
+        <v>437</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>74</v>
+        <v>146</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>1147</v>
+        <v>169</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>1148</v>
+        <v>1159</v>
       </c>
       <c r="F4" s="2">
-        <v>46051.76666666666</v>
+        <v>46054.705555555556</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1149</v>
+        <v>1160</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>549</v>
+        <v>1161</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>146</v>
+        <v>424</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>75</v>
+        <v>186</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>550</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2">
-        <v>46051.6375</v>
+        <v>46054.82986111111</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1150</v>
+        <v>1162</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>368</v>
+        <v>1163</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>146</v>
+        <v>234</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>1151</v>
+        <v>1164</v>
       </c>
       <c r="F6" s="2">
-        <v>46051.61944444444</v>
+        <v>46052.674305555556</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>1152</v>
+        <v>1165</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>1153</v>
+        <v>1166</v>
       </c>
       <c r="F7" s="2">
-        <v>46051.61597222222</v>
+        <v>46053.77916666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F8" s="2">
+        <v>46055.40763888889</v>
       </c>
     </row>
   </sheetData>
@@ -13473,6 +13667,7 @@
     <hyperlink ref="A5" r:id="rId4"/>
     <hyperlink ref="A6" r:id="rId5"/>
     <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-02-03 12:31
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2307" uniqueCount="1170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2342" uniqueCount="1187">
   <si>
     <t>link</t>
   </si>
@@ -3528,6 +3528,57 @@
   </si>
   <si>
     <t>84480060140</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/bauska-and-reg/vecsaules-pag/kffcn.html</t>
+  </si>
+  <si>
+    <t>40920090234</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/cesis-and-reg/cesis/cxhdf.html</t>
+  </si>
+  <si>
+    <t>42460060005</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/upmalas-pag/bhhlnf.html</t>
+  </si>
+  <si>
+    <t>76900060029</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/dricanu-pag/jhdxd.html</t>
+  </si>
+  <si>
+    <t>4.70 ha.</t>
+  </si>
+  <si>
+    <t>78500020015</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/veremu-pag/bgglm.html</t>
+  </si>
+  <si>
+    <t>8.40 ha.</t>
+  </si>
+  <si>
+    <t>78960030042</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/valka-and-reg/smiltene/piixf.html</t>
+  </si>
+  <si>
+    <t>0.25 ha.</t>
+  </si>
+  <si>
+    <t>94480020026</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/other/hjkix.html</t>
+  </si>
+  <si>
+    <t>42660060086</t>
   </si>
 </sst>
 </file>
@@ -3940,7 +3991,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F453"/>
+  <dimension ref="A1:F460"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -13015,6 +13066,146 @@
       </c>
       <c r="F453" s="2">
         <v>46051.61597222222</v>
+      </c>
+    </row>
+    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A454" s="3" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B454" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C454" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D454" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E454" s="4" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F454" s="2">
+        <v>46055.46388888889</v>
+      </c>
+    </row>
+    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A455" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B455" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C455" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D455" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E455" s="4" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F455" s="2">
+        <v>46055.36041666666</v>
+      </c>
+    </row>
+    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A456" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B456" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="C456" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D456" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E456" s="4" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F456" s="2">
+        <v>46054.705555555556</v>
+      </c>
+    </row>
+    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A457" s="3" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B457" s="4" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C457" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D457" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E457" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F457" s="2">
+        <v>46054.82986111111</v>
+      </c>
+    </row>
+    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A458" s="3" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B458" s="4" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C458" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D458" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E458" s="4" t="s">
+        <v>1164</v>
+      </c>
+      <c r="F458" s="2">
+        <v>46052.674305555556</v>
+      </c>
+    </row>
+    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A459" s="3" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B459" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C459" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D459" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E459" s="4" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F459" s="2">
+        <v>46053.77916666667</v>
+      </c>
+    </row>
+    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A460" s="3" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B460" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C460" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D460" s="4" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E460" s="4" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F460" s="2">
+        <v>46055.40763888889</v>
       </c>
     </row>
   </sheetData>
@@ -13471,6 +13662,13 @@
     <hyperlink ref="A451" r:id="rId450"/>
     <hyperlink ref="A452" r:id="rId451"/>
     <hyperlink ref="A453" r:id="rId452"/>
+    <hyperlink ref="A454" r:id="rId453"/>
+    <hyperlink ref="A455" r:id="rId454"/>
+    <hyperlink ref="A456" r:id="rId455"/>
+    <hyperlink ref="A457" r:id="rId456"/>
+    <hyperlink ref="A458" r:id="rId457"/>
+    <hyperlink ref="A459" r:id="rId458"/>
+    <hyperlink ref="A460" r:id="rId459"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -13521,142 +13719,142 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1154</v>
+        <v>1170</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>576</v>
+        <v>414</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>272</v>
+        <v>82</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1155</v>
+        <v>1171</v>
       </c>
       <c r="F2" s="2">
-        <v>46055.46388888889</v>
+        <v>46056.336111111115</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1156</v>
+        <v>1172</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>435</v>
+        <v>63</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>94</v>
+        <v>272</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1157</v>
+        <v>1173</v>
       </c>
       <c r="F3" s="2">
-        <v>46055.36041666666</v>
+        <v>46056.475694444445</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1158</v>
+        <v>1174</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>437</v>
+        <v>290</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>146</v>
+        <v>284</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>169</v>
+        <v>24</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>1159</v>
+        <v>1175</v>
       </c>
       <c r="F4" s="2">
-        <v>46054.705555555556</v>
+        <v>46055.675</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1160</v>
+        <v>1176</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1161</v>
+        <v>150</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>424</v>
+        <v>294</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>186</v>
+        <v>1177</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>25</v>
+        <v>1178</v>
       </c>
       <c r="F5" s="2">
-        <v>46054.82986111111</v>
+        <v>46056.495833333334</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1162</v>
+        <v>1179</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1163</v>
+        <v>88</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>234</v>
+        <v>294</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>82</v>
+        <v>1180</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>1164</v>
+        <v>1181</v>
       </c>
       <c r="F6" s="2">
-        <v>46052.674305555556</v>
+        <v>46055.882638888885</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>1165</v>
+        <v>1182</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>174</v>
+        <v>1075</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>275</v>
+        <v>392</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>75</v>
+        <v>1183</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>1166</v>
+        <v>1184</v>
       </c>
       <c r="F7" s="2">
-        <v>46053.77916666667</v>
+        <v>46056.513194444444</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>1167</v>
+        <v>1185</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>576</v>
+        <v>414</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>346</v>
+        <v>25</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>1168</v>
+        <v>82</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>1169</v>
+        <v>1186</v>
       </c>
       <c r="F8" s="2">
-        <v>46055.40763888889</v>
+        <v>46056.30208333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update forest data - 2026-02-04 12:31
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2342" uniqueCount="1187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2357" uniqueCount="1197">
   <si>
     <t>link</t>
   </si>
@@ -3579,6 +3579,36 @@
   </si>
   <si>
     <t>42660060086</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aizkraukle-and-reg/daudzeses-pag/jfbgx.html</t>
+  </si>
+  <si>
+    <t>107 000 €</t>
+  </si>
+  <si>
+    <t>9.44 ha.</t>
+  </si>
+  <si>
+    <t>32500090004</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/aloja/copmo.html</t>
+  </si>
+  <si>
+    <t>12.40 ha.</t>
+  </si>
+  <si>
+    <t>66270040050</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/pelecu-pag/bxolie.html</t>
+  </si>
+  <si>
+    <t>2.82 ha.</t>
+  </si>
+  <si>
+    <t>76560050295</t>
   </si>
 </sst>
 </file>
@@ -3991,7 +4021,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F460"/>
+  <dimension ref="A1:F467"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -13206,6 +13236,146 @@
       </c>
       <c r="F460" s="2">
         <v>46055.40763888889</v>
+      </c>
+    </row>
+    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A461" s="3" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B461" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="C461" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D461" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E461" s="4" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F461" s="2">
+        <v>46056.336111111115</v>
+      </c>
+    </row>
+    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A462" s="3" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B462" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C462" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D462" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E462" s="4" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F462" s="2">
+        <v>46056.475694444445</v>
+      </c>
+    </row>
+    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A463" s="3" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B463" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C463" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D463" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E463" s="4" t="s">
+        <v>1175</v>
+      </c>
+      <c r="F463" s="2">
+        <v>46055.675</v>
+      </c>
+    </row>
+    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A464" s="3" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B464" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C464" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D464" s="4" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E464" s="4" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F464" s="2">
+        <v>46056.495833333334</v>
+      </c>
+    </row>
+    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A465" s="3" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B465" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C465" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D465" s="4" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E465" s="4" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F465" s="2">
+        <v>46055.882638888885</v>
+      </c>
+    </row>
+    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A466" s="3" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B466" s="4" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C466" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D466" s="4" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E466" s="4" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F466" s="2">
+        <v>46056.513194444444</v>
+      </c>
+    </row>
+    <row r="467" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A467" s="3" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B467" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="C467" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D467" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E467" s="4" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F467" s="2">
+        <v>46056.30208333333</v>
       </c>
     </row>
   </sheetData>
@@ -13669,6 +13839,13 @@
     <hyperlink ref="A458" r:id="rId457"/>
     <hyperlink ref="A459" r:id="rId458"/>
     <hyperlink ref="A460" r:id="rId459"/>
+    <hyperlink ref="A461" r:id="rId460"/>
+    <hyperlink ref="A462" r:id="rId461"/>
+    <hyperlink ref="A463" r:id="rId462"/>
+    <hyperlink ref="A464" r:id="rId463"/>
+    <hyperlink ref="A465" r:id="rId464"/>
+    <hyperlink ref="A466" r:id="rId465"/>
+    <hyperlink ref="A467" r:id="rId466"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -13680,7 +13857,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -13719,142 +13896,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1170</v>
+        <v>1187</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>414</v>
+        <v>1188</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>82</v>
+        <v>1189</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1171</v>
+        <v>1190</v>
       </c>
       <c r="F2" s="2">
-        <v>46056.336111111115</v>
+        <v>46056.825</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1172</v>
+        <v>1191</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>39</v>
+        <v>274</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>63</v>
+        <v>208</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>272</v>
+        <v>1192</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1173</v>
+        <v>1193</v>
       </c>
       <c r="F3" s="2">
-        <v>46056.475694444445</v>
+        <v>46057.47916666667</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1174</v>
+        <v>1194</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>290</v>
+        <v>116</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>284</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>24</v>
+        <v>1195</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>1175</v>
+        <v>1196</v>
       </c>
       <c r="F4" s="2">
-        <v>46055.675</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>1176</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>1177</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>1178</v>
-      </c>
-      <c r="F5" s="2">
-        <v>46056.495833333334</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>1179</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>1180</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>1181</v>
-      </c>
-      <c r="F6" s="2">
-        <v>46055.882638888885</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1182</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>1075</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>1183</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>1184</v>
-      </c>
-      <c r="F7" s="2">
-        <v>46056.513194444444</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>1185</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>414</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>1186</v>
-      </c>
-      <c r="F8" s="2">
-        <v>46056.30208333333</v>
+        <v>46057.58125</v>
       </c>
     </row>
   </sheetData>
@@ -13862,10 +13959,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-02-05 12:32
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2357" uniqueCount="1197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2367" uniqueCount="1201">
   <si>
     <t>link</t>
   </si>
@@ -3609,6 +3609,18 @@
   </si>
   <si>
     <t>76560050295</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/gulbene-and-reg/gulbene/ggxmf.html</t>
+  </si>
+  <si>
+    <t>50440140001</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/zalesjes-pag/bmhjim.html</t>
+  </si>
+  <si>
+    <t>68960050098</t>
   </si>
 </sst>
 </file>
@@ -4021,7 +4033,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F467"/>
+  <dimension ref="A1:F470"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -13376,6 +13388,66 @@
       </c>
       <c r="F467" s="2">
         <v>46056.30208333333</v>
+      </c>
+    </row>
+    <row r="468" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A468" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B468" s="4" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C468" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D468" s="4" t="s">
+        <v>1189</v>
+      </c>
+      <c r="E468" s="4" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F468" s="2">
+        <v>46056.825</v>
+      </c>
+    </row>
+    <row r="469" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A469" s="3" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B469" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C469" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D469" s="4" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E469" s="4" t="s">
+        <v>1193</v>
+      </c>
+      <c r="F469" s="2">
+        <v>46057.47916666667</v>
+      </c>
+    </row>
+    <row r="470" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A470" s="3" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B470" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C470" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D470" s="4" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E470" s="4" t="s">
+        <v>1196</v>
+      </c>
+      <c r="F470" s="2">
+        <v>46057.58125</v>
       </c>
     </row>
   </sheetData>
@@ -13846,6 +13918,9 @@
     <hyperlink ref="A465" r:id="rId464"/>
     <hyperlink ref="A466" r:id="rId465"/>
     <hyperlink ref="A467" r:id="rId466"/>
+    <hyperlink ref="A468" r:id="rId467"/>
+    <hyperlink ref="A469" r:id="rId468"/>
+    <hyperlink ref="A470" r:id="rId469"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -13857,7 +13932,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -13896,69 +13971,48 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1187</v>
+        <v>1197</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1188</v>
+        <v>307</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>124</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1189</v>
+        <v>186</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1190</v>
+        <v>1198</v>
       </c>
       <c r="F2" s="2">
-        <v>46056.825</v>
+        <v>46058.45763888889</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1191</v>
+        <v>1199</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>274</v>
+        <v>246</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>1192</v>
+        <v>32</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1193</v>
+        <v>1200</v>
       </c>
       <c r="F3" s="2">
-        <v>46057.47916666667</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1194</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>1195</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>1196</v>
-      </c>
-      <c r="F4" s="2">
-        <v>46057.58125</v>
+        <v>46058.49097222222</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-02-06 12:30
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2367" uniqueCount="1201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2392" uniqueCount="1211">
   <si>
     <t>link</t>
   </si>
@@ -3621,6 +3621,36 @@
   </si>
   <si>
     <t>68960050098</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/liepaja-and-reg/dunikas-pag/bljip.html</t>
+  </si>
+  <si>
+    <t>6 400 €</t>
+  </si>
+  <si>
+    <t>64520050033</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/katvaru-pag/blfig.html</t>
+  </si>
+  <si>
+    <t>6652 006 0004</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/sarkanu-pag/idpic.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/sakstagala-pag/fdlph.html</t>
+  </si>
+  <si>
+    <t>78860020157</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/valka-and-reg/planu-pag/ooflx.html</t>
+  </si>
+  <si>
+    <t>94760120100</t>
   </si>
 </sst>
 </file>
@@ -4033,7 +4063,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F470"/>
+  <dimension ref="A1:F472"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -13448,6 +13478,46 @@
       </c>
       <c r="F470" s="2">
         <v>46057.58125</v>
+      </c>
+    </row>
+    <row r="471" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A471" s="3" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B471" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C471" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D471" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E471" s="4" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F471" s="2">
+        <v>46058.45763888889</v>
+      </c>
+    </row>
+    <row r="472" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A472" s="3" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B472" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C472" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D472" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E472" s="4" t="s">
+        <v>1200</v>
+      </c>
+      <c r="F472" s="2">
+        <v>46058.49097222222</v>
       </c>
     </row>
   </sheetData>
@@ -13921,6 +13991,8 @@
     <hyperlink ref="A468" r:id="rId467"/>
     <hyperlink ref="A469" r:id="rId468"/>
     <hyperlink ref="A470" r:id="rId469"/>
+    <hyperlink ref="A471" r:id="rId470"/>
+    <hyperlink ref="A472" r:id="rId471"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -13932,7 +14004,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -13971,48 +14043,111 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1197</v>
+        <v>1201</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>307</v>
+        <v>1202</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>124</v>
+        <v>190</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>186</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1198</v>
+        <v>1203</v>
       </c>
       <c r="F2" s="2">
-        <v>46058.45763888889</v>
+        <v>46059.478472222225</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1199</v>
+        <v>1204</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>246</v>
+        <v>268</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>234</v>
+        <v>208</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1200</v>
+        <v>1205</v>
       </c>
       <c r="F3" s="2">
-        <v>46058.49097222222</v>
+        <v>46059.490277777775</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="F4" s="2">
+        <v>46058.90486111111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F5" s="2">
+        <v>46058.62291666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>1210</v>
+      </c>
+      <c r="F6" s="2">
+        <v>46059.51666666666</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-02-09 12:39
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2392" uniqueCount="1211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2427" uniqueCount="1227">
   <si>
     <t>link</t>
   </si>
@@ -3651,6 +3651,54 @@
   </si>
   <si>
     <t>94760120100</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/dobele-and-reg/iles-pag/ddbij.html</t>
+  </si>
+  <si>
+    <t>46640030057</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kuldiga-and-reg/ivandes-pag/hibnf.html</t>
+  </si>
+  <si>
+    <t>62540020101</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/limbadzi-and-reg/vilkenes-pag/anfhd.html</t>
+  </si>
+  <si>
+    <t>66880080087</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/rundenu-pag/mjejj.html</t>
+  </si>
+  <si>
+    <t>68920070032</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/pasienes-pag/knxof.html</t>
+  </si>
+  <si>
+    <t>68840010017</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/sausnejas-pag/hjfch.html</t>
+  </si>
+  <si>
+    <t>105 200 €</t>
+  </si>
+  <si>
+    <t>26.30 ha.</t>
+  </si>
+  <si>
+    <t>70920080064</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ogre-and-reg/mengeles-pag/lpixx.html</t>
+  </si>
+  <si>
+    <t>74760030145</t>
   </si>
 </sst>
 </file>
@@ -4063,7 +4111,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F472"/>
+  <dimension ref="A1:F477"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -13518,6 +13566,106 @@
       </c>
       <c r="F472" s="2">
         <v>46058.49097222222</v>
+      </c>
+    </row>
+    <row r="473" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A473" s="3" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B473" s="4" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C473" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D473" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E473" s="4" t="s">
+        <v>1203</v>
+      </c>
+      <c r="F473" s="2">
+        <v>46059.478472222225</v>
+      </c>
+    </row>
+    <row r="474" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A474" s="3" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B474" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C474" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D474" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E474" s="4" t="s">
+        <v>1205</v>
+      </c>
+      <c r="F474" s="2">
+        <v>46059.490277777775</v>
+      </c>
+    </row>
+    <row r="475" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A475" s="3" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B475" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C475" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D475" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E475" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="F475" s="2">
+        <v>46058.90486111111</v>
+      </c>
+    </row>
+    <row r="476" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A476" s="3" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B476" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C476" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D476" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E476" s="4" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F476" s="2">
+        <v>46058.62291666667</v>
+      </c>
+    </row>
+    <row r="477" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A477" s="3" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B477" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C477" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D477" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E477" s="4" t="s">
+        <v>1210</v>
+      </c>
+      <c r="F477" s="2">
+        <v>46059.51666666666</v>
       </c>
     </row>
   </sheetData>
@@ -13993,6 +14141,11 @@
     <hyperlink ref="A470" r:id="rId469"/>
     <hyperlink ref="A471" r:id="rId470"/>
     <hyperlink ref="A472" r:id="rId471"/>
+    <hyperlink ref="A473" r:id="rId472"/>
+    <hyperlink ref="A474" r:id="rId473"/>
+    <hyperlink ref="A475" r:id="rId474"/>
+    <hyperlink ref="A476" r:id="rId475"/>
+    <hyperlink ref="A477" r:id="rId476"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -14004,7 +14157,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -14043,102 +14196,142 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1201</v>
+        <v>1211</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1202</v>
+        <v>116</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>190</v>
+        <v>117</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>186</v>
+        <v>82</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1203</v>
+        <v>1212</v>
       </c>
       <c r="F2" s="2">
-        <v>46059.478472222225</v>
+        <v>46062.60277777778</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1204</v>
+        <v>1213</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>268</v>
+        <v>70</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>208</v>
+        <v>424</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1205</v>
+        <v>1214</v>
       </c>
       <c r="F3" s="2">
-        <v>46059.490277777775</v>
+        <v>46061.79652777778</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1206</v>
+        <v>1215</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>268</v>
+        <v>629</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>256</v>
+        <v>208</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>433</v>
+        <v>1216</v>
       </c>
       <c r="F4" s="2">
-        <v>46058.90486111111</v>
+        <v>46060.64583333333</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1207</v>
+        <v>1217</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>116</v>
+        <v>461</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>294</v>
+        <v>234</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>36</v>
+        <v>903</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>1208</v>
+        <v>1218</v>
       </c>
       <c r="F5" s="2">
-        <v>46058.62291666667</v>
+        <v>46062.361805555556</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1209</v>
+        <v>1219</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>91</v>
+        <v>290</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>392</v>
+        <v>234</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>1210</v>
+        <v>1220</v>
       </c>
       <c r="F6" s="2">
-        <v>46059.51666666666</v>
+        <v>46061.39236111111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>1223</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F7" s="2">
+        <v>46062.375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F8" s="2">
+        <v>46060.48819444445</v>
       </c>
     </row>
   </sheetData>
@@ -14148,6 +14341,8 @@
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
     <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-02-10 12:42
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2427" uniqueCount="1227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2447" uniqueCount="1240">
   <si>
     <t>link</t>
   </si>
@@ -3699,6 +3699,45 @@
   </si>
   <si>
     <t>74760030145</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/sokolku-pag/nlfdl.html</t>
+  </si>
+  <si>
+    <t>2 800 €</t>
+  </si>
+  <si>
+    <t>1.12 ha.</t>
+  </si>
+  <si>
+    <t>78900020063</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/ozolaines-pag/bncjm.html</t>
+  </si>
+  <si>
+    <t>3 600 €</t>
+  </si>
+  <si>
+    <t>1.21 ha.</t>
+  </si>
+  <si>
+    <t>78760030189</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/nautrenu-pag/igeho.html</t>
+  </si>
+  <si>
+    <t>11.55 ha.</t>
+  </si>
+  <si>
+    <t>68740050088</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/tukums-and-reg/slampes-pag/ndbim.html</t>
+  </si>
+  <si>
+    <t>90800030014</t>
   </si>
 </sst>
 </file>
@@ -4111,7 +4150,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F477"/>
+  <dimension ref="A1:F484"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -13666,6 +13705,146 @@
       </c>
       <c r="F477" s="2">
         <v>46059.51666666666</v>
+      </c>
+    </row>
+    <row r="478" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A478" s="3" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B478" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C478" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D478" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E478" s="4" t="s">
+        <v>1212</v>
+      </c>
+      <c r="F478" s="2">
+        <v>46062.60277777778</v>
+      </c>
+    </row>
+    <row r="479" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A479" s="3" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B479" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C479" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D479" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E479" s="4" t="s">
+        <v>1214</v>
+      </c>
+      <c r="F479" s="2">
+        <v>46061.79652777778</v>
+      </c>
+    </row>
+    <row r="480" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A480" s="3" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B480" s="4" t="s">
+        <v>629</v>
+      </c>
+      <c r="C480" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D480" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E480" s="4" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F480" s="2">
+        <v>46060.64583333333</v>
+      </c>
+    </row>
+    <row r="481" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A481" s="3" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B481" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="C481" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D481" s="4" t="s">
+        <v>903</v>
+      </c>
+      <c r="E481" s="4" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F481" s="2">
+        <v>46062.361805555556</v>
+      </c>
+    </row>
+    <row r="482" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A482" s="3" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B482" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C482" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D482" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E482" s="4" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F482" s="2">
+        <v>46061.39236111111</v>
+      </c>
+    </row>
+    <row r="483" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A483" s="3" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B483" s="4" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C483" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D483" s="4" t="s">
+        <v>1223</v>
+      </c>
+      <c r="E483" s="4" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F483" s="2">
+        <v>46062.375</v>
+      </c>
+    </row>
+    <row r="484" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A484" s="3" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B484" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C484" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D484" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E484" s="4" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F484" s="2">
+        <v>46060.48819444445</v>
       </c>
     </row>
   </sheetData>
@@ -14146,6 +14325,13 @@
     <hyperlink ref="A475" r:id="rId474"/>
     <hyperlink ref="A476" r:id="rId475"/>
     <hyperlink ref="A477" r:id="rId476"/>
+    <hyperlink ref="A478" r:id="rId477"/>
+    <hyperlink ref="A479" r:id="rId478"/>
+    <hyperlink ref="A480" r:id="rId479"/>
+    <hyperlink ref="A481" r:id="rId480"/>
+    <hyperlink ref="A482" r:id="rId481"/>
+    <hyperlink ref="A483" r:id="rId482"/>
+    <hyperlink ref="A484" r:id="rId483"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -14157,7 +14343,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -14196,142 +14382,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1211</v>
+        <v>1227</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>116</v>
+        <v>1228</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>117</v>
+        <v>294</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>82</v>
+        <v>1229</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1212</v>
+        <v>1230</v>
       </c>
       <c r="F2" s="2">
-        <v>46062.60277777778</v>
+        <v>46063.59722222222</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1213</v>
+        <v>1231</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>70</v>
+        <v>1232</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>424</v>
+        <v>294</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>17</v>
+        <v>1233</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1214</v>
+        <v>1234</v>
       </c>
       <c r="F3" s="2">
-        <v>46061.79652777778</v>
+        <v>46063.57083333333</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1215</v>
+        <v>1235</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>629</v>
+        <v>274</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>208</v>
+        <v>294</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>13</v>
+        <v>1236</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>1216</v>
+        <v>1237</v>
       </c>
       <c r="F4" s="2">
-        <v>46060.64583333333</v>
+        <v>46063.51597222222</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1217</v>
+        <v>1238</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>461</v>
+        <v>271</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>234</v>
+        <v>376</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>903</v>
+        <v>36</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>1218</v>
+        <v>1239</v>
       </c>
       <c r="F5" s="2">
-        <v>46062.361805555556</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>1219</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>1220</v>
-      </c>
-      <c r="F6" s="2">
-        <v>46061.39236111111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1221</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>1222</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>1223</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>1224</v>
-      </c>
-      <c r="F7" s="2">
-        <v>46062.375</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>1226</v>
-      </c>
-      <c r="F8" s="2">
-        <v>46060.48819444445</v>
+        <v>46063.50555555556</v>
       </c>
     </row>
   </sheetData>
@@ -14340,9 +14466,6 @@
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-02-11 12:38
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2447" uniqueCount="1240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2482" uniqueCount="1260">
   <si>
     <t>link</t>
   </si>
@@ -3738,6 +3738,66 @@
   </si>
   <si>
     <t>90800030014</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/laucesas-pag/icdoc.html</t>
+  </si>
+  <si>
+    <t>4.45 ha.</t>
+  </si>
+  <si>
+    <t>44640020143</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/graveru-pag/mpcdk.html</t>
+  </si>
+  <si>
+    <t>4.63 ha.</t>
+  </si>
+  <si>
+    <t>60580020056</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kraslavas-pag/cgjgei.html</t>
+  </si>
+  <si>
+    <t>6.20 ha.</t>
+  </si>
+  <si>
+    <t>60780010301</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/andrupenes-pag/gdkbg.html</t>
+  </si>
+  <si>
+    <t>60420030037</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/udrisu-pag/ngipb.html</t>
+  </si>
+  <si>
+    <t>8.10 ha.</t>
+  </si>
+  <si>
+    <t>60960080289</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kombulu-pag/pbxmm.html</t>
+  </si>
+  <si>
+    <t>122 000 €</t>
+  </si>
+  <si>
+    <t>26.50 ha.</t>
+  </si>
+  <si>
+    <t>60740040533</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kombulu-pag/olnkj.html</t>
+  </si>
+  <si>
+    <t>2.90 ha.</t>
   </si>
 </sst>
 </file>
@@ -4150,7 +4210,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F484"/>
+  <dimension ref="A1:F488"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -13845,6 +13905,86 @@
       </c>
       <c r="F484" s="2">
         <v>46060.48819444445</v>
+      </c>
+    </row>
+    <row r="485" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A485" s="3" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B485" s="4" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C485" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D485" s="4" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E485" s="4" t="s">
+        <v>1230</v>
+      </c>
+      <c r="F485" s="2">
+        <v>46063.59722222222</v>
+      </c>
+    </row>
+    <row r="486" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A486" s="3" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B486" s="4" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C486" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D486" s="4" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E486" s="4" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F486" s="2">
+        <v>46063.57083333333</v>
+      </c>
+    </row>
+    <row r="487" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A487" s="3" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B487" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C487" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D487" s="4" t="s">
+        <v>1236</v>
+      </c>
+      <c r="E487" s="4" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F487" s="2">
+        <v>46063.51597222222</v>
+      </c>
+    </row>
+    <row r="488" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A488" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B488" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C488" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D488" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E488" s="4" t="s">
+        <v>1239</v>
+      </c>
+      <c r="F488" s="2">
+        <v>46063.50555555556</v>
       </c>
     </row>
   </sheetData>
@@ -14332,6 +14472,10 @@
     <hyperlink ref="A482" r:id="rId481"/>
     <hyperlink ref="A483" r:id="rId482"/>
     <hyperlink ref="A484" r:id="rId483"/>
+    <hyperlink ref="A485" r:id="rId484"/>
+    <hyperlink ref="A486" r:id="rId485"/>
+    <hyperlink ref="A487" r:id="rId486"/>
+    <hyperlink ref="A488" r:id="rId487"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -14343,7 +14487,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -14382,82 +14526,142 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1227</v>
+        <v>1240</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1228</v>
+        <v>793</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>294</v>
+        <v>74</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1229</v>
+        <v>1241</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1230</v>
+        <v>1242</v>
       </c>
       <c r="F2" s="2">
-        <v>46063.59722222222</v>
+        <v>46063.78958333333</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1231</v>
+        <v>1243</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1232</v>
+        <v>150</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>294</v>
+        <v>146</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>1233</v>
+        <v>1244</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1234</v>
+        <v>1245</v>
       </c>
       <c r="F3" s="2">
-        <v>46063.57083333333</v>
+        <v>46063.913888888885</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1235</v>
+        <v>1246</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>274</v>
+        <v>185</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>294</v>
+        <v>146</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>1236</v>
+        <v>1247</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>1237</v>
+        <v>1248</v>
       </c>
       <c r="F4" s="2">
-        <v>46063.51597222222</v>
+        <v>46063.85486111111</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1238</v>
+        <v>1249</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>271</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>376</v>
+        <v>146</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>36</v>
+        <v>930</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>1239</v>
+        <v>1250</v>
       </c>
       <c r="F5" s="2">
-        <v>46063.50555555556</v>
+        <v>46063.82083333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>1252</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>1253</v>
+      </c>
+      <c r="F6" s="2">
+        <v>46063.73055555555</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F7" s="2">
+        <v>46063.663194444445</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F8" s="2">
+        <v>46063.65555555555</v>
       </c>
     </row>
   </sheetData>
@@ -14466,6 +14670,9 @@
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-02-12 12:35
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2482" uniqueCount="1260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2502" uniqueCount="1272">
   <si>
     <t>link</t>
   </si>
@@ -3798,6 +3798,42 @@
   </si>
   <si>
     <t>2.90 ha.</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/aizkraukle-and-reg/kokneses-pag/hmcij.html</t>
+  </si>
+  <si>
+    <t>7.50 ha.</t>
+  </si>
+  <si>
+    <t>32600040206</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/zvirgzdenes-pag/bcfjoi.html</t>
+  </si>
+  <si>
+    <t>61 500 €</t>
+  </si>
+  <si>
+    <t>21.21 ha.</t>
+  </si>
+  <si>
+    <t>68980080265</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/kaunatas-pag/obpeg.html</t>
+  </si>
+  <si>
+    <t>2.08 ha.</t>
+  </si>
+  <si>
+    <t>78620030347</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/rezekne-and-reg/kaunatas-pag/jckep.html</t>
+  </si>
+  <si>
+    <t>78620130045</t>
   </si>
 </sst>
 </file>
@@ -4210,7 +4246,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F488"/>
+  <dimension ref="A1:F495"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -13985,6 +14021,146 @@
       </c>
       <c r="F488" s="2">
         <v>46063.50555555556</v>
+      </c>
+    </row>
+    <row r="489" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A489" s="3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B489" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="C489" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D489" s="4" t="s">
+        <v>1241</v>
+      </c>
+      <c r="E489" s="4" t="s">
+        <v>1242</v>
+      </c>
+      <c r="F489" s="2">
+        <v>46063.78958333333</v>
+      </c>
+    </row>
+    <row r="490" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A490" s="3" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B490" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C490" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D490" s="4" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E490" s="4" t="s">
+        <v>1245</v>
+      </c>
+      <c r="F490" s="2">
+        <v>46063.913888888885</v>
+      </c>
+    </row>
+    <row r="491" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A491" s="3" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B491" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C491" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D491" s="4" t="s">
+        <v>1247</v>
+      </c>
+      <c r="E491" s="4" t="s">
+        <v>1248</v>
+      </c>
+      <c r="F491" s="2">
+        <v>46063.85486111111</v>
+      </c>
+    </row>
+    <row r="492" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A492" s="3" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B492" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C492" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D492" s="4" t="s">
+        <v>930</v>
+      </c>
+      <c r="E492" s="4" t="s">
+        <v>1250</v>
+      </c>
+      <c r="F492" s="2">
+        <v>46063.82083333333</v>
+      </c>
+    </row>
+    <row r="493" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A493" s="3" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B493" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C493" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D493" s="4" t="s">
+        <v>1252</v>
+      </c>
+      <c r="E493" s="4" t="s">
+        <v>1253</v>
+      </c>
+      <c r="F493" s="2">
+        <v>46063.73055555555</v>
+      </c>
+    </row>
+    <row r="494" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A494" s="3" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B494" s="4" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C494" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D494" s="4" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E494" s="4" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F494" s="2">
+        <v>46063.663194444445</v>
+      </c>
+    </row>
+    <row r="495" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A495" s="3" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B495" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C495" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D495" s="4" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E495" s="4" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F495" s="2">
+        <v>46063.65555555555</v>
       </c>
     </row>
   </sheetData>
@@ -14476,6 +14652,13 @@
     <hyperlink ref="A486" r:id="rId485"/>
     <hyperlink ref="A487" r:id="rId486"/>
     <hyperlink ref="A488" r:id="rId487"/>
+    <hyperlink ref="A489" r:id="rId488"/>
+    <hyperlink ref="A490" r:id="rId489"/>
+    <hyperlink ref="A491" r:id="rId490"/>
+    <hyperlink ref="A492" r:id="rId491"/>
+    <hyperlink ref="A493" r:id="rId492"/>
+    <hyperlink ref="A494" r:id="rId493"/>
+    <hyperlink ref="A495" r:id="rId494"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -14487,7 +14670,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -14526,142 +14709,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1240</v>
+        <v>1260</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>793</v>
+        <v>204</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1241</v>
+        <v>1261</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1242</v>
+        <v>1262</v>
       </c>
       <c r="F2" s="2">
-        <v>46063.78958333333</v>
+        <v>46064.67847222222</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1243</v>
+        <v>1263</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>150</v>
+        <v>1264</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>146</v>
+        <v>234</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>1244</v>
+        <v>1265</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1245</v>
+        <v>1266</v>
       </c>
       <c r="F3" s="2">
-        <v>46063.913888888885</v>
+        <v>46065.509722222225</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1246</v>
+        <v>1267</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>185</v>
+        <v>576</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>146</v>
+        <v>294</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>1247</v>
+        <v>1268</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>1248</v>
+        <v>1269</v>
       </c>
       <c r="F4" s="2">
-        <v>46063.85486111111</v>
+        <v>46064.75625</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>1249</v>
+        <v>1270</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>43</v>
+        <v>334</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>146</v>
+        <v>294</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>930</v>
+        <v>1259</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>1250</v>
+        <v>1271</v>
       </c>
       <c r="F5" s="2">
-        <v>46063.82083333333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>1251</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>1252</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>1253</v>
-      </c>
-      <c r="F6" s="2">
-        <v>46063.73055555555</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>1254</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>1255</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>1256</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>1257</v>
-      </c>
-      <c r="F7" s="2">
-        <v>46063.663194444445</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>1258</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>1259</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>1257</v>
-      </c>
-      <c r="F8" s="2">
-        <v>46063.65555555555</v>
+        <v>46064.74097222222</v>
       </c>
     </row>
   </sheetData>
@@ -14670,9 +14793,6 @@
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-02-13 12:30
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2502" uniqueCount="1272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2512" uniqueCount="1277">
   <si>
     <t>link</t>
   </si>
@@ -3834,6 +3834,21 @@
   </si>
   <si>
     <t>78620130045</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ludza-and-reg/malnavas-pag/bmgcnj.html</t>
+  </si>
+  <si>
+    <t>68680110102</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/ventspils-and-reg/targales-pag/andgg.html</t>
+  </si>
+  <si>
+    <t>40 €</t>
+  </si>
+  <si>
+    <t>900000000000</t>
   </si>
 </sst>
 </file>
@@ -4246,7 +4261,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F495"/>
+  <dimension ref="A1:F499"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -14161,6 +14176,86 @@
       </c>
       <c r="F495" s="2">
         <v>46063.65555555555</v>
+      </c>
+    </row>
+    <row r="496" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A496" s="3" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B496" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C496" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D496" s="4" t="s">
+        <v>1261</v>
+      </c>
+      <c r="E496" s="4" t="s">
+        <v>1262</v>
+      </c>
+      <c r="F496" s="2">
+        <v>46064.67847222222</v>
+      </c>
+    </row>
+    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A497" s="3" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B497" s="4" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C497" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D497" s="4" t="s">
+        <v>1265</v>
+      </c>
+      <c r="E497" s="4" t="s">
+        <v>1266</v>
+      </c>
+      <c r="F497" s="2">
+        <v>46065.509722222225</v>
+      </c>
+    </row>
+    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A498" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B498" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C498" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D498" s="4" t="s">
+        <v>1268</v>
+      </c>
+      <c r="E498" s="4" t="s">
+        <v>1269</v>
+      </c>
+      <c r="F498" s="2">
+        <v>46064.75625</v>
+      </c>
+    </row>
+    <row r="499" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A499" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B499" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C499" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D499" s="4" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E499" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="F499" s="2">
+        <v>46064.74097222222</v>
       </c>
     </row>
   </sheetData>
@@ -14659,6 +14754,10 @@
     <hyperlink ref="A493" r:id="rId492"/>
     <hyperlink ref="A494" r:id="rId493"/>
     <hyperlink ref="A495" r:id="rId494"/>
+    <hyperlink ref="A496" r:id="rId495"/>
+    <hyperlink ref="A497" r:id="rId496"/>
+    <hyperlink ref="A498" r:id="rId497"/>
+    <hyperlink ref="A499" r:id="rId498"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -14670,7 +14769,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -14709,90 +14808,48 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1260</v>
+        <v>1272</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>204</v>
+        <v>102</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>234</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1261</v>
+        <v>209</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1262</v>
+        <v>1273</v>
       </c>
       <c r="F2" s="2">
-        <v>46064.67847222222</v>
+        <v>46065.61875</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1263</v>
+        <v>1274</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1264</v>
+        <v>1275</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>234</v>
+        <v>404</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>1265</v>
+        <v>162</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1266</v>
+        <v>1276</v>
       </c>
       <c r="F3" s="2">
-        <v>46065.509722222225</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1267</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>576</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>1268</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>1269</v>
-      </c>
-      <c r="F4" s="2">
-        <v>46064.75625</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>1270</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>1259</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>1271</v>
-      </c>
-      <c r="F5" s="2">
-        <v>46064.74097222222</v>
+        <v>46066.601388888885</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-02-16 12:33
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2512" uniqueCount="1277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2532" uniqueCount="1285">
   <si>
     <t>link</t>
   </si>
@@ -3849,6 +3849,30 @@
   </si>
   <si>
     <t>900000000000</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/daugavpils-and-reg/sventes-pag/ombfj.html</t>
+  </si>
+  <si>
+    <t>44880040024</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/madona-and-reg/sarkanu-pag/iegck.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/rozkalnu-pag/hodnc.html</t>
+  </si>
+  <si>
+    <t>76640040150</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/preilu-pag/plmkm.html</t>
+  </si>
+  <si>
+    <t>1.52 ha.</t>
+  </si>
+  <si>
+    <t>76780040110</t>
   </si>
 </sst>
 </file>
@@ -4261,7 +4285,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F499"/>
+  <dimension ref="A1:F501"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -14256,6 +14280,46 @@
       </c>
       <c r="F499" s="2">
         <v>46064.74097222222</v>
+      </c>
+    </row>
+    <row r="500" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A500" s="3" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B500" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C500" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D500" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E500" s="4" t="s">
+        <v>1273</v>
+      </c>
+      <c r="F500" s="2">
+        <v>46065.61875</v>
+      </c>
+    </row>
+    <row r="501" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A501" s="3" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B501" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C501" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="D501" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E501" s="4" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F501" s="2">
+        <v>46066.601388888885</v>
       </c>
     </row>
   </sheetData>
@@ -14758,6 +14822,8 @@
     <hyperlink ref="A497" r:id="rId496"/>
     <hyperlink ref="A498" r:id="rId497"/>
     <hyperlink ref="A499" r:id="rId498"/>
+    <hyperlink ref="A500" r:id="rId499"/>
+    <hyperlink ref="A501" r:id="rId500"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -14769,7 +14835,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -14808,48 +14874,90 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1272</v>
+        <v>1277</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>102</v>
+        <v>467</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>234</v>
+        <v>74</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1273</v>
+        <v>1278</v>
       </c>
       <c r="F2" s="2">
-        <v>46065.61875</v>
+        <v>46066.75833333333</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1274</v>
+        <v>1279</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1275</v>
+        <v>268</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>404</v>
+        <v>256</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>162</v>
+        <v>85</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1276</v>
+        <v>433</v>
       </c>
       <c r="F3" s="2">
-        <v>46066.601388888885</v>
+        <v>46068.87291666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>1281</v>
+      </c>
+      <c r="F4" s="2">
+        <v>46069.334027777775</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F5" s="2">
+        <v>46068.884722222225</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-02-17 12:33
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2532" uniqueCount="1285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2542" uniqueCount="1289">
   <si>
     <t>link</t>
   </si>
@@ -3873,6 +3873,18 @@
   </si>
   <si>
     <t>76780040110</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kuldiga-and-reg/rudbarzu-pag/abmcb.html</t>
+  </si>
+  <si>
+    <t>62820130020</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/valmiera-and-reg/brengulu-pag/jcolh.html</t>
+  </si>
+  <si>
+    <t>96460030273</t>
   </si>
 </sst>
 </file>
@@ -4285,7 +4297,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F501"/>
+  <dimension ref="A1:F505"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -14320,6 +14332,86 @@
       </c>
       <c r="F501" s="2">
         <v>46066.601388888885</v>
+      </c>
+    </row>
+    <row r="502" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A502" s="3" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B502" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C502" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D502" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E502" s="4" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F502" s="2">
+        <v>46066.75833333333</v>
+      </c>
+    </row>
+    <row r="503" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A503" s="3" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B503" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C503" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D503" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E503" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="F503" s="2">
+        <v>46068.87291666667</v>
+      </c>
+    </row>
+    <row r="504" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A504" s="3" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B504" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C504" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D504" s="4" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E504" s="4" t="s">
+        <v>1281</v>
+      </c>
+      <c r="F504" s="2">
+        <v>46069.334027777775</v>
+      </c>
+    </row>
+    <row r="505" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A505" s="3" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B505" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="C505" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D505" s="4" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E505" s="4" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F505" s="2">
+        <v>46068.884722222225</v>
       </c>
     </row>
   </sheetData>
@@ -14824,6 +14916,10 @@
     <hyperlink ref="A499" r:id="rId498"/>
     <hyperlink ref="A500" r:id="rId499"/>
     <hyperlink ref="A501" r:id="rId500"/>
+    <hyperlink ref="A502" r:id="rId501"/>
+    <hyperlink ref="A503" r:id="rId502"/>
+    <hyperlink ref="A504" r:id="rId503"/>
+    <hyperlink ref="A505" r:id="rId504"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -14835,7 +14931,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -14874,90 +14970,48 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1277</v>
+        <v>1285</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>467</v>
+        <v>23</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>74</v>
+        <v>424</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>186</v>
+        <v>24</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1278</v>
+        <v>1286</v>
       </c>
       <c r="F2" s="2">
-        <v>46066.75833333333</v>
+        <v>46069.785416666666</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1279</v>
+        <v>1287</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>268</v>
+        <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>256</v>
+        <v>396</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>433</v>
+        <v>1288</v>
       </c>
       <c r="F3" s="2">
-        <v>46068.87291666667</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1280</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>1281</v>
-      </c>
-      <c r="F4" s="2">
-        <v>46069.334027777775</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>1282</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>793</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>1283</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>1284</v>
-      </c>
-      <c r="F5" s="2">
-        <v>46068.884722222225</v>
+        <v>46070.54375</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-02-18 12:33
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2542" uniqueCount="1289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2562" uniqueCount="1295">
   <si>
     <t>link</t>
   </si>
@@ -3885,6 +3885,24 @@
   </si>
   <si>
     <t>96460030273</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/bauska-and-reg/iecavas-nov/afidf.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/aulejas-pag/opihc.html</t>
+  </si>
+  <si>
+    <t>60480050132</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/robeznieku-pag/bxjmlo.html</t>
+  </si>
+  <si>
+    <t>60860010082, 0222</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/tukums-and-reg/dzukstes-pag/aoxce.html</t>
   </si>
 </sst>
 </file>
@@ -4297,7 +4315,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F505"/>
+  <dimension ref="A1:F507"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -14412,6 +14430,46 @@
       </c>
       <c r="F505" s="2">
         <v>46068.884722222225</v>
+      </c>
+    </row>
+    <row r="506" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A506" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B506" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C506" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D506" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E506" s="4" t="s">
+        <v>1286</v>
+      </c>
+      <c r="F506" s="2">
+        <v>46069.785416666666</v>
+      </c>
+    </row>
+    <row r="507" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A507" s="3" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B507" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C507" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="D507" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E507" s="4" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F507" s="2">
+        <v>46070.54375</v>
       </c>
     </row>
   </sheetData>
@@ -14920,6 +14978,8 @@
     <hyperlink ref="A503" r:id="rId502"/>
     <hyperlink ref="A504" r:id="rId503"/>
     <hyperlink ref="A505" r:id="rId504"/>
+    <hyperlink ref="A506" r:id="rId505"/>
+    <hyperlink ref="A507" r:id="rId506"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -14931,7 +14991,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -14970,48 +15030,90 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1285</v>
+        <v>1289</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>650</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>424</v>
+        <v>48</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>24</v>
+        <v>186</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1286</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>46069.785416666666</v>
+        <v>46071.475694444445</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1287</v>
+        <v>1290</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>505</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>396</v>
+        <v>146</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>272</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1288</v>
+        <v>1291</v>
       </c>
       <c r="F3" s="2">
-        <v>46070.54375</v>
+        <v>46070.861805555556</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>1293</v>
+      </c>
+      <c r="F4" s="2">
+        <v>46070.72430555556</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2">
+        <v>46071.4875</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-02-19 12:35
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2562" uniqueCount="1295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2577" uniqueCount="1302">
   <si>
     <t>link</t>
   </si>
@@ -3903,6 +3903,27 @@
   </si>
   <si>
     <t>https://www.ss.com/msg/lv/real-estate/wood/tukums-and-reg/dzukstes-pag/aoxce.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/bauska-and-reg/iecavas-nov/lclfm.html</t>
+  </si>
+  <si>
+    <t>40460060490</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/kraslava-and-reg/kepovas-pag/mxnne.html</t>
+  </si>
+  <si>
+    <t>60800040007</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/rozupes-pag/ilhhk.html</t>
+  </si>
+  <si>
+    <t>10 €</t>
+  </si>
+  <si>
+    <t>76660010146</t>
   </si>
 </sst>
 </file>
@@ -4315,7 +4336,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F507"/>
+  <dimension ref="A1:F511"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -14470,6 +14491,86 @@
       </c>
       <c r="F507" s="2">
         <v>46070.54375</v>
+      </c>
+    </row>
+    <row r="508" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A508" s="3" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B508" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="C508" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D508" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E508" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F508" s="2">
+        <v>46071.475694444445</v>
+      </c>
+    </row>
+    <row r="509" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A509" s="3" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B509" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="C509" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D509" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E509" s="4" t="s">
+        <v>1291</v>
+      </c>
+      <c r="F509" s="2">
+        <v>46070.861805555556</v>
+      </c>
+    </row>
+    <row r="510" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A510" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B510" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C510" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D510" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E510" s="4" t="s">
+        <v>1293</v>
+      </c>
+      <c r="F510" s="2">
+        <v>46070.72430555556</v>
+      </c>
+    </row>
+    <row r="511" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A511" s="3" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B511" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="C511" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D511" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E511" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F511" s="2">
+        <v>46071.4875</v>
       </c>
     </row>
   </sheetData>
@@ -14980,6 +15081,10 @@
     <hyperlink ref="A505" r:id="rId504"/>
     <hyperlink ref="A506" r:id="rId505"/>
     <hyperlink ref="A507" r:id="rId506"/>
+    <hyperlink ref="A508" r:id="rId507"/>
+    <hyperlink ref="A509" r:id="rId508"/>
+    <hyperlink ref="A510" r:id="rId509"/>
+    <hyperlink ref="A511" r:id="rId510"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -14991,7 +15096,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -15030,82 +15135,62 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1289</v>
+        <v>1295</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>650</v>
+        <v>979</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>186</v>
+        <v>82</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>1296</v>
       </c>
       <c r="F2" s="2">
-        <v>46071.475694444445</v>
+        <v>46071.69236111111</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1290</v>
+        <v>1297</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>505</v>
+        <v>290</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>272</v>
+        <v>918</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1291</v>
+        <v>1298</v>
       </c>
       <c r="F3" s="2">
-        <v>46070.861805555556</v>
+        <v>46072.018055555556</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1292</v>
+        <v>1299</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>274</v>
+        <v>1300</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>146</v>
+        <v>284</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>1293</v>
+        <v>1301</v>
       </c>
       <c r="F4" s="2">
-        <v>46070.72430555556</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>1294</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>533</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2">
-        <v>46071.4875</v>
+        <v>46072.54166666667</v>
       </c>
     </row>
   </sheetData>
@@ -15113,7 +15198,6 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Update forest data - 2026-02-20 12:30
</commit_message>
<xml_diff>
--- a/forests-scraped.xlsx
+++ b/forests-scraped.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2577" uniqueCount="1302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2592" uniqueCount="1307">
   <si>
     <t>link</t>
   </si>
@@ -3924,6 +3924,21 @@
   </si>
   <si>
     <t>76660010146</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/balvi-and-reg/viksnas-pag/eeedd.html</t>
+  </si>
+  <si>
+    <t>2.27 ha.</t>
+  </si>
+  <si>
+    <t>38940060037</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/gulbene-and-reg/stradu-pag/nlppl.html</t>
+  </si>
+  <si>
+    <t>https://www.ss.com/msg/lv/real-estate/wood/preili-and-reg/preilu-pag/cckmx.html</t>
   </si>
 </sst>
 </file>
@@ -4336,7 +4351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F511"/>
+  <dimension ref="A1:F514"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -14571,6 +14586,66 @@
       </c>
       <c r="F511" s="2">
         <v>46071.4875</v>
+      </c>
+    </row>
+    <row r="512" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A512" s="3" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B512" s="4" t="s">
+        <v>979</v>
+      </c>
+      <c r="C512" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D512" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E512" s="4" t="s">
+        <v>1296</v>
+      </c>
+      <c r="F512" s="2">
+        <v>46071.69236111111</v>
+      </c>
+    </row>
+    <row r="513" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A513" s="3" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B513" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C513" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D513" s="4" t="s">
+        <v>918</v>
+      </c>
+      <c r="E513" s="4" t="s">
+        <v>1298</v>
+      </c>
+      <c r="F513" s="2">
+        <v>46072.018055555556</v>
+      </c>
+    </row>
+    <row r="514" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A514" s="3" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B514" s="4" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C514" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D514" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E514" s="4" t="s">
+        <v>1301</v>
+      </c>
+      <c r="F514" s="2">
+        <v>46072.54166666667</v>
       </c>
     </row>
   </sheetData>
@@ -15085,6 +15160,9 @@
     <hyperlink ref="A509" r:id="rId508"/>
     <hyperlink ref="A510" r:id="rId509"/>
     <hyperlink ref="A511" r:id="rId510"/>
+    <hyperlink ref="A512" r:id="rId511"/>
+    <hyperlink ref="A513" r:id="rId512"/>
+    <hyperlink ref="A514" r:id="rId513"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -15135,50 +15213,50 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1295</v>
+        <v>1302</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>979</v>
+        <v>88</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>82</v>
+        <v>1303</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1296</v>
+        <v>1304</v>
       </c>
       <c r="F2" s="2">
-        <v>46071.69236111111</v>
+        <v>46072.90694444445</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1297</v>
+        <v>1305</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>290</v>
+        <v>106</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>918</v>
+        <v>135</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1298</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2">
-        <v>46072.018055555556</v>
+        <v>46073.47083333333</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1299</v>
+        <v>1306</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1300</v>
+        <v>467</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>284</v>
@@ -15190,7 +15268,7 @@
         <v>1301</v>
       </c>
       <c r="F4" s="2">
-        <v>46072.54166666667</v>
+        <v>46072.83888888889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>